<commit_message>
modified:   .gitignore 	modified:   0 SYS-sourcen/S1/S1a/PF01.MAC 	modified:   0 SYS-sourcen/S1/S1a/S1A.HEX 	modified:   0 SYS-sourcen/S1/S1a/S1Aa.HEX 	modified:   0 SYS-sourcen/S1/S1a/S1Ab.HEX 	modified:   0 SYS-sourcen/S1/S1a/SD01.MAC 	modified:   0 SYS-sourcen/S1/S1a/SY01.MAC 	modified:   0 SYS-sourcen/S1/S1b/KM.MAC 	modified:   0 SYS-sourcen/S1/S1b/S1B-PRN.MAC 	modified:   0 SYS-sourcen/S1/S1b/S1B.HEX 	modified:   0 SYS-sourcen/S1/S1b/S1B.REL 	modified:   0 SYS-sourcen/S1/S1b/S1Ba.HEX 	deleted:    BIN1/S12-neu.bin 	modified:   BIN1/S12.bin 	modified:   DOC/DEG2000.xlsx 	new file:   FONT/1/6x14.FNT 	new file:   FONT/1/6x8.FNT 	new file:   FONT/1/8x14.FNT 	new file:   FONT/1/8x14apl.FNT 	new file:   FONT/1/8x14thin.FNT 	new file:   FONT/1/8x8.FNT 	new file:   FONT/1/8x8thin.FNT
</commit_message>
<xml_diff>
--- a/DOC/DEG2000.xlsx
+++ b/DOC/DEG2000.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\devel\1 DEG2000\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6CB513-2B29-4628-9CFD-1509D0A2B1DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4821B5E9-55A7-4CA8-AA67-BB10D3F3ED14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22020" windowHeight="11100" activeTab="6" xr2:uid="{F91C61BF-F393-4C13-9000-551DF6FEF055}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22020" windowHeight="11100" activeTab="11" xr2:uid="{F91C61BF-F393-4C13-9000-551DF6FEF055}"/>
   </bookViews>
   <sheets>
     <sheet name="DataGridView" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1714" uniqueCount="982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="981">
   <si>
     <t>cpuStatus</t>
   </si>
@@ -1658,9 +1658,6 @@
   </si>
   <si>
     <t>099D</t>
-  </si>
-  <si>
-    <t>DEG2</t>
   </si>
   <si>
     <t>DATE</t>
@@ -8800,7 +8797,7 @@
         <v>342</v>
       </c>
       <c r="F3" s="219" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="G3" s="220" t="s">
         <v>348</v>
@@ -9647,7 +9644,7 @@
         <v>342</v>
       </c>
       <c r="F54" s="437" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="G54" s="438" t="s">
         <v>348</v>
@@ -9660,7 +9657,7 @@
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E55" s="472" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F55" s="473" t="s">
         <v>490</v>
@@ -9674,7 +9671,7 @@
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E56" s="475" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="F56" s="296" t="s">
         <v>334</v>
@@ -9686,7 +9683,7 @@
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E57" s="476" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="F57" s="298" t="s">
         <v>333</v>
@@ -9700,31 +9697,31 @@
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E58" s="467" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="F58" s="468" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="G58" s="469"/>
       <c r="H58" s="470" t="s">
+        <v>841</v>
+      </c>
+      <c r="I58" s="470" t="s">
         <v>842</v>
-      </c>
-      <c r="I58" s="470" t="s">
-        <v>843</v>
       </c>
       <c r="J58" s="471"/>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E59" s="466" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="F59" s="441" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="G59" s="442"/>
       <c r="H59" s="443"/>
       <c r="I59" s="443" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="J59" s="444"/>
     </row>
@@ -9733,12 +9730,12 @@
         <v>268</v>
       </c>
       <c r="F60" s="455" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="G60" s="447"/>
       <c r="H60" s="448"/>
       <c r="I60" s="448" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="J60" s="449"/>
     </row>
@@ -9747,34 +9744,34 @@
         <v>268</v>
       </c>
       <c r="F61" s="455" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="G61" s="447"/>
       <c r="H61" s="448"/>
       <c r="I61" s="448" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="J61" s="449"/>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E62" s="456" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F62" s="457" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="G62" s="458"/>
       <c r="H62" s="459" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="I62" s="459" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="J62" s="460"/>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E63" s="461" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="F63" s="462" t="s">
         <v>112</v>
@@ -9782,71 +9779,71 @@
       <c r="G63" s="463"/>
       <c r="H63" s="464"/>
       <c r="I63" s="464" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="J63" s="465"/>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E64" s="466" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F64" s="441" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="G64" s="442"/>
       <c r="H64" s="443"/>
       <c r="I64" s="443" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="J64" s="444"/>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E65" s="445" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="F65" s="446" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="G65" s="447"/>
       <c r="H65" s="448"/>
       <c r="I65" s="448" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="J65" s="444"/>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E66" s="456" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="F66" s="457" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="G66" s="458"/>
       <c r="H66" s="459" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="I66" s="459" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="J66" s="460"/>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E67" s="461" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="F67" s="462" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="G67" s="463"/>
       <c r="H67" s="464"/>
       <c r="I67" s="464" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="J67" s="465"/>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E68" s="445" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F68" s="446" t="s">
         <v>112</v>
@@ -9854,51 +9851,51 @@
       <c r="G68" s="447"/>
       <c r="H68" s="448"/>
       <c r="I68" s="448" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="J68" s="449"/>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E69" s="445" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="F69" s="446" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="G69" s="447"/>
       <c r="H69" s="448"/>
       <c r="I69" s="448" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="J69" s="449"/>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E70" s="445" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="F70" s="446" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="G70" s="447"/>
       <c r="H70" s="448"/>
       <c r="I70" s="448" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="J70" s="449"/>
     </row>
     <row r="71" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E71" s="450" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="F71" s="451" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="G71" s="452"/>
       <c r="H71" s="453" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="I71" s="453" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="J71" s="454"/>
     </row>
@@ -10453,8 +10450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3A67EE2-2541-4C21-B409-F79E37C3B854}">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10478,15 +10475,15 @@
       </c>
       <c r="D2" s="375"/>
       <c r="E2" s="371" t="s">
+        <v>590</v>
+      </c>
+      <c r="F2" s="365" t="s">
         <v>591</v>
-      </c>
-      <c r="F2" s="365" t="s">
-        <v>592</v>
       </c>
       <c r="G2" s="365"/>
       <c r="H2" s="365"/>
       <c r="I2" s="366" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="J2" s="367"/>
     </row>
@@ -10495,10 +10492,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="F3" s="368" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
@@ -10516,14 +10513,16 @@
         <v>2</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="F4" s="368" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
-      <c r="I4" s="225"/>
+      <c r="I4" s="225" t="s">
+        <v>592</v>
+      </c>
       <c r="J4" s="226"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -10534,14 +10533,16 @@
         <v>3</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="F5" s="368" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
-      <c r="I5" s="225"/>
+      <c r="I5" s="225" t="s">
+        <v>592</v>
+      </c>
       <c r="J5" s="226"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -10552,10 +10553,10 @@
         <v>4</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="F6" s="368" t="s">
-        <v>561</v>
+        <v>510</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
@@ -10567,16 +10568,14 @@
         <v>5</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="F7" s="368" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
-      <c r="I7" s="225" t="s">
-        <v>593</v>
-      </c>
+      <c r="I7" s="225"/>
       <c r="J7" s="226"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -10584,10 +10583,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="F8" s="368" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
@@ -10599,12 +10598,14 @@
         <v>7</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="F9" s="368" t="s">
-        <v>513</v>
-      </c>
-      <c r="G9" s="17"/>
+        <v>516</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>500</v>
+      </c>
       <c r="H9" s="17"/>
       <c r="I9" s="225"/>
       <c r="J9" s="226"/>
@@ -10614,12 +10615,14 @@
         <v>8</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="F10" s="368" t="s">
-        <v>515</v>
-      </c>
-      <c r="G10" s="17"/>
+        <v>518</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>500</v>
+      </c>
       <c r="H10" s="17"/>
       <c r="I10" s="225"/>
       <c r="J10" s="226"/>
@@ -10629,14 +10632,12 @@
         <v>9</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
       <c r="F11" s="368" t="s">
-        <v>517</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>500</v>
-      </c>
+        <v>522</v>
+      </c>
+      <c r="G11" s="17"/>
       <c r="H11" s="17"/>
       <c r="I11" s="225"/>
       <c r="J11" s="226"/>
@@ -10646,14 +10647,12 @@
         <v>10</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>518</v>
+        <v>523</v>
       </c>
       <c r="F12" s="368" t="s">
-        <v>519</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>500</v>
-      </c>
+        <v>524</v>
+      </c>
+      <c r="G12" s="17"/>
       <c r="H12" s="17"/>
       <c r="I12" s="225"/>
       <c r="J12" s="226"/>
@@ -10663,10 +10662,10 @@
         <v>11</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="F13" s="368" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
@@ -10678,14 +10677,16 @@
         <v>12</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="F14" s="368" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
-      <c r="I14" s="225"/>
+      <c r="I14" s="225" t="s">
+        <v>592</v>
+      </c>
       <c r="J14" s="226"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -10693,14 +10694,16 @@
         <v>13</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
       <c r="F15" s="368" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
-      <c r="I15" s="225"/>
+      <c r="I15" s="225" t="s">
+        <v>952</v>
+      </c>
       <c r="J15" s="226"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -10708,14 +10711,20 @@
         <v>14</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="F16" s="368" t="s">
-        <v>527</v>
-      </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="225"/>
+        <v>530</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>533</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>535</v>
+      </c>
+      <c r="I16" s="225" t="s">
+        <v>592</v>
+      </c>
       <c r="J16" s="226"/>
     </row>
     <row r="17" spans="4:10" x14ac:dyDescent="0.25">
@@ -10723,14 +10732,20 @@
         <v>15</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="F17" s="368" t="s">
-        <v>529</v>
-      </c>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="225"/>
+        <v>532</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>534</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>535</v>
+      </c>
+      <c r="I17" s="225" t="s">
+        <v>592</v>
+      </c>
       <c r="J17" s="226"/>
     </row>
     <row r="18" spans="4:10" x14ac:dyDescent="0.25">
@@ -10738,20 +10753,16 @@
         <v>16</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="F18" s="368" t="s">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>534</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>536</v>
-      </c>
-      <c r="I18" s="225" t="s">
-        <v>593</v>
-      </c>
+        <v>540</v>
+      </c>
+      <c r="H18" s="17"/>
+      <c r="I18" s="225"/>
       <c r="J18" s="226"/>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.25">
@@ -10759,20 +10770,16 @@
         <v>17</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c r="F19" s="368" t="s">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>535</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>536</v>
-      </c>
-      <c r="I19" s="225" t="s">
-        <v>593</v>
-      </c>
+        <v>544</v>
+      </c>
+      <c r="H19" s="17"/>
+      <c r="I19" s="225"/>
       <c r="J19" s="226"/>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.25">
@@ -10780,13 +10787,13 @@
         <v>18</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="F20" s="368" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="225"/>
@@ -10797,13 +10804,13 @@
         <v>19</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>539</v>
+        <v>545</v>
       </c>
       <c r="F21" s="368" t="s">
-        <v>540</v>
+        <v>546</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="H21" s="17"/>
       <c r="I21" s="225"/>
@@ -10814,14 +10821,12 @@
         <v>20</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>542</v>
+        <v>501</v>
       </c>
       <c r="F22" s="368" t="s">
-        <v>543</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>544</v>
-      </c>
+        <v>502</v>
+      </c>
+      <c r="G22" s="17"/>
       <c r="H22" s="17"/>
       <c r="I22" s="225"/>
       <c r="J22" s="226"/>
@@ -10831,14 +10836,12 @@
         <v>21</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="F23" s="368" t="s">
-        <v>547</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>548</v>
-      </c>
+        <v>549</v>
+      </c>
+      <c r="G23" s="17"/>
       <c r="H23" s="17"/>
       <c r="I23" s="225"/>
       <c r="J23" s="226"/>
@@ -10848,10 +10851,10 @@
         <v>22</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>549</v>
+        <v>695</v>
       </c>
       <c r="F24" s="368" t="s">
-        <v>550</v>
+        <v>560</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="17"/>
@@ -10863,13 +10866,13 @@
         <v>23</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F25" s="368" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="H25" s="17"/>
       <c r="I25" s="225"/>
@@ -10880,13 +10883,13 @@
         <v>24</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F26" s="368" t="s">
+        <v>553</v>
+      </c>
+      <c r="G26" s="17" t="s">
         <v>554</v>
-      </c>
-      <c r="G26" s="17" t="s">
-        <v>555</v>
       </c>
       <c r="H26" s="17"/>
       <c r="I26" s="225"/>
@@ -10897,13 +10900,13 @@
         <v>25</v>
       </c>
       <c r="E27" s="16" t="s">
+        <v>556</v>
+      </c>
+      <c r="F27" s="368" t="s">
         <v>557</v>
       </c>
-      <c r="F27" s="368" t="s">
+      <c r="G27" s="17" t="s">
         <v>558</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>559</v>
       </c>
       <c r="H27" s="17"/>
       <c r="I27" s="225"/>
@@ -10914,10 +10917,10 @@
         <v>26</v>
       </c>
       <c r="E28" s="16" t="s">
+        <v>559</v>
+      </c>
+      <c r="F28" s="368" t="s">
         <v>560</v>
-      </c>
-      <c r="F28" s="368" t="s">
-        <v>561</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="17"/>
@@ -10938,13 +10941,13 @@
         <v>1</v>
       </c>
       <c r="E30" s="373" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F30" s="369"/>
       <c r="G30" s="369"/>
       <c r="H30" s="369"/>
       <c r="I30" s="254" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J30" s="255"/>
     </row>
@@ -10953,13 +10956,13 @@
         <v>2</v>
       </c>
       <c r="E31" s="373" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F31" s="369"/>
       <c r="G31" s="369"/>
       <c r="H31" s="369"/>
       <c r="I31" s="254" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J31" s="255"/>
     </row>
@@ -10968,13 +10971,13 @@
         <v>3</v>
       </c>
       <c r="E32" s="373" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F32" s="369"/>
       <c r="G32" s="369"/>
       <c r="H32" s="369"/>
       <c r="I32" s="254" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J32" s="255"/>
     </row>
@@ -10983,13 +10986,13 @@
         <v>4</v>
       </c>
       <c r="E33" s="373" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F33" s="369"/>
       <c r="G33" s="369"/>
       <c r="H33" s="369"/>
       <c r="I33" s="254" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J33" s="255"/>
     </row>
@@ -10998,13 +11001,13 @@
         <v>5</v>
       </c>
       <c r="E34" s="373" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F34" s="369"/>
       <c r="G34" s="369"/>
       <c r="H34" s="369"/>
       <c r="I34" s="254" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J34" s="255"/>
     </row>
@@ -11013,13 +11016,13 @@
         <v>6</v>
       </c>
       <c r="E35" s="373" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F35" s="369"/>
       <c r="G35" s="369"/>
       <c r="H35" s="369"/>
       <c r="I35" s="254" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J35" s="255"/>
     </row>
@@ -11028,13 +11031,13 @@
         <v>7</v>
       </c>
       <c r="E36" s="373" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F36" s="369"/>
       <c r="G36" s="369"/>
       <c r="H36" s="369"/>
       <c r="I36" s="254" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J36" s="255"/>
     </row>
@@ -11043,13 +11046,13 @@
         <v>8</v>
       </c>
       <c r="E37" s="373" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F37" s="369"/>
       <c r="G37" s="369"/>
       <c r="H37" s="369"/>
       <c r="I37" s="254" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J37" s="255"/>
     </row>
@@ -11058,13 +11061,13 @@
         <v>9</v>
       </c>
       <c r="E38" s="373" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F38" s="369"/>
       <c r="G38" s="369"/>
       <c r="H38" s="369"/>
       <c r="I38" s="380" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J38" s="255"/>
     </row>
@@ -11073,13 +11076,13 @@
         <v>10</v>
       </c>
       <c r="E39" s="373" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F39" s="369"/>
       <c r="G39" s="369"/>
       <c r="H39" s="369"/>
       <c r="I39" s="380" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J39" s="255"/>
     </row>
@@ -11088,13 +11091,13 @@
         <v>11</v>
       </c>
       <c r="E40" s="373" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F40" s="369"/>
       <c r="G40" s="369"/>
       <c r="H40" s="369"/>
       <c r="I40" s="254" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J40" s="255"/>
     </row>
@@ -11103,13 +11106,13 @@
         <v>12</v>
       </c>
       <c r="E41" s="373" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F41" s="369"/>
       <c r="G41" s="369"/>
       <c r="H41" s="369"/>
       <c r="I41" s="254" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J41" s="255"/>
     </row>
@@ -11118,13 +11121,13 @@
         <v>13</v>
       </c>
       <c r="E42" s="373" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F42" s="369"/>
       <c r="G42" s="369"/>
       <c r="H42" s="369"/>
       <c r="I42" s="254" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J42" s="255"/>
     </row>
@@ -11133,13 +11136,13 @@
         <v>14</v>
       </c>
       <c r="E43" s="373" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F43" s="369"/>
       <c r="G43" s="369"/>
       <c r="H43" s="369"/>
       <c r="I43" s="254" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J43" s="255"/>
     </row>
@@ -11148,7 +11151,7 @@
         <v>15</v>
       </c>
       <c r="E44" s="373" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F44" s="369"/>
       <c r="G44" s="369"/>
@@ -11161,7 +11164,7 @@
         <v>16</v>
       </c>
       <c r="E45" s="373" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F45" s="369"/>
       <c r="G45" s="369"/>
@@ -11174,7 +11177,7 @@
         <v>17</v>
       </c>
       <c r="E46" s="373" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F46" s="369"/>
       <c r="G46" s="369"/>
@@ -11187,7 +11190,7 @@
         <v>18</v>
       </c>
       <c r="E47" s="373" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F47" s="369"/>
       <c r="G47" s="369"/>
@@ -11200,7 +11203,7 @@
         <v>19</v>
       </c>
       <c r="E48" s="373" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F48" s="369"/>
       <c r="G48" s="369"/>
@@ -11213,7 +11216,7 @@
         <v>20</v>
       </c>
       <c r="E49" s="373" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F49" s="369"/>
       <c r="G49" s="369"/>
@@ -11226,13 +11229,13 @@
         <v>21</v>
       </c>
       <c r="E50" s="373" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F50" s="369"/>
       <c r="G50" s="369"/>
       <c r="H50" s="369"/>
       <c r="I50" s="254" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J50" s="255"/>
     </row>
@@ -11241,13 +11244,13 @@
         <v>22</v>
       </c>
       <c r="E51" s="373" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F51" s="369"/>
       <c r="G51" s="369"/>
       <c r="H51" s="369"/>
       <c r="I51" s="254" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J51" s="255"/>
     </row>
@@ -11256,13 +11259,13 @@
         <v>23</v>
       </c>
       <c r="E52" s="373" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="F52" s="369"/>
       <c r="G52" s="369"/>
       <c r="H52" s="369"/>
       <c r="I52" s="254" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J52" s="255"/>
     </row>
@@ -11271,7 +11274,7 @@
         <v>24</v>
       </c>
       <c r="E53" s="373" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="F53" s="369"/>
       <c r="G53" s="369"/>
@@ -11284,7 +11287,7 @@
         <v>25</v>
       </c>
       <c r="E54" s="373" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F54" s="369"/>
       <c r="G54" s="369"/>
@@ -11297,7 +11300,7 @@
         <v>26</v>
       </c>
       <c r="E55" s="373" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F55" s="369"/>
       <c r="G55" s="369"/>
@@ -11310,7 +11313,7 @@
         <v>27</v>
       </c>
       <c r="E56" s="373" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F56" s="369"/>
       <c r="G56" s="369"/>
@@ -11323,7 +11326,7 @@
         <v>28</v>
       </c>
       <c r="E57" s="373" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F57" s="369"/>
       <c r="G57" s="369"/>
@@ -11336,7 +11339,7 @@
         <v>29</v>
       </c>
       <c r="E58" s="373" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F58" s="369"/>
       <c r="G58" s="369"/>
@@ -11349,7 +11352,7 @@
         <v>30</v>
       </c>
       <c r="E59" s="374" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F59" s="370"/>
       <c r="G59" s="370"/>
@@ -11391,7 +11394,7 @@
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="744" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C3" s="745"/>
       <c r="D3" s="745"/>
@@ -11401,63 +11404,63 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="477" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C4" s="481"/>
       <c r="D4" s="484" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E4" s="338"/>
       <c r="F4" s="482" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="G4" s="478"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="479" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C5" s="335"/>
       <c r="D5" s="319" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E5" s="322"/>
       <c r="F5" s="372" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G5" s="213"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="479" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C6" s="335"/>
       <c r="D6" s="319" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E6" s="322"/>
       <c r="F6" s="372" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="G6" s="213"/>
     </row>
     <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="480" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C7" s="337"/>
       <c r="D7" s="321" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E7" s="323"/>
       <c r="F7" s="483" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="G7" s="216"/>
     </row>
     <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="747" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C8" s="748"/>
       <c r="D8" s="748"/>
@@ -11467,63 +11470,63 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="477" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C9" s="481"/>
       <c r="D9" s="484" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E9" s="338"/>
       <c r="F9" s="482" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="G9" s="478"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="479" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C10" s="335"/>
       <c r="D10" s="319" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E10" s="322"/>
       <c r="F10" s="372" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G10" s="213"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="479" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C11" s="335"/>
       <c r="D11" s="319" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E11" s="322"/>
       <c r="F11" s="372" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="G11" s="213"/>
     </row>
     <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="480" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C12" s="337"/>
       <c r="D12" s="321" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E12" s="323"/>
       <c r="F12" s="483" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="G12" s="216"/>
     </row>
     <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="747" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C13" s="748"/>
       <c r="D13" s="748"/>
@@ -11533,63 +11536,63 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="477" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C14" s="481"/>
       <c r="D14" s="484" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E14" s="338"/>
       <c r="F14" s="482" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="G14" s="478"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="479" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C15" s="335"/>
       <c r="D15" s="319" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E15" s="322"/>
       <c r="F15" s="372" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G15" s="213"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="479" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C16" s="335"/>
       <c r="D16" s="319" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E16" s="322"/>
       <c r="F16" s="372" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="G16" s="213"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="480" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C17" s="337"/>
       <c r="D17" s="321" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E17" s="323"/>
       <c r="F17" s="483" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="G17" s="216"/>
     </row>
     <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="747" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C18" s="748"/>
       <c r="D18" s="748"/>
@@ -11599,57 +11602,57 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="477" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C19" s="481"/>
       <c r="D19" s="484" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E19" s="338"/>
       <c r="F19" s="482" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="G19" s="478"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="479" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C20" s="335"/>
       <c r="D20" s="319" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E20" s="322"/>
       <c r="F20" s="372" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G20" s="213"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="479" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C21" s="335"/>
       <c r="D21" s="319" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E21" s="322"/>
       <c r="F21" s="372" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="G21" s="213"/>
     </row>
     <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="480" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C22" s="337"/>
       <c r="D22" s="321" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E22" s="323"/>
       <c r="F22" s="483" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="G22" s="216"/>
     </row>
@@ -11687,7 +11690,7 @@
   <sheetData>
     <row r="2" spans="2:7" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="743" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="C2" s="750"/>
       <c r="D2" s="750"/>
@@ -11697,7 +11700,7 @@
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="744" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C3" s="745"/>
       <c r="D3" s="745"/>
@@ -11707,83 +11710,83 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="505" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C4" s="506" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D4" s="507" t="s">
+        <v>850</v>
+      </c>
+      <c r="E4" s="508" t="s">
+        <v>862</v>
+      </c>
+      <c r="F4" s="509" t="s">
         <v>851</v>
       </c>
-      <c r="E4" s="508" t="s">
-        <v>863</v>
-      </c>
-      <c r="F4" s="509" t="s">
-        <v>852</v>
-      </c>
       <c r="G4" s="510" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="511" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C5" s="512" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D5" s="513" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E5" s="514"/>
       <c r="F5" s="515" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G5" s="516" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="511" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C6" s="512" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D6" s="513" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E6" s="514"/>
       <c r="F6" s="515" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="G6" s="516" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="517" t="s">
+        <v>705</v>
+      </c>
+      <c r="C7" s="520" t="s">
+        <v>872</v>
+      </c>
+      <c r="D7" s="518" t="s">
         <v>706</v>
       </c>
-      <c r="C7" s="520" t="s">
-        <v>873</v>
-      </c>
-      <c r="D7" s="518" t="s">
+      <c r="E7" s="521" t="s">
+        <v>870</v>
+      </c>
+      <c r="F7" s="519" t="s">
         <v>707</v>
       </c>
-      <c r="E7" s="521" t="s">
+      <c r="G7" s="522" t="s">
         <v>871</v>
-      </c>
-      <c r="F7" s="519" t="s">
-        <v>708</v>
-      </c>
-      <c r="G7" s="522" t="s">
-        <v>872</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="747" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C8" s="748"/>
       <c r="D8" s="748"/>
@@ -11793,63 +11796,63 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="487" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C9" s="488"/>
       <c r="D9" s="489" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E9" s="490"/>
       <c r="F9" s="491" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="G9" s="492"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="493" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C10" s="494"/>
       <c r="D10" s="495" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E10" s="496"/>
       <c r="F10" s="497" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G10" s="498"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="493" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C11" s="494"/>
       <c r="D11" s="495" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E11" s="496"/>
       <c r="F11" s="497" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="G11" s="498"/>
     </row>
     <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="499" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C12" s="500"/>
       <c r="D12" s="501" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E12" s="502"/>
       <c r="F12" s="503" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="G12" s="504"/>
     </row>
     <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="747" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C13" s="748"/>
       <c r="D13" s="748"/>
@@ -11859,63 +11862,63 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="487" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C14" s="488"/>
       <c r="D14" s="489" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E14" s="490"/>
       <c r="F14" s="491" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="G14" s="492"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="493" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C15" s="494"/>
       <c r="D15" s="495" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E15" s="496"/>
       <c r="F15" s="497" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G15" s="498"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="493" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C16" s="494"/>
       <c r="D16" s="495" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E16" s="496"/>
       <c r="F16" s="497" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="G16" s="498"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="499" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C17" s="500"/>
       <c r="D17" s="501" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E17" s="502"/>
       <c r="F17" s="503" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="G17" s="504"/>
     </row>
     <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="747" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C18" s="748"/>
       <c r="D18" s="748"/>
@@ -11925,66 +11928,66 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="487" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C19" s="488"/>
       <c r="D19" s="489" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E19" s="490"/>
       <c r="F19" s="491" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="G19" s="492"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="493" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C20" s="494"/>
       <c r="D20" s="495" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E20" s="496"/>
       <c r="F20" s="497" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G20" s="498"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="493" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C21" s="494"/>
       <c r="D21" s="495" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E21" s="496"/>
       <c r="F21" s="497" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="G21" s="498"/>
     </row>
     <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="499" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C22" s="500"/>
       <c r="D22" s="501" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E22" s="502"/>
       <c r="F22" s="503" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="G22" s="504"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>863</v>
+      </c>
+      <c r="C24" t="s">
         <v>864</v>
-      </c>
-      <c r="C24" t="s">
-        <v>865</v>
       </c>
     </row>
   </sheetData>
@@ -13699,7 +13702,7 @@
         <v>88</v>
       </c>
       <c r="I5" s="573" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="6" spans="3:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -13716,7 +13719,7 @@
         <v>33</v>
       </c>
       <c r="I6" s="709" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
@@ -13747,7 +13750,7 @@
         <v>73</v>
       </c>
       <c r="E9" s="81" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="F9" s="82" t="s">
         <v>82</v>
@@ -13772,7 +13775,7 @@
         <v>32</v>
       </c>
       <c r="I10" s="707" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
@@ -13953,7 +13956,7 @@
         <v>64</v>
       </c>
       <c r="E25" s="97" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="F25" s="82" t="s">
         <v>78</v>
@@ -13972,10 +13975,10 @@
         <v>54</v>
       </c>
       <c r="E26" s="565" t="s">
+        <v>881</v>
+      </c>
+      <c r="F26" s="566" t="s">
         <v>882</v>
-      </c>
-      <c r="F26" s="566" t="s">
-        <v>883</v>
       </c>
       <c r="G26" s="567" t="s">
         <v>259</v>
@@ -13984,7 +13987,7 @@
         <v>33</v>
       </c>
       <c r="I26" s="578" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="27" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -13993,13 +13996,13 @@
       <c r="E27" s="528"/>
       <c r="F27" s="62"/>
       <c r="G27" s="63" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="H27" s="557" t="s">
         <v>33</v>
       </c>
       <c r="I27" s="717" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="28" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14041,7 +14044,7 @@
         <v>88</v>
       </c>
       <c r="O29" s="576" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="30" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -14060,7 +14063,7 @@
       <c r="J30" s="548"/>
       <c r="K30" s="549"/>
       <c r="L30" s="543" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="M30" s="543" t="s">
         <v>258</v>
@@ -14069,7 +14072,7 @@
         <v>32</v>
       </c>
       <c r="O30" s="709" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.25">
@@ -14084,10 +14087,10 @@
       <c r="J31" s="550"/>
       <c r="K31" s="73"/>
       <c r="L31" s="66" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="M31" s="66" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="N31" s="536" t="s">
         <v>32</v>
@@ -14106,10 +14109,10 @@
       <c r="J32" s="550"/>
       <c r="K32" s="73"/>
       <c r="L32" s="66" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="M32" s="66" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="N32" s="536" t="s">
         <v>32</v>
@@ -14122,7 +14125,7 @@
         <v>73</v>
       </c>
       <c r="E33" s="533" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="F33" s="535" t="s">
         <v>76</v>
@@ -14137,7 +14140,7 @@
         <v>76</v>
       </c>
       <c r="M33" s="66" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="N33" s="536" t="s">
         <v>32</v>
@@ -14160,7 +14163,7 @@
       <c r="J34" s="550"/>
       <c r="K34" s="73"/>
       <c r="L34" s="66" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="M34" s="66" t="s">
         <v>257</v>
@@ -14185,7 +14188,7 @@
         <v>307</v>
       </c>
       <c r="M35" s="66" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="N35" s="536" t="s">
         <v>32</v>
@@ -14204,10 +14207,10 @@
       <c r="J36" s="545"/>
       <c r="K36" s="65"/>
       <c r="L36" s="66" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="M36" s="66" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="N36" s="537" t="s">
         <v>33</v>
@@ -14220,7 +14223,7 @@
         <v>73</v>
       </c>
       <c r="E37" s="81" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="F37" s="82" t="s">
         <v>75</v>
@@ -14239,7 +14242,7 @@
         <v>75</v>
       </c>
       <c r="M37" s="544" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="N37" s="538" t="s">
         <v>33</v>
@@ -14671,7 +14674,7 @@
         <v>88</v>
       </c>
       <c r="O65" s="575" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="66" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -14702,7 +14705,7 @@
         <v>33</v>
       </c>
       <c r="O66" s="706" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="67" spans="3:15" x14ac:dyDescent="0.25">
@@ -16275,43 +16278,43 @@
       <c r="B2" s="594"/>
       <c r="C2" s="595"/>
       <c r="D2" s="718" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E2" s="719"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="720" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="C3" s="721"/>
       <c r="D3" s="596" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E3" s="597" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="598" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="C4" s="155" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="D4" s="599" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E4" s="600"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="598" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="C5" s="155" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="D5" s="599" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E5" s="600"/>
     </row>
@@ -16323,25 +16326,25 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="598" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="C7" s="155" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="D7" s="599" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="E7" s="600"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="598" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="C8" s="155" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="D8" s="599" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="E8" s="600"/>
     </row>
@@ -16353,20 +16356,20 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="598" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="C10" s="155" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="D10" s="599"/>
       <c r="E10" s="600"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="598" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="C11" s="155" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="D11" s="599"/>
       <c r="E11" s="600"/>
@@ -16451,23 +16454,23 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="601" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C25" s="155" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="D25" s="599" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="E25" s="600" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="601"/>
       <c r="C26" s="155"/>
       <c r="D26" s="599" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E26" s="600"/>
     </row>
@@ -16479,23 +16482,23 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="601" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C28" s="155" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="D28" s="599" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E28" s="600" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="601"/>
       <c r="C29" s="155"/>
       <c r="D29" s="599" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E29" s="600"/>
     </row>
@@ -16507,43 +16510,43 @@
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="601" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="C31" s="155" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="D31" s="599" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E31" s="600" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="601"/>
       <c r="C32" s="155"/>
       <c r="D32" s="599" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="E32" s="600"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="601"/>
       <c r="C33" s="155" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D33" s="599" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="E33" s="600" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="601"/>
       <c r="C34" s="155"/>
       <c r="D34" s="599" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E34" s="600"/>
     </row>
@@ -16556,40 +16559,40 @@
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="601"/>
       <c r="C36" s="155" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D36" s="599" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="E36" s="600" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="601"/>
       <c r="C37" s="155"/>
       <c r="D37" s="599" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="E37" s="600"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="601"/>
       <c r="C38" s="155" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D38" s="599" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E38" s="600" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="601"/>
       <c r="C39" s="155"/>
       <c r="D39" s="599" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E39" s="600"/>
     </row>
@@ -16601,10 +16604,10 @@
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="601" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="C41" s="155" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D41" s="599"/>
       <c r="E41" s="600"/>
@@ -16662,21 +16665,21 @@
     <row r="2" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B3" s="591" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C3" s="722" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B4" s="592" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C4" s="723"/>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B5" s="592" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="C5" s="723"/>
       <c r="F5" s="607" t="s">
@@ -16724,23 +16727,23 @@
       </c>
       <c r="AA5" s="606"/>
       <c r="AB5" s="610" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="AC5" s="606"/>
       <c r="AD5" s="606"/>
     </row>
     <row r="6" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B6" s="592" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C6" s="723"/>
       <c r="F6" s="606"/>
       <c r="G6" s="608" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="H6" s="606"/>
       <c r="I6" s="608" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="J6" s="606"/>
       <c r="K6" s="608" t="s">
@@ -16748,33 +16751,33 @@
       </c>
       <c r="L6" s="606"/>
       <c r="M6" s="608" t="s">
+        <v>965</v>
+      </c>
+      <c r="N6" s="606" t="s">
+        <v>960</v>
+      </c>
+      <c r="O6" s="608" t="s">
         <v>966</v>
-      </c>
-      <c r="N6" s="606" t="s">
-        <v>961</v>
-      </c>
-      <c r="O6" s="608" t="s">
-        <v>967</v>
       </c>
       <c r="P6" s="606"/>
       <c r="Q6" s="608" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="R6" s="606"/>
       <c r="S6" s="608" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="T6" s="606"/>
       <c r="U6" s="608" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="V6" s="606"/>
       <c r="W6" s="608" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="X6" s="606"/>
       <c r="Y6" s="608" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="Z6" s="606"/>
       <c r="AA6" s="610" t="s">
@@ -16788,17 +16791,17 @@
     </row>
     <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B7" s="592" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="C7" s="723"/>
       <c r="F7" s="606"/>
       <c r="G7" s="606"/>
       <c r="H7" s="608" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="I7" s="606"/>
       <c r="J7" s="608" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="K7" s="606"/>
       <c r="L7" s="608" t="s">
@@ -16814,21 +16817,21 @@
       </c>
       <c r="Q7" s="606"/>
       <c r="R7" s="608" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="S7" s="606"/>
       <c r="T7" s="608" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="U7" s="606"/>
       <c r="V7" s="608" t="s">
+        <v>976</v>
+      </c>
+      <c r="W7" s="606" t="s">
+        <v>960</v>
+      </c>
+      <c r="X7" s="608" t="s">
         <v>977</v>
-      </c>
-      <c r="W7" s="606" t="s">
-        <v>961</v>
-      </c>
-      <c r="X7" s="608" t="s">
-        <v>978</v>
       </c>
       <c r="Y7" s="606"/>
       <c r="Z7" s="610" t="s">
@@ -16845,7 +16848,7 @@
     </row>
     <row r="8" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B8" s="592" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="C8" s="723"/>
       <c r="F8" s="606"/>
@@ -16854,21 +16857,21 @@
       </c>
       <c r="H8" s="606"/>
       <c r="I8" s="608" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="J8" s="606"/>
       <c r="K8" s="608" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L8" s="606" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="M8" s="608" t="s">
         <v>317</v>
       </c>
       <c r="N8" s="606"/>
       <c r="O8" s="608" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="P8" s="606"/>
       <c r="Q8" s="608" t="s">
@@ -16876,11 +16879,11 @@
       </c>
       <c r="R8" s="606"/>
       <c r="S8" s="608" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="T8" s="606"/>
       <c r="U8" s="608" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="V8" s="606"/>
       <c r="W8" s="611" t="s">
@@ -16900,13 +16903,13 @@
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" s="592" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C9" s="723"/>
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" s="592" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C10" s="723"/>
       <c r="F10" s="610" t="s">
@@ -16961,48 +16964,48 @@
     </row>
     <row r="11" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="592" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="C11" s="723"/>
       <c r="F11" s="606"/>
       <c r="G11" s="608" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="H11" s="606"/>
       <c r="I11" s="608" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="J11" s="606"/>
       <c r="K11" s="608" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="L11" s="606"/>
       <c r="M11" s="608" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="N11" s="606"/>
       <c r="O11" s="608" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="P11" s="606"/>
       <c r="Q11" s="608" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="R11" s="606"/>
       <c r="S11" s="608" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="T11" s="606"/>
       <c r="U11" s="608" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="V11" s="606"/>
       <c r="W11" s="608" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="X11" s="606"/>
       <c r="Y11" s="608" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="Z11" s="606"/>
       <c r="AA11" s="611" t="s">
@@ -17020,39 +17023,39 @@
       <c r="F12" s="606"/>
       <c r="G12" s="606"/>
       <c r="H12" s="608" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="I12" s="606"/>
       <c r="J12" s="608" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="K12" s="606"/>
       <c r="L12" s="608" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="M12" s="606"/>
       <c r="N12" s="608" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="O12" s="606"/>
       <c r="P12" s="608" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="Q12" s="606"/>
       <c r="R12" s="608" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="S12" s="606"/>
       <c r="T12" s="608" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="U12" s="606"/>
       <c r="V12" s="608" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="W12" s="606"/>
       <c r="X12" s="608" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="Y12" s="606"/>
       <c r="Z12" s="611" t="s">
@@ -17069,10 +17072,10 @@
     </row>
     <row r="13" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B13" s="592" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="C13" s="724" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="F13" s="606"/>
       <c r="G13" s="607" t="s">
@@ -17080,33 +17083,33 @@
       </c>
       <c r="H13" s="606"/>
       <c r="I13" s="608" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="J13" s="606"/>
       <c r="K13" s="608" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="L13" s="606"/>
       <c r="M13" s="608" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="N13" s="606"/>
       <c r="O13" s="608" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="P13" s="609"/>
       <c r="Q13" s="608" t="s">
+        <v>958</v>
+      </c>
+      <c r="R13" s="609" t="s">
+        <v>960</v>
+      </c>
+      <c r="S13" s="608" t="s">
         <v>959</v>
-      </c>
-      <c r="R13" s="609" t="s">
-        <v>961</v>
-      </c>
-      <c r="S13" s="608" t="s">
-        <v>960</v>
       </c>
       <c r="T13" s="606"/>
       <c r="U13" s="608" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="V13" s="606"/>
       <c r="W13" s="611" t="s">
@@ -17126,19 +17129,19 @@
     </row>
     <row r="14" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B14" s="592" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C14" s="725"/>
     </row>
     <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B15" s="592" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="C15" s="725"/>
     </row>
     <row r="16" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="593" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="C16" s="726"/>
     </row>
@@ -17156,7 +17159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3341CA24-FB90-4043-B78E-A547E1AF13CD}">
   <dimension ref="B1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
@@ -17189,19 +17192,19 @@
         <v>0</v>
       </c>
       <c r="C3" s="366" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D3" s="414" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="E3" s="421" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="F3" s="422" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="G3" s="430" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17209,19 +17212,19 @@
         <v>0</v>
       </c>
       <c r="C4" s="416" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D4" s="417" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E4" s="423" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="F4" s="424" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="G4" s="431" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17229,19 +17232,19 @@
         <v>0</v>
       </c>
       <c r="C5" s="416" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D5" s="417" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E5" s="423" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F5" s="424" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G5" s="431" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17249,19 +17252,19 @@
         <v>0</v>
       </c>
       <c r="C6" s="416" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D6" s="417" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E6" s="423" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F6" s="424" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="G6" s="431" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17269,19 +17272,19 @@
         <v>0</v>
       </c>
       <c r="C7" s="416" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D7" s="417" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E7" s="423" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="F7" s="424" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G7" s="431" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17289,19 +17292,19 @@
         <v>0</v>
       </c>
       <c r="C8" s="416" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D8" s="417" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E8" s="423" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="F8" s="424" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="G8" s="431" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17309,19 +17312,19 @@
         <v>0</v>
       </c>
       <c r="C9" s="416" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D9" s="417" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E9" s="423" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="F9" s="424" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="G9" s="431" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17329,19 +17332,19 @@
         <v>0</v>
       </c>
       <c r="C10" s="416" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D10" s="417" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E10" s="423" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="F10" s="424" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="G10" s="431" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17349,19 +17352,19 @@
         <v>0</v>
       </c>
       <c r="C11" s="416" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D11" s="417" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E11" s="423" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F11" s="424" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="G11" s="431" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17369,19 +17372,19 @@
         <v>0</v>
       </c>
       <c r="C12" s="416" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D12" s="417" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E12" s="423" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="F12" s="424" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="G12" s="431" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17389,19 +17392,19 @@
         <v>0</v>
       </c>
       <c r="C13" s="416" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D13" s="417" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E13" s="423" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="F13" s="424" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G13" s="431" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -17409,19 +17412,19 @@
         <v>0</v>
       </c>
       <c r="C14" s="630" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D14" s="624" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E14" s="625" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="F14" s="626" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="G14" s="627" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17429,16 +17432,16 @@
         <v>1</v>
       </c>
       <c r="C15" s="366" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D15" s="414" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E15" s="421" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="F15" s="422" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="G15" s="628"/>
     </row>
@@ -17447,19 +17450,19 @@
         <v>1</v>
       </c>
       <c r="C16" s="416" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D16" s="417" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E16" s="423" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="F16" s="424" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="G16" s="431" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17467,19 +17470,19 @@
         <v>1</v>
       </c>
       <c r="C17" s="416" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D17" s="417" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E17" s="423" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F17" s="424" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G17" s="431" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17487,19 +17490,19 @@
         <v>1</v>
       </c>
       <c r="C18" s="416" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D18" s="417" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E18" s="423" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="F18" s="424" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="G18" s="431" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17507,19 +17510,19 @@
         <v>1</v>
       </c>
       <c r="C19" s="416" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D19" s="417" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E19" s="423" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="F19" s="424" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="G19" s="431" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17527,19 +17530,19 @@
         <v>1</v>
       </c>
       <c r="C20" s="416" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D20" s="417" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E20" s="423" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="F20" s="424" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="G20" s="431" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17547,19 +17550,19 @@
         <v>1</v>
       </c>
       <c r="C21" s="416" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D21" s="417" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E21" s="423" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="F21" s="424" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="G21" s="431" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17567,19 +17570,19 @@
         <v>1</v>
       </c>
       <c r="C22" s="416" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D22" s="417" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E22" s="423" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="F22" s="424" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="G22" s="431" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17587,19 +17590,19 @@
         <v>1</v>
       </c>
       <c r="C23" s="416" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D23" s="417" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E23" s="423" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="F23" s="424" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="G23" s="431" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17607,19 +17610,19 @@
         <v>1</v>
       </c>
       <c r="C24" s="416" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D24" s="417" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E24" s="423" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="F24" s="424" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="G24" s="431" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -17627,16 +17630,16 @@
         <v>1</v>
       </c>
       <c r="C25" s="416" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D25" s="417" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E25" s="423" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="F25" s="424" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="G25" s="434"/>
     </row>
@@ -17645,16 +17648,16 @@
         <v>1</v>
       </c>
       <c r="C26" s="419" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D26" s="420" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="E26" s="631" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F26" s="632" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G26" s="429"/>
     </row>
@@ -17663,16 +17666,16 @@
         <v>2</v>
       </c>
       <c r="C27" s="416" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D27" s="417" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E27" s="423" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="F27" s="424" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="G27" s="427"/>
     </row>
@@ -17681,16 +17684,16 @@
         <v>2</v>
       </c>
       <c r="C28" s="416" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D28" s="417" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E28" s="431" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="F28" s="424" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="G28" s="427"/>
     </row>
@@ -17699,16 +17702,16 @@
         <v>2</v>
       </c>
       <c r="C29" s="416" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D29" s="417" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E29" s="431" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="F29" s="424" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="G29" s="427"/>
     </row>
@@ -17717,16 +17720,16 @@
         <v>2</v>
       </c>
       <c r="C30" s="619" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D30" s="620" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E30" s="621" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="F30" s="622" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="G30" s="623"/>
     </row>
@@ -17735,16 +17738,16 @@
         <v>2</v>
       </c>
       <c r="C31" s="613" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D31" s="614" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E31" s="615" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F31" s="616" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="G31" s="617"/>
     </row>
@@ -17753,16 +17756,16 @@
         <v>2</v>
       </c>
       <c r="C32" s="416" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D32" s="417" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="E32" s="431" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="F32" s="424" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="G32" s="427"/>
     </row>
@@ -17771,13 +17774,13 @@
         <v>2</v>
       </c>
       <c r="C33" s="416" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D33" s="417" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E33" s="431" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="F33" s="426"/>
       <c r="G33" s="427"/>
@@ -17787,10 +17790,10 @@
         <v>2</v>
       </c>
       <c r="C34" s="416" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D34" s="417" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E34" s="425"/>
       <c r="F34" s="426"/>
@@ -17801,10 +17804,10 @@
         <v>2</v>
       </c>
       <c r="C35" s="416" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D35" s="417" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E35" s="425"/>
       <c r="F35" s="426"/>
@@ -17815,13 +17818,13 @@
         <v>2</v>
       </c>
       <c r="C36" s="416" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D36" s="417" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="E36" s="431" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="F36" s="426"/>
       <c r="G36" s="427"/>
@@ -17831,13 +17834,13 @@
         <v>2</v>
       </c>
       <c r="C37" s="416" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D37" s="417" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="E37" s="431" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="F37" s="426"/>
       <c r="G37" s="427"/>
@@ -17847,13 +17850,13 @@
         <v>2</v>
       </c>
       <c r="C38" s="419" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D38" s="420" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E38" s="633" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="F38" s="428"/>
       <c r="G38" s="429"/>
@@ -17863,13 +17866,13 @@
         <v>3</v>
       </c>
       <c r="C39" s="416" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D39" s="417" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E39" s="432" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="F39" s="426"/>
       <c r="G39" s="427"/>
@@ -17879,13 +17882,13 @@
         <v>3</v>
       </c>
       <c r="C40" s="416" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D40" s="417" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E40" s="432" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="F40" s="426"/>
       <c r="G40" s="427"/>
@@ -17895,13 +17898,13 @@
         <v>3</v>
       </c>
       <c r="C41" s="416" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D41" s="417" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E41" s="432" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="F41" s="426"/>
       <c r="G41" s="427"/>
@@ -17911,13 +17914,13 @@
         <v>3</v>
       </c>
       <c r="C42" s="416" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D42" s="417" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E42" s="432" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="F42" s="426"/>
       <c r="G42" s="427"/>
@@ -17927,13 +17930,13 @@
         <v>3</v>
       </c>
       <c r="C43" s="416" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D43" s="417" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E43" s="432" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F43" s="426"/>
       <c r="G43" s="427"/>
@@ -17943,13 +17946,13 @@
         <v>3</v>
       </c>
       <c r="C44" s="416" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D44" s="417" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E44" s="432" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F44" s="426"/>
       <c r="G44" s="427"/>
@@ -17959,13 +17962,13 @@
         <v>3</v>
       </c>
       <c r="C45" s="416" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D45" s="417" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E45" s="432" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="F45" s="426"/>
       <c r="G45" s="427"/>
@@ -17975,13 +17978,13 @@
         <v>3</v>
       </c>
       <c r="C46" s="416" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D46" s="417" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E46" s="432" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="F46" s="426"/>
       <c r="G46" s="427"/>
@@ -17991,13 +17994,13 @@
         <v>3</v>
       </c>
       <c r="C47" s="416" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D47" s="417" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E47" s="432" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F47" s="426"/>
       <c r="G47" s="427"/>
@@ -18007,13 +18010,13 @@
         <v>3</v>
       </c>
       <c r="C48" s="416" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D48" s="417" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E48" s="432" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F48" s="426"/>
       <c r="G48" s="427"/>
@@ -18023,13 +18026,13 @@
         <v>3</v>
       </c>
       <c r="C49" s="416" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D49" s="417" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E49" s="432" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F49" s="426"/>
       <c r="G49" s="427"/>
@@ -18039,13 +18042,13 @@
         <v>3</v>
       </c>
       <c r="C50" s="419" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D50" s="420" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E50" s="433" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F50" s="428"/>
       <c r="G50" s="429"/>
@@ -18075,11 +18078,11 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="727" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C1" s="728"/>
       <c r="D1" s="390" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E1" s="339"/>
       <c r="F1" s="339"/>
@@ -18093,51 +18096,51 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="140" t="s">
+        <v>650</v>
+      </c>
+      <c r="C2" s="141" t="s">
         <v>651</v>
-      </c>
-      <c r="C2" s="141" t="s">
-        <v>652</v>
       </c>
       <c r="D2" s="139"/>
       <c r="E2" s="403" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="F2" s="403" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G2" s="403" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H2" s="382" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I2" s="382" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="J2" s="382" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="400" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="383" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B3" s="384">
         <v>0</v>
       </c>
       <c r="C3" s="387" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D3" s="391" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E3" s="401"/>
       <c r="F3" s="401" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="G3" s="401"/>
       <c r="H3" s="27"/>
@@ -18145,7 +18148,7 @@
       <c r="J3" s="27"/>
       <c r="K3" s="45"/>
       <c r="L3" s="396" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -18172,7 +18175,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="388" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D5" s="48"/>
       <c r="E5" s="16"/>
@@ -18190,20 +18193,20 @@
         <v>6</v>
       </c>
       <c r="C6" s="388" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D6" s="392" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E6" s="402" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F6" s="402"/>
       <c r="G6" s="402"/>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
       <c r="J6" s="368" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="K6" s="43"/>
       <c r="L6" s="397"/>
@@ -18217,17 +18220,17 @@
         <v>389</v>
       </c>
       <c r="D7" s="392" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E7" s="402" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F7" s="402"/>
       <c r="G7" s="402"/>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
       <c r="J7" s="368" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="K7" s="43"/>
       <c r="L7" s="397"/>
@@ -18238,7 +18241,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="388" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D8" s="48"/>
       <c r="E8" s="16"/>
@@ -18256,7 +18259,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="388" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D9" s="48"/>
       <c r="E9" s="16"/>
@@ -18274,7 +18277,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="388" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D10" s="48"/>
       <c r="E10" s="16"/>
@@ -18295,11 +18298,11 @@
         <v>367</v>
       </c>
       <c r="D11" s="392" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E11" s="402"/>
       <c r="F11" s="402" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G11" s="402"/>
       <c r="H11" s="17"/>
@@ -18307,7 +18310,7 @@
       <c r="J11" s="17"/>
       <c r="K11" s="43"/>
       <c r="L11" s="398" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -18355,17 +18358,17 @@
         <v>379</v>
       </c>
       <c r="D14" s="392" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E14" s="402" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F14" s="402"/>
       <c r="G14" s="402"/>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
       <c r="J14" s="368" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="K14" s="43"/>
       <c r="L14" s="397"/>
@@ -18379,17 +18382,17 @@
         <v>129</v>
       </c>
       <c r="D15" s="392" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E15" s="402" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="F15" s="402"/>
       <c r="G15" s="402"/>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
       <c r="J15" s="368" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="K15" s="43"/>
       <c r="L15" s="397"/>
@@ -18400,7 +18403,7 @@
         <v>26</v>
       </c>
       <c r="C16" s="388" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D16" s="48"/>
       <c r="E16" s="16"/>
@@ -18418,7 +18421,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="388" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D17" s="48"/>
       <c r="E17" s="16"/>
@@ -18436,7 +18439,7 @@
         <v>30</v>
       </c>
       <c r="C18" s="388" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D18" s="48"/>
       <c r="E18" s="16"/>
@@ -18454,7 +18457,7 @@
         <v>32</v>
       </c>
       <c r="C19" s="388" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D19" s="48"/>
       <c r="E19" s="16"/>
@@ -18465,7 +18468,7 @@
       <c r="J19" s="17"/>
       <c r="K19" s="43"/>
       <c r="L19" s="398" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -18474,7 +18477,7 @@
         <v>34</v>
       </c>
       <c r="C20" s="388" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D20" s="48"/>
       <c r="E20" s="16"/>
@@ -18492,14 +18495,14 @@
         <v>36</v>
       </c>
       <c r="C21" s="388" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D21" s="392" t="s">
         <v>54</v>
       </c>
       <c r="E21" s="402"/>
       <c r="F21" s="404" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="G21" s="402"/>
       <c r="H21" s="17"/>
@@ -18516,7 +18519,7 @@
         <v>38</v>
       </c>
       <c r="C22" s="388" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D22" s="48"/>
       <c r="E22" s="16"/>
@@ -18525,7 +18528,7 @@
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
       <c r="J22" s="368" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="K22" s="43"/>
       <c r="L22" s="397"/>
@@ -18536,17 +18539,17 @@
         <v>40</v>
       </c>
       <c r="C23" s="388" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D23" s="392"/>
       <c r="E23" s="402"/>
       <c r="F23" s="402"/>
       <c r="G23" s="402"/>
       <c r="H23" s="368" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="I23" s="368" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="J23" s="17"/>
       <c r="K23" s="43"/>
@@ -18558,7 +18561,7 @@
         <v>42</v>
       </c>
       <c r="C24" s="388" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D24" s="48"/>
       <c r="E24" s="16"/>
@@ -18576,7 +18579,7 @@
         <v>44</v>
       </c>
       <c r="C25" s="388" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D25" s="48"/>
       <c r="E25" s="16"/>
@@ -18594,7 +18597,7 @@
         <v>46</v>
       </c>
       <c r="C26" s="388" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D26" s="48"/>
       <c r="E26" s="16"/>
@@ -18612,7 +18615,7 @@
         <v>48</v>
       </c>
       <c r="C27" s="388" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D27" s="48"/>
       <c r="E27" s="16"/>
@@ -18623,7 +18626,7 @@
       <c r="J27" s="17"/>
       <c r="K27" s="43"/>
       <c r="L27" s="398" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -18632,7 +18635,7 @@
         <v>50</v>
       </c>
       <c r="C28" s="388" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D28" s="48"/>
       <c r="E28" s="16"/>
@@ -18650,7 +18653,7 @@
         <v>52</v>
       </c>
       <c r="C29" s="388" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D29" s="48"/>
       <c r="E29" s="16"/>
@@ -18668,7 +18671,7 @@
         <v>54</v>
       </c>
       <c r="C30" s="388" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D30" s="48"/>
       <c r="E30" s="16"/>
@@ -18677,7 +18680,7 @@
       <c r="H30" s="17"/>
       <c r="I30" s="17"/>
       <c r="J30" s="368" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="K30" s="43"/>
       <c r="L30" s="397"/>
@@ -18688,7 +18691,7 @@
         <v>56</v>
       </c>
       <c r="C31" s="388" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D31" s="48"/>
       <c r="E31" s="16"/>
@@ -18696,7 +18699,7 @@
       <c r="G31" s="16"/>
       <c r="H31" s="368"/>
       <c r="I31" s="368" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J31" s="17"/>
       <c r="K31" s="43"/>
@@ -18708,7 +18711,7 @@
         <v>58</v>
       </c>
       <c r="C32" s="388" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D32" s="48"/>
       <c r="E32" s="16"/>
@@ -18726,7 +18729,7 @@
         <v>60</v>
       </c>
       <c r="C33" s="388" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D33" s="48"/>
       <c r="E33" s="16"/>
@@ -18744,7 +18747,7 @@
         <v>62</v>
       </c>
       <c r="C34" s="388" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D34" s="48"/>
       <c r="E34" s="16"/>
@@ -18762,7 +18765,7 @@
         <v>64</v>
       </c>
       <c r="C35" s="388" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D35" s="48"/>
       <c r="E35" s="16"/>
@@ -18773,7 +18776,7 @@
       <c r="J35" s="17"/>
       <c r="K35" s="43"/>
       <c r="L35" s="398" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -18782,7 +18785,7 @@
         <v>66</v>
       </c>
       <c r="C36" s="388" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D36" s="48"/>
       <c r="E36" s="16"/>
@@ -18800,7 +18803,7 @@
         <v>68</v>
       </c>
       <c r="C37" s="388" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D37" s="48"/>
       <c r="E37" s="16"/>
@@ -18818,7 +18821,7 @@
         <v>70</v>
       </c>
       <c r="C38" s="388" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D38" s="48"/>
       <c r="E38" s="16"/>
@@ -18836,13 +18839,13 @@
         <v>72</v>
       </c>
       <c r="C39" s="388" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D39" s="392" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="E39" s="402" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="F39" s="402"/>
       <c r="G39" s="402"/>
@@ -18858,7 +18861,7 @@
         <v>74</v>
       </c>
       <c r="C40" s="388" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D40" s="48"/>
       <c r="E40" s="16"/>
@@ -18876,13 +18879,13 @@
         <v>76</v>
       </c>
       <c r="C41" s="388" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D41" s="392" t="s">
         <v>485</v>
       </c>
       <c r="E41" s="402" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="F41" s="402"/>
       <c r="G41" s="402"/>
@@ -18898,7 +18901,7 @@
         <v>78</v>
       </c>
       <c r="C42" s="388" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D42" s="48"/>
       <c r="E42" s="16"/>
@@ -18916,7 +18919,7 @@
         <v>80</v>
       </c>
       <c r="C43" s="388" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D43" s="48"/>
       <c r="E43" s="16"/>
@@ -18927,7 +18930,7 @@
       <c r="J43" s="17"/>
       <c r="K43" s="43"/>
       <c r="L43" s="398" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -18936,7 +18939,7 @@
         <v>82</v>
       </c>
       <c r="C44" s="388" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D44" s="48"/>
       <c r="E44" s="16"/>
@@ -18954,7 +18957,7 @@
         <v>84</v>
       </c>
       <c r="C45" s="388" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D45" s="48"/>
       <c r="E45" s="16"/>
@@ -18972,7 +18975,7 @@
         <v>86</v>
       </c>
       <c r="C46" s="388" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D46" s="48"/>
       <c r="E46" s="16"/>
@@ -18990,20 +18993,20 @@
         <v>88</v>
       </c>
       <c r="C47" s="388" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D47" s="392" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E47" s="402"/>
       <c r="F47" s="402"/>
       <c r="G47" s="404" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="H47" s="17"/>
       <c r="I47" s="17"/>
       <c r="J47" s="368" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="K47" s="43"/>
       <c r="L47" s="397"/>
@@ -19014,7 +19017,7 @@
         <v>90</v>
       </c>
       <c r="C48" s="388" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D48" s="48"/>
       <c r="E48" s="16"/>
@@ -19032,7 +19035,7 @@
         <v>92</v>
       </c>
       <c r="C49" s="388" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D49" s="48"/>
       <c r="E49" s="16"/>
@@ -19050,7 +19053,7 @@
         <v>94</v>
       </c>
       <c r="C50" s="388" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D50" s="48"/>
       <c r="E50" s="16"/>
@@ -19068,7 +19071,7 @@
         <v>96</v>
       </c>
       <c r="C51" s="388" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D51" s="48"/>
       <c r="E51" s="16"/>
@@ -19079,7 +19082,7 @@
       <c r="J51" s="17"/>
       <c r="K51" s="43"/>
       <c r="L51" s="398" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -19088,7 +19091,7 @@
         <v>98</v>
       </c>
       <c r="C52" s="388" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D52" s="48"/>
       <c r="E52" s="16"/>
@@ -19106,7 +19109,7 @@
         <v>100</v>
       </c>
       <c r="C53" s="388" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D53" s="48"/>
       <c r="E53" s="16"/>
@@ -19124,7 +19127,7 @@
         <v>102</v>
       </c>
       <c r="C54" s="388" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D54" s="48"/>
       <c r="E54" s="16"/>
@@ -19142,21 +19145,21 @@
         <v>104</v>
       </c>
       <c r="C55" s="388" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D55" s="392"/>
       <c r="E55" s="402" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="F55" s="402"/>
       <c r="G55" s="402"/>
       <c r="H55" s="368" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="I55" s="368"/>
       <c r="J55" s="17"/>
       <c r="K55" s="394" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="L55" s="397"/>
     </row>
@@ -19166,7 +19169,7 @@
         <v>106</v>
       </c>
       <c r="C56" s="388" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D56" s="48"/>
       <c r="E56" s="16"/>
@@ -19184,7 +19187,7 @@
         <v>108</v>
       </c>
       <c r="C57" s="388" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D57" s="48"/>
       <c r="E57" s="16"/>
@@ -19202,7 +19205,7 @@
         <v>110</v>
       </c>
       <c r="C58" s="388" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D58" s="48"/>
       <c r="E58" s="16"/>
@@ -19231,7 +19234,7 @@
       <c r="J59" s="17"/>
       <c r="K59" s="43"/>
       <c r="L59" s="398" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
@@ -19240,7 +19243,7 @@
         <v>114</v>
       </c>
       <c r="C60" s="388" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D60" s="48"/>
       <c r="E60" s="16"/>
@@ -19258,20 +19261,20 @@
         <v>116</v>
       </c>
       <c r="C61" s="388" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D61" s="392" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E61" s="402" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="F61" s="402"/>
       <c r="G61" s="402"/>
       <c r="H61" s="17"/>
       <c r="I61" s="17"/>
       <c r="J61" s="368" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="K61" s="43"/>
       <c r="L61" s="397"/>
@@ -19282,20 +19285,20 @@
         <v>118</v>
       </c>
       <c r="C62" s="388" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D62" s="392" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E62" s="402" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="F62" s="402"/>
       <c r="G62" s="402"/>
       <c r="H62" s="17"/>
       <c r="I62" s="17"/>
       <c r="J62" s="368" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="K62" s="43"/>
       <c r="L62" s="397"/>
@@ -19306,7 +19309,7 @@
         <v>120</v>
       </c>
       <c r="C63" s="388" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D63" s="48"/>
       <c r="E63" s="16"/>
@@ -19324,7 +19327,7 @@
         <v>122</v>
       </c>
       <c r="C64" s="388" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D64" s="48"/>
       <c r="E64" s="16"/>
@@ -19342,7 +19345,7 @@
         <v>124</v>
       </c>
       <c r="C65" s="388" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D65" s="48"/>
       <c r="E65" s="16"/>
@@ -19360,7 +19363,7 @@
         <v>126</v>
       </c>
       <c r="C66" s="389" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D66" s="49"/>
       <c r="E66" s="20"/>

</xml_diff>

<commit_message>
new file:   0 SYS-sourcen/S1/TRACE/TRACE.REL 	new file:   DOC/images/Bildschirm.jpg 	new file:   DOC/images/DEG2000.jpg 	new file:   DOC/images/DEG2000.psd 	new file:   DOC/images/Laufwerke.jpg 	new file:   DOC/images/Tastatur.jpg 	new file:   DOC/images/Zentrale.jpg 	new file:   DOC/screen Probleme/S44/hc0059.jpg 	new file:   DOC/screen Probleme/S44/hc0060.jpg 	new file:   DOC/screen Probleme/S44/hc0061.jpg 	new file:   DOC/screen Probleme/S44/hc0062.jpg 	new file:   DOC/screen Probleme/S44/hc0063.jpg 	new file:   DOC/screen Probleme/S44/hc0064.jpg 	modified:   README.md
</commit_message>
<xml_diff>
--- a/DOC/DEG2000.xlsx
+++ b/DOC/DEG2000.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\devel\1 DEG2000\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E86DE6C-E08A-4AD2-A288-40073CB82B22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2426431E-4C8F-4056-AF0C-5BCAC653128A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22020" windowHeight="11100" firstSheet="4" activeTab="9" xr2:uid="{F91C61BF-F393-4C13-9000-551DF6FEF055}"/>
   </bookViews>
@@ -3093,9 +3093,6 @@
     <t>Pufferadresse ?</t>
   </si>
   <si>
-    <t>HS-Bereich !!!!</t>
-  </si>
-  <si>
     <t>K0.LPD</t>
   </si>
   <si>
@@ -3103,6 +3100,9 @@
   </si>
   <si>
     <t>Länge der Daten  im Puffer  10</t>
+  </si>
+  <si>
+    <t>Zähler für "Kmbg"</t>
   </si>
 </sst>
 </file>
@@ -8264,24 +8264,6 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="235" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="115" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="115" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="129" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="115" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="129" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="15" fillId="11" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -8349,9 +8331,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="252" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="270" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="246" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8385,16 +8364,40 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="243" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="277" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="278" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="279" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -8410,119 +8413,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="68" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -8576,24 +8524,88 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="68" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="184" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="185" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="192" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="200" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="178" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="201" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="180" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="181" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="187" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="188" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8602,25 +8614,13 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="186" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="187" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="203" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="179" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="176" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="180" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="181" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="200" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="178" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="179" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="188" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -8631,10 +8631,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="178" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="201" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="184" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="203" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="185" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="192" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="216" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8752,35 +8755,32 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="138" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="277" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="278" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="279" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="270" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="15" borderId="115" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="115" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="129" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="241" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="240" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9135,16 +9135,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="6"/>
-      <c r="F1" s="704" t="s">
+      <c r="F1" s="705" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="705"/>
-      <c r="H1" s="705"/>
-      <c r="I1" s="706" t="s">
+      <c r="G1" s="706"/>
+      <c r="H1" s="706"/>
+      <c r="I1" s="707" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="707"/>
-      <c r="K1" s="708"/>
+      <c r="J1" s="708"/>
+      <c r="K1" s="709"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
@@ -9486,7 +9486,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B62" sqref="B62"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55:B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9532,46 +9532,46 @@
       <c r="K3" s="565"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="687"/>
-      <c r="C4" s="696"/>
-      <c r="D4" s="828" t="s">
+      <c r="B4" s="681"/>
+      <c r="C4" s="689"/>
+      <c r="D4" s="696" t="s">
+        <v>985</v>
+      </c>
+      <c r="E4" s="698">
+        <v>6</v>
+      </c>
+      <c r="F4" s="828">
+        <v>1</v>
+      </c>
+      <c r="G4" s="691" t="s">
+        <v>112</v>
+      </c>
+      <c r="H4" s="692"/>
+      <c r="I4" s="683"/>
+      <c r="J4" s="684"/>
+      <c r="K4" s="685"/>
+    </row>
+    <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="682"/>
+      <c r="C5" s="690"/>
+      <c r="D5" s="697" t="s">
+        <v>984</v>
+      </c>
+      <c r="E5" s="699">
+        <v>2</v>
+      </c>
+      <c r="F5" s="829">
+        <v>2</v>
+      </c>
+      <c r="G5" s="688" t="s">
         <v>986</v>
       </c>
-      <c r="E4" s="830">
-        <v>6</v>
-      </c>
-      <c r="F4" s="700">
-        <v>1</v>
-      </c>
-      <c r="G4" s="698" t="s">
-        <v>112</v>
-      </c>
-      <c r="H4" s="699"/>
-      <c r="I4" s="690"/>
-      <c r="J4" s="691"/>
-      <c r="K4" s="692"/>
-    </row>
-    <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="689"/>
-      <c r="C5" s="697"/>
-      <c r="D5" s="829" t="s">
-        <v>985</v>
-      </c>
-      <c r="E5" s="831">
-        <v>2</v>
-      </c>
-      <c r="F5" s="701">
-        <v>2</v>
-      </c>
-      <c r="G5" s="695" t="s">
-        <v>987</v>
-      </c>
-      <c r="H5" s="693"/>
-      <c r="I5" s="693"/>
-      <c r="J5" s="694" t="s">
+      <c r="H5" s="686"/>
+      <c r="I5" s="686"/>
+      <c r="J5" s="687" t="s">
         <v>407</v>
       </c>
-      <c r="K5" s="827" t="s">
+      <c r="K5" s="695" t="s">
         <v>408</v>
       </c>
     </row>
@@ -9585,10 +9585,10 @@
       <c r="D6" s="302" t="s">
         <v>343</v>
       </c>
-      <c r="E6" s="832">
+      <c r="E6" s="700">
         <v>0</v>
       </c>
-      <c r="F6" s="688">
+      <c r="F6" s="830">
         <v>3</v>
       </c>
       <c r="G6" s="397" t="s">
@@ -9609,8 +9609,8 @@
       <c r="B7" s="568"/>
       <c r="C7" s="298"/>
       <c r="D7" s="303"/>
-      <c r="E7" s="833"/>
-      <c r="F7" s="659"/>
+      <c r="E7" s="701"/>
+      <c r="F7" s="831"/>
       <c r="G7" s="259"/>
       <c r="H7" s="247"/>
       <c r="I7" s="220">
@@ -9625,8 +9625,8 @@
       <c r="B8" s="568"/>
       <c r="C8" s="298"/>
       <c r="D8" s="303"/>
-      <c r="E8" s="833"/>
-      <c r="F8" s="659"/>
+      <c r="E8" s="701"/>
+      <c r="F8" s="831"/>
       <c r="G8" s="259"/>
       <c r="H8" s="247">
         <v>1</v>
@@ -9641,8 +9641,8 @@
       <c r="B9" s="568"/>
       <c r="C9" s="298"/>
       <c r="D9" s="303"/>
-      <c r="E9" s="833"/>
-      <c r="F9" s="659"/>
+      <c r="E9" s="701"/>
+      <c r="F9" s="831"/>
       <c r="G9" s="259"/>
       <c r="H9" s="247"/>
       <c r="I9" s="220">
@@ -9657,8 +9657,8 @@
       <c r="B10" s="568"/>
       <c r="C10" s="298"/>
       <c r="D10" s="303"/>
-      <c r="E10" s="833"/>
-      <c r="F10" s="659"/>
+      <c r="E10" s="701"/>
+      <c r="F10" s="831"/>
       <c r="G10" s="259"/>
       <c r="H10" s="247">
         <v>2</v>
@@ -9675,8 +9675,8 @@
       <c r="B11" s="568"/>
       <c r="C11" s="298"/>
       <c r="D11" s="303"/>
-      <c r="E11" s="833"/>
-      <c r="F11" s="659"/>
+      <c r="E11" s="701"/>
+      <c r="F11" s="831"/>
       <c r="G11" s="259"/>
       <c r="H11" s="247"/>
       <c r="I11" s="220">
@@ -9691,8 +9691,8 @@
       <c r="B12" s="568"/>
       <c r="C12" s="298"/>
       <c r="D12" s="303"/>
-      <c r="E12" s="833"/>
-      <c r="F12" s="659"/>
+      <c r="E12" s="701"/>
+      <c r="F12" s="831"/>
       <c r="G12" s="259"/>
       <c r="H12" s="247">
         <v>3</v>
@@ -9703,7 +9703,7 @@
       <c r="J12" s="220" t="s">
         <v>354</v>
       </c>
-      <c r="K12" s="812" t="s">
+      <c r="K12" s="813" t="s">
         <v>362</v>
       </c>
     </row>
@@ -9711,8 +9711,8 @@
       <c r="B13" s="568"/>
       <c r="C13" s="298"/>
       <c r="D13" s="303"/>
-      <c r="E13" s="833"/>
-      <c r="F13" s="659"/>
+      <c r="E13" s="701"/>
+      <c r="F13" s="831"/>
       <c r="G13" s="259"/>
       <c r="H13" s="247"/>
       <c r="I13" s="220">
@@ -9721,14 +9721,14 @@
       <c r="J13" s="220" t="s">
         <v>355</v>
       </c>
-      <c r="K13" s="812"/>
+      <c r="K13" s="813"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="570"/>
       <c r="C14" s="299"/>
       <c r="D14" s="35"/>
-      <c r="E14" s="834"/>
-      <c r="F14" s="660"/>
+      <c r="E14" s="702"/>
+      <c r="F14" s="832"/>
       <c r="G14" s="260"/>
       <c r="H14" s="248">
         <v>4</v>
@@ -9745,8 +9745,8 @@
       <c r="B15" s="570"/>
       <c r="C15" s="300"/>
       <c r="D15" s="304"/>
-      <c r="E15" s="834"/>
-      <c r="F15" s="660"/>
+      <c r="E15" s="702"/>
+      <c r="F15" s="832"/>
       <c r="G15" s="260"/>
       <c r="H15" s="248"/>
       <c r="I15" s="220">
@@ -9761,8 +9761,8 @@
       <c r="B16" s="570"/>
       <c r="C16" s="300"/>
       <c r="D16" s="304"/>
-      <c r="E16" s="834"/>
-      <c r="F16" s="660"/>
+      <c r="E16" s="702"/>
+      <c r="F16" s="832"/>
       <c r="G16" s="260"/>
       <c r="H16" s="248">
         <v>5</v>
@@ -9779,8 +9779,8 @@
       <c r="B17" s="570"/>
       <c r="C17" s="300"/>
       <c r="D17" s="304"/>
-      <c r="E17" s="834"/>
-      <c r="F17" s="660"/>
+      <c r="E17" s="702"/>
+      <c r="F17" s="832"/>
       <c r="G17" s="260"/>
       <c r="H17" s="248"/>
       <c r="I17" s="220">
@@ -9795,8 +9795,8 @@
       <c r="B18" s="570"/>
       <c r="C18" s="300"/>
       <c r="D18" s="304"/>
-      <c r="E18" s="834"/>
-      <c r="F18" s="660"/>
+      <c r="E18" s="702"/>
+      <c r="F18" s="832"/>
       <c r="G18" s="260"/>
       <c r="H18" s="248">
         <v>6</v>
@@ -9807,7 +9807,7 @@
       <c r="J18" s="220" t="s">
         <v>360</v>
       </c>
-      <c r="K18" s="812" t="s">
+      <c r="K18" s="813" t="s">
         <v>362</v>
       </c>
     </row>
@@ -9815,8 +9815,8 @@
       <c r="B19" s="570"/>
       <c r="C19" s="300"/>
       <c r="D19" s="304"/>
-      <c r="E19" s="834"/>
-      <c r="F19" s="660"/>
+      <c r="E19" s="702"/>
+      <c r="F19" s="832"/>
       <c r="G19" s="260"/>
       <c r="H19" s="248"/>
       <c r="I19" s="220">
@@ -9825,14 +9825,14 @@
       <c r="J19" s="220" t="s">
         <v>361</v>
       </c>
-      <c r="K19" s="812"/>
+      <c r="K19" s="813"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="570"/>
       <c r="C20" s="300"/>
       <c r="D20" s="304"/>
-      <c r="E20" s="834"/>
-      <c r="F20" s="660"/>
+      <c r="E20" s="702"/>
+      <c r="F20" s="832"/>
       <c r="G20" s="260"/>
       <c r="H20" s="248">
         <v>7</v>
@@ -9849,8 +9849,8 @@
       <c r="B21" s="571"/>
       <c r="C21" s="301"/>
       <c r="D21" s="305"/>
-      <c r="E21" s="835"/>
-      <c r="F21" s="661"/>
+      <c r="E21" s="703"/>
+      <c r="F21" s="833"/>
       <c r="G21" s="261"/>
       <c r="H21" s="249"/>
       <c r="I21" s="222">
@@ -9871,10 +9871,10 @@
       <c r="D22" s="306" t="s">
         <v>343</v>
       </c>
-      <c r="E22" s="836">
+      <c r="E22" s="704">
         <v>1</v>
       </c>
-      <c r="F22" s="662">
+      <c r="F22" s="834">
         <v>4</v>
       </c>
       <c r="G22" s="262" t="s">
@@ -9889,8 +9889,8 @@
       <c r="B23" s="575"/>
       <c r="C23" s="237"/>
       <c r="D23" s="304"/>
-      <c r="E23" s="834"/>
-      <c r="F23" s="663"/>
+      <c r="E23" s="702"/>
+      <c r="F23" s="832"/>
       <c r="G23" s="263"/>
       <c r="H23" s="251"/>
       <c r="I23" s="224" t="s">
@@ -9905,8 +9905,8 @@
       <c r="B24" s="575"/>
       <c r="C24" s="237"/>
       <c r="D24" s="304"/>
-      <c r="E24" s="834"/>
-      <c r="F24" s="663"/>
+      <c r="E24" s="702"/>
+      <c r="F24" s="832"/>
       <c r="G24" s="263"/>
       <c r="H24" s="251"/>
       <c r="I24" s="224" t="s">
@@ -9921,8 +9921,8 @@
       <c r="B25" s="575"/>
       <c r="C25" s="237"/>
       <c r="D25" s="304"/>
-      <c r="E25" s="834"/>
-      <c r="F25" s="663"/>
+      <c r="E25" s="702"/>
+      <c r="F25" s="832"/>
       <c r="G25" s="263"/>
       <c r="H25" s="251"/>
       <c r="I25" s="224" t="s">
@@ -9937,8 +9937,8 @@
       <c r="B26" s="575"/>
       <c r="C26" s="237"/>
       <c r="D26" s="304"/>
-      <c r="E26" s="834"/>
-      <c r="F26" s="663"/>
+      <c r="E26" s="702"/>
+      <c r="F26" s="832"/>
       <c r="G26" s="263"/>
       <c r="H26" s="251"/>
       <c r="I26" s="224" t="s">
@@ -9953,8 +9953,8 @@
       <c r="B27" s="575"/>
       <c r="C27" s="237"/>
       <c r="D27" s="304"/>
-      <c r="E27" s="834"/>
-      <c r="F27" s="663"/>
+      <c r="E27" s="702"/>
+      <c r="F27" s="832"/>
       <c r="G27" s="263"/>
       <c r="H27" s="251"/>
       <c r="I27" s="224" t="s">
@@ -9969,8 +9969,8 @@
       <c r="B28" s="575"/>
       <c r="C28" s="237"/>
       <c r="D28" s="304"/>
-      <c r="E28" s="834"/>
-      <c r="F28" s="663"/>
+      <c r="E28" s="702"/>
+      <c r="F28" s="832"/>
       <c r="G28" s="263"/>
       <c r="H28" s="251"/>
       <c r="I28" s="224" t="s">
@@ -9985,8 +9985,8 @@
       <c r="B29" s="575"/>
       <c r="C29" s="237"/>
       <c r="D29" s="304"/>
-      <c r="E29" s="834"/>
-      <c r="F29" s="663"/>
+      <c r="E29" s="702"/>
+      <c r="F29" s="832"/>
       <c r="G29" s="263"/>
       <c r="H29" s="251"/>
       <c r="I29" s="224" t="s">
@@ -10001,8 +10001,8 @@
       <c r="B30" s="575"/>
       <c r="C30" s="237"/>
       <c r="D30" s="304"/>
-      <c r="E30" s="834"/>
-      <c r="F30" s="663"/>
+      <c r="E30" s="702"/>
+      <c r="F30" s="832"/>
       <c r="G30" s="263"/>
       <c r="H30" s="251"/>
       <c r="I30" s="224" t="s">
@@ -10017,8 +10017,8 @@
       <c r="B31" s="575"/>
       <c r="C31" s="237"/>
       <c r="D31" s="304"/>
-      <c r="E31" s="834"/>
-      <c r="F31" s="663"/>
+      <c r="E31" s="702"/>
+      <c r="F31" s="832"/>
       <c r="G31" s="263"/>
       <c r="H31" s="251"/>
       <c r="I31" s="224" t="s">
@@ -10033,8 +10033,8 @@
       <c r="B32" s="577"/>
       <c r="C32" s="238"/>
       <c r="D32" s="305"/>
-      <c r="E32" s="835"/>
-      <c r="F32" s="664"/>
+      <c r="E32" s="703"/>
+      <c r="F32" s="833"/>
       <c r="G32" s="264"/>
       <c r="H32" s="252"/>
       <c r="I32" s="225" t="s">
@@ -10049,16 +10049,14 @@
       <c r="B33" s="579" t="s">
         <v>332</v>
       </c>
-      <c r="C33" s="702">
+      <c r="C33" s="693">
         <v>2</v>
       </c>
       <c r="D33" s="306" t="s">
         <v>343</v>
       </c>
-      <c r="E33" s="601">
-        <v>3</v>
-      </c>
-      <c r="F33" s="665"/>
+      <c r="E33" s="601"/>
+      <c r="F33" s="659"/>
       <c r="G33" s="265" t="s">
         <v>332</v>
       </c>
@@ -10067,7 +10065,7 @@
       <c r="J33" s="228" t="s">
         <v>385</v>
       </c>
-      <c r="K33" s="703"/>
+      <c r="K33" s="694"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="582" t="s">
@@ -10079,10 +10077,8 @@
       <c r="D34" s="305" t="s">
         <v>343</v>
       </c>
-      <c r="E34" s="603">
-        <v>4</v>
-      </c>
-      <c r="F34" s="667"/>
+      <c r="E34" s="603"/>
+      <c r="F34" s="661"/>
       <c r="G34" s="266" t="s">
         <v>333</v>
       </c>
@@ -10103,10 +10099,8 @@
       <c r="D35" s="306" t="s">
         <v>343</v>
       </c>
-      <c r="E35" s="604">
-        <v>5</v>
-      </c>
-      <c r="F35" s="668"/>
+      <c r="E35" s="604"/>
+      <c r="F35" s="662"/>
       <c r="G35" s="267" t="s">
         <v>334</v>
       </c>
@@ -10120,7 +10114,7 @@
       <c r="C36" s="235"/>
       <c r="D36" s="304"/>
       <c r="E36" s="605"/>
-      <c r="F36" s="669"/>
+      <c r="F36" s="663"/>
       <c r="G36" s="260"/>
       <c r="H36" s="248"/>
       <c r="I36" s="220" t="s">
@@ -10136,7 +10130,7 @@
       <c r="C37" s="235"/>
       <c r="D37" s="304"/>
       <c r="E37" s="605"/>
-      <c r="F37" s="669"/>
+      <c r="F37" s="663"/>
       <c r="G37" s="260"/>
       <c r="H37" s="248"/>
       <c r="I37" s="220" t="s">
@@ -10154,7 +10148,7 @@
       <c r="C38" s="235"/>
       <c r="D38" s="304"/>
       <c r="E38" s="605"/>
-      <c r="F38" s="669"/>
+      <c r="F38" s="663"/>
       <c r="G38" s="260"/>
       <c r="H38" s="248"/>
       <c r="I38" s="220" t="s">
@@ -10170,7 +10164,7 @@
       <c r="C39" s="235"/>
       <c r="D39" s="304"/>
       <c r="E39" s="605"/>
-      <c r="F39" s="669"/>
+      <c r="F39" s="663"/>
       <c r="G39" s="260"/>
       <c r="H39" s="248"/>
       <c r="I39" s="220" t="s">
@@ -10186,7 +10180,7 @@
       <c r="C40" s="235"/>
       <c r="D40" s="304"/>
       <c r="E40" s="605"/>
-      <c r="F40" s="669"/>
+      <c r="F40" s="663"/>
       <c r="G40" s="260"/>
       <c r="H40" s="248"/>
       <c r="I40" s="220" t="s">
@@ -10202,7 +10196,7 @@
       <c r="C41" s="235"/>
       <c r="D41" s="304"/>
       <c r="E41" s="605"/>
-      <c r="F41" s="669"/>
+      <c r="F41" s="663"/>
       <c r="G41" s="260"/>
       <c r="H41" s="248"/>
       <c r="I41" s="220" t="s">
@@ -10218,7 +10212,7 @@
       <c r="C42" s="235"/>
       <c r="D42" s="304"/>
       <c r="E42" s="605"/>
-      <c r="F42" s="669"/>
+      <c r="F42" s="663"/>
       <c r="G42" s="260"/>
       <c r="H42" s="248"/>
       <c r="I42" s="220" t="s">
@@ -10234,7 +10228,7 @@
       <c r="C43" s="235"/>
       <c r="D43" s="304"/>
       <c r="E43" s="605"/>
-      <c r="F43" s="669"/>
+      <c r="F43" s="663"/>
       <c r="G43" s="260"/>
       <c r="H43" s="248"/>
       <c r="I43" s="220" t="s">
@@ -10250,7 +10244,7 @@
       <c r="C44" s="235"/>
       <c r="D44" s="304"/>
       <c r="E44" s="605"/>
-      <c r="F44" s="669"/>
+      <c r="F44" s="663"/>
       <c r="G44" s="260"/>
       <c r="H44" s="248"/>
       <c r="I44" s="220" t="s">
@@ -10266,7 +10260,7 @@
       <c r="C45" s="235"/>
       <c r="D45" s="304"/>
       <c r="E45" s="605"/>
-      <c r="F45" s="669"/>
+      <c r="F45" s="663"/>
       <c r="G45" s="260"/>
       <c r="H45" s="248"/>
       <c r="I45" s="220" t="s">
@@ -10282,7 +10276,7 @@
       <c r="C46" s="242"/>
       <c r="D46" s="307"/>
       <c r="E46" s="606"/>
-      <c r="F46" s="670"/>
+      <c r="F46" s="664"/>
       <c r="G46" s="268"/>
       <c r="H46" s="257"/>
       <c r="I46" s="227" t="s">
@@ -10301,13 +10295,9 @@
         <v>5</v>
       </c>
       <c r="D47" s="308"/>
-      <c r="E47" s="602">
-        <v>6</v>
-      </c>
-      <c r="F47" s="666"/>
-      <c r="G47" s="686" t="s">
-        <v>984</v>
-      </c>
+      <c r="E47" s="602"/>
+      <c r="F47" s="660"/>
+      <c r="G47" s="680"/>
       <c r="H47" s="254"/>
       <c r="I47" s="229"/>
       <c r="J47" s="229"/>
@@ -10322,7 +10312,7 @@
       </c>
       <c r="D48" s="304"/>
       <c r="E48" s="607"/>
-      <c r="F48" s="671"/>
+      <c r="F48" s="665"/>
       <c r="G48" s="269"/>
       <c r="H48" s="258"/>
       <c r="I48" s="231"/>
@@ -10342,7 +10332,7 @@
       <c r="E49" s="607">
         <v>7</v>
       </c>
-      <c r="F49" s="671"/>
+      <c r="F49" s="665"/>
       <c r="G49" s="269" t="s">
         <v>338</v>
       </c>
@@ -10364,7 +10354,7 @@
       <c r="E50" s="608">
         <v>8</v>
       </c>
-      <c r="F50" s="672"/>
+      <c r="F50" s="666"/>
       <c r="G50" s="270" t="s">
         <v>344</v>
       </c>
@@ -10382,7 +10372,7 @@
       </c>
       <c r="D51" s="310"/>
       <c r="E51" s="245"/>
-      <c r="F51" s="673"/>
+      <c r="F51" s="667"/>
       <c r="G51" s="269"/>
       <c r="H51" s="258"/>
       <c r="I51" s="231"/>
@@ -10398,7 +10388,7 @@
       </c>
       <c r="D52" s="310"/>
       <c r="E52" s="245"/>
-      <c r="F52" s="673"/>
+      <c r="F52" s="667"/>
       <c r="G52" s="269"/>
       <c r="H52" s="258"/>
       <c r="I52" s="231"/>
@@ -10414,7 +10404,7 @@
       </c>
       <c r="D53" s="310"/>
       <c r="E53" s="245"/>
-      <c r="F53" s="673"/>
+      <c r="F53" s="667"/>
       <c r="G53" s="269"/>
       <c r="H53" s="258"/>
       <c r="I53" s="231"/>
@@ -10430,7 +10420,7 @@
       </c>
       <c r="D54" s="310"/>
       <c r="E54" s="245"/>
-      <c r="F54" s="673"/>
+      <c r="F54" s="667"/>
       <c r="G54" s="269"/>
       <c r="H54" s="258"/>
       <c r="I54" s="231"/>
@@ -10438,13 +10428,15 @@
       <c r="K54" s="590"/>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B55" s="592"/>
+      <c r="B55" s="835" t="s">
+        <v>987</v>
+      </c>
       <c r="C55" s="244">
         <v>13</v>
       </c>
       <c r="D55" s="310"/>
       <c r="E55" s="245"/>
-      <c r="F55" s="673"/>
+      <c r="F55" s="667"/>
       <c r="G55" s="269"/>
       <c r="H55" s="258"/>
       <c r="I55" s="231"/>
@@ -10452,13 +10444,13 @@
       <c r="K55" s="590"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B56" s="592"/>
+      <c r="B56" s="836"/>
       <c r="C56" s="244">
         <v>14</v>
       </c>
       <c r="D56" s="310"/>
       <c r="E56" s="245"/>
-      <c r="F56" s="673"/>
+      <c r="F56" s="667"/>
       <c r="G56" s="269"/>
       <c r="H56" s="258"/>
       <c r="I56" s="231"/>
@@ -10472,7 +10464,7 @@
       </c>
       <c r="D57" s="310"/>
       <c r="E57" s="245"/>
-      <c r="F57" s="673"/>
+      <c r="F57" s="667"/>
       <c r="G57" s="269"/>
       <c r="H57" s="258"/>
       <c r="I57" s="231"/>
@@ -10486,7 +10478,7 @@
       </c>
       <c r="D58" s="310"/>
       <c r="E58" s="245"/>
-      <c r="F58" s="673"/>
+      <c r="F58" s="667"/>
       <c r="G58" s="269"/>
       <c r="H58" s="258"/>
       <c r="I58" s="231"/>
@@ -10502,7 +10494,7 @@
       </c>
       <c r="D59" s="310"/>
       <c r="E59" s="245"/>
-      <c r="F59" s="673"/>
+      <c r="F59" s="667"/>
       <c r="G59" s="269"/>
       <c r="H59" s="258"/>
       <c r="I59" s="231"/>
@@ -10516,7 +10508,7 @@
       </c>
       <c r="D60" s="310"/>
       <c r="E60" s="245"/>
-      <c r="F60" s="673"/>
+      <c r="F60" s="667"/>
       <c r="G60" s="269"/>
       <c r="H60" s="258"/>
       <c r="I60" s="231"/>
@@ -10530,7 +10522,7 @@
       </c>
       <c r="D61" s="310"/>
       <c r="E61" s="245"/>
-      <c r="F61" s="673"/>
+      <c r="F61" s="667"/>
       <c r="G61" s="269"/>
       <c r="H61" s="258"/>
       <c r="I61" s="231"/>
@@ -10544,7 +10536,7 @@
       </c>
       <c r="D62" s="310"/>
       <c r="E62" s="245"/>
-      <c r="F62" s="673"/>
+      <c r="F62" s="667"/>
       <c r="G62" s="269"/>
       <c r="H62" s="258"/>
       <c r="I62" s="231"/>
@@ -10560,7 +10552,7 @@
       </c>
       <c r="D63" s="310"/>
       <c r="E63" s="245"/>
-      <c r="F63" s="673"/>
+      <c r="F63" s="667"/>
       <c r="G63" s="269"/>
       <c r="H63" s="258"/>
       <c r="I63" s="231"/>
@@ -10574,7 +10566,7 @@
       </c>
       <c r="D64" s="310"/>
       <c r="E64" s="245"/>
-      <c r="F64" s="673"/>
+      <c r="F64" s="667"/>
       <c r="G64" s="269"/>
       <c r="H64" s="258"/>
       <c r="I64" s="231"/>
@@ -10590,7 +10582,7 @@
       </c>
       <c r="D65" s="310"/>
       <c r="E65" s="245"/>
-      <c r="F65" s="673"/>
+      <c r="F65" s="667"/>
       <c r="G65" s="269"/>
       <c r="H65" s="258"/>
       <c r="I65" s="231"/>
@@ -10604,7 +10596,7 @@
       </c>
       <c r="D66" s="310"/>
       <c r="E66" s="245"/>
-      <c r="F66" s="673"/>
+      <c r="F66" s="667"/>
       <c r="G66" s="269"/>
       <c r="H66" s="258"/>
       <c r="I66" s="231"/>
@@ -10620,7 +10612,7 @@
       </c>
       <c r="D67" s="310"/>
       <c r="E67" s="245"/>
-      <c r="F67" s="673"/>
+      <c r="F67" s="667"/>
       <c r="G67" s="269"/>
       <c r="H67" s="258"/>
       <c r="I67" s="231"/>
@@ -10636,7 +10628,7 @@
       </c>
       <c r="D68" s="310"/>
       <c r="E68" s="245"/>
-      <c r="F68" s="673"/>
+      <c r="F68" s="667"/>
       <c r="G68" s="269"/>
       <c r="H68" s="258"/>
       <c r="I68" s="231"/>
@@ -10650,7 +10642,7 @@
       </c>
       <c r="D69" s="310"/>
       <c r="E69" s="245"/>
-      <c r="F69" s="673"/>
+      <c r="F69" s="667"/>
       <c r="G69" s="269"/>
       <c r="H69" s="258"/>
       <c r="I69" s="231"/>
@@ -10664,7 +10656,7 @@
       <c r="E70" s="609" t="s">
         <v>342</v>
       </c>
-      <c r="F70" s="674"/>
+      <c r="F70" s="668"/>
       <c r="G70" s="555" t="s">
         <v>827</v>
       </c>
@@ -10686,7 +10678,7 @@
       <c r="E71" s="610" t="s">
         <v>819</v>
       </c>
-      <c r="F71" s="675">
+      <c r="F71" s="669">
         <v>1</v>
       </c>
       <c r="G71" s="260" t="s">
@@ -10708,7 +10700,7 @@
       <c r="E72" s="611" t="s">
         <v>820</v>
       </c>
-      <c r="F72" s="675">
+      <c r="F72" s="669">
         <v>2</v>
       </c>
       <c r="G72" s="260" t="s">
@@ -10728,7 +10720,7 @@
       <c r="E73" s="612" t="s">
         <v>821</v>
       </c>
-      <c r="F73" s="676">
+      <c r="F73" s="670">
         <v>3</v>
       </c>
       <c r="G73" s="261" t="s">
@@ -10750,7 +10742,7 @@
       <c r="E74" s="613" t="s">
         <v>822</v>
       </c>
-      <c r="F74" s="677">
+      <c r="F74" s="671">
         <v>4</v>
       </c>
       <c r="G74" s="394" t="s">
@@ -10767,14 +10759,14 @@
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B75" s="580"/>
-      <c r="C75" s="813">
+      <c r="C75" s="814">
         <v>31</v>
       </c>
       <c r="D75" s="621"/>
       <c r="E75" s="631" t="s">
         <v>845</v>
       </c>
-      <c r="F75" s="816">
+      <c r="F75" s="817">
         <v>4</v>
       </c>
       <c r="G75" s="632" t="s">
@@ -10789,12 +10781,12 @@
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B76" s="589"/>
-      <c r="C76" s="814"/>
+      <c r="C76" s="815"/>
       <c r="D76" s="39"/>
       <c r="E76" s="636" t="s">
         <v>268</v>
       </c>
-      <c r="F76" s="817"/>
+      <c r="F76" s="818"/>
       <c r="G76" s="637" t="s">
         <v>832</v>
       </c>
@@ -10807,12 +10799,12 @@
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B77" s="589"/>
-      <c r="C77" s="815"/>
+      <c r="C77" s="816"/>
       <c r="D77" s="39"/>
       <c r="E77" s="636" t="s">
         <v>268</v>
       </c>
-      <c r="F77" s="818"/>
+      <c r="F77" s="819"/>
       <c r="G77" s="637" t="s">
         <v>834</v>
       </c>
@@ -10832,7 +10824,7 @@
       <c r="E78" s="641" t="s">
         <v>823</v>
       </c>
-      <c r="F78" s="679">
+      <c r="F78" s="673">
         <v>5</v>
       </c>
       <c r="G78" s="642" t="s">
@@ -10856,7 +10848,7 @@
       <c r="E79" s="617" t="s">
         <v>829</v>
       </c>
-      <c r="F79" s="680">
+      <c r="F79" s="674">
         <v>4</v>
       </c>
       <c r="G79" s="391" t="s">
@@ -10878,7 +10870,7 @@
       <c r="E80" s="614" t="s">
         <v>823</v>
       </c>
-      <c r="F80" s="681">
+      <c r="F80" s="675">
         <v>5</v>
       </c>
       <c r="G80" s="382" t="s">
@@ -10900,7 +10892,7 @@
       <c r="E81" s="615" t="s">
         <v>824</v>
       </c>
-      <c r="F81" s="682">
+      <c r="F81" s="676">
         <v>6</v>
       </c>
       <c r="G81" s="385" t="s">
@@ -10922,7 +10914,7 @@
       <c r="E82" s="616" t="s">
         <v>825</v>
       </c>
-      <c r="F82" s="683">
+      <c r="F82" s="677">
         <v>7</v>
       </c>
       <c r="G82" s="388" t="s">
@@ -10946,7 +10938,7 @@
       <c r="E83" s="646" t="s">
         <v>822</v>
       </c>
-      <c r="F83" s="684">
+      <c r="F83" s="678">
         <v>4</v>
       </c>
       <c r="G83" s="647" t="s">
@@ -10968,7 +10960,7 @@
       <c r="E84" s="636" t="s">
         <v>823</v>
       </c>
-      <c r="F84" s="678">
+      <c r="F84" s="672">
         <v>5</v>
       </c>
       <c r="G84" s="651" t="s">
@@ -10990,7 +10982,7 @@
       <c r="E85" s="636" t="s">
         <v>824</v>
       </c>
-      <c r="F85" s="678">
+      <c r="F85" s="672">
         <v>6</v>
       </c>
       <c r="G85" s="651" t="s">
@@ -11012,7 +11004,7 @@
       <c r="E86" s="636" t="s">
         <v>825</v>
       </c>
-      <c r="F86" s="678">
+      <c r="F86" s="672">
         <v>7</v>
       </c>
       <c r="G86" s="651" t="s">
@@ -11034,7 +11026,7 @@
       <c r="E87" s="652" t="s">
         <v>826</v>
       </c>
-      <c r="F87" s="685">
+      <c r="F87" s="679">
         <v>8</v>
       </c>
       <c r="G87" s="653" t="s">
@@ -11062,11 +11054,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="K12:K13"/>
     <mergeCell ref="K18:K19"/>
     <mergeCell ref="C75:C77"/>
     <mergeCell ref="F75:F77"/>
+    <mergeCell ref="B55:B56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12556,22 +12549,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="819"/>
-      <c r="C2" s="819"/>
-      <c r="D2" s="819"/>
-      <c r="E2" s="819"/>
-      <c r="F2" s="819"/>
-      <c r="G2" s="819"/>
+      <c r="B2" s="820"/>
+      <c r="C2" s="820"/>
+      <c r="D2" s="820"/>
+      <c r="E2" s="820"/>
+      <c r="F2" s="820"/>
+      <c r="G2" s="820"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="820" t="s">
+      <c r="B3" s="821" t="s">
         <v>855</v>
       </c>
-      <c r="C3" s="821"/>
-      <c r="D3" s="821"/>
-      <c r="E3" s="821"/>
-      <c r="F3" s="821"/>
-      <c r="G3" s="822"/>
+      <c r="C3" s="822"/>
+      <c r="D3" s="822"/>
+      <c r="E3" s="822"/>
+      <c r="F3" s="822"/>
+      <c r="G3" s="823"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="398" t="s">
@@ -12630,14 +12623,14 @@
       <c r="G7" s="216"/>
     </row>
     <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="823" t="s">
+      <c r="B8" s="824" t="s">
         <v>856</v>
       </c>
-      <c r="C8" s="824"/>
-      <c r="D8" s="824"/>
-      <c r="E8" s="824"/>
-      <c r="F8" s="824"/>
-      <c r="G8" s="825"/>
+      <c r="C8" s="825"/>
+      <c r="D8" s="825"/>
+      <c r="E8" s="825"/>
+      <c r="F8" s="825"/>
+      <c r="G8" s="826"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="398" t="s">
@@ -12696,14 +12689,14 @@
       <c r="G12" s="216"/>
     </row>
     <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="823" t="s">
+      <c r="B13" s="824" t="s">
         <v>857</v>
       </c>
-      <c r="C13" s="824"/>
-      <c r="D13" s="824"/>
-      <c r="E13" s="824"/>
-      <c r="F13" s="824"/>
-      <c r="G13" s="825"/>
+      <c r="C13" s="825"/>
+      <c r="D13" s="825"/>
+      <c r="E13" s="825"/>
+      <c r="F13" s="825"/>
+      <c r="G13" s="826"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="398" t="s">
@@ -12762,14 +12755,14 @@
       <c r="G17" s="216"/>
     </row>
     <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="823" t="s">
+      <c r="B18" s="824" t="s">
         <v>858</v>
       </c>
-      <c r="C18" s="824"/>
-      <c r="D18" s="824"/>
-      <c r="E18" s="824"/>
-      <c r="F18" s="824"/>
-      <c r="G18" s="825"/>
+      <c r="C18" s="825"/>
+      <c r="D18" s="825"/>
+      <c r="E18" s="825"/>
+      <c r="F18" s="825"/>
+      <c r="G18" s="826"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="398" t="s">
@@ -12860,24 +12853,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="819" t="s">
+      <c r="B2" s="820" t="s">
         <v>868</v>
       </c>
-      <c r="C2" s="826"/>
-      <c r="D2" s="826"/>
-      <c r="E2" s="826"/>
-      <c r="F2" s="826"/>
-      <c r="G2" s="826"/>
+      <c r="C2" s="827"/>
+      <c r="D2" s="827"/>
+      <c r="E2" s="827"/>
+      <c r="F2" s="827"/>
+      <c r="G2" s="827"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="820" t="s">
+      <c r="B3" s="821" t="s">
         <v>855</v>
       </c>
-      <c r="C3" s="821"/>
-      <c r="D3" s="821"/>
-      <c r="E3" s="821"/>
-      <c r="F3" s="821"/>
-      <c r="G3" s="822"/>
+      <c r="C3" s="822"/>
+      <c r="D3" s="822"/>
+      <c r="E3" s="822"/>
+      <c r="F3" s="822"/>
+      <c r="G3" s="823"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="425" t="s">
@@ -12956,14 +12949,14 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="823" t="s">
+      <c r="B8" s="824" t="s">
         <v>856</v>
       </c>
-      <c r="C8" s="824"/>
-      <c r="D8" s="824"/>
-      <c r="E8" s="824"/>
-      <c r="F8" s="824"/>
-      <c r="G8" s="825"/>
+      <c r="C8" s="825"/>
+      <c r="D8" s="825"/>
+      <c r="E8" s="825"/>
+      <c r="F8" s="825"/>
+      <c r="G8" s="826"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="407" t="s">
@@ -13022,14 +13015,14 @@
       <c r="G12" s="424"/>
     </row>
     <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="823" t="s">
+      <c r="B13" s="824" t="s">
         <v>857</v>
       </c>
-      <c r="C13" s="824"/>
-      <c r="D13" s="824"/>
-      <c r="E13" s="824"/>
-      <c r="F13" s="824"/>
-      <c r="G13" s="825"/>
+      <c r="C13" s="825"/>
+      <c r="D13" s="825"/>
+      <c r="E13" s="825"/>
+      <c r="F13" s="825"/>
+      <c r="G13" s="826"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="407" t="s">
@@ -13088,14 +13081,14 @@
       <c r="G17" s="424"/>
     </row>
     <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="823" t="s">
+      <c r="B18" s="824" t="s">
         <v>858</v>
       </c>
-      <c r="C18" s="824"/>
-      <c r="D18" s="824"/>
-      <c r="E18" s="824"/>
-      <c r="F18" s="824"/>
-      <c r="G18" s="825"/>
+      <c r="C18" s="825"/>
+      <c r="D18" s="825"/>
+      <c r="E18" s="825"/>
+      <c r="F18" s="825"/>
+      <c r="G18" s="826"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="407" t="s">
@@ -13200,29 +13193,29 @@
       <c r="L3" s="115" t="s">
         <v>112</v>
       </c>
-      <c r="M3" s="726">
+      <c r="M3" s="718">
         <v>0</v>
       </c>
-      <c r="N3" s="748"/>
-      <c r="O3" s="726" t="s">
+      <c r="N3" s="732"/>
+      <c r="O3" s="718" t="s">
         <v>119</v>
       </c>
-      <c r="P3" s="736"/>
-      <c r="Q3" s="736"/>
-      <c r="R3" s="736"/>
-      <c r="S3" s="736"/>
-      <c r="T3" s="737"/>
-      <c r="U3" s="709">
+      <c r="P3" s="719"/>
+      <c r="Q3" s="719"/>
+      <c r="R3" s="719"/>
+      <c r="S3" s="719"/>
+      <c r="T3" s="720"/>
+      <c r="U3" s="730">
         <v>2</v>
       </c>
-      <c r="V3" s="709">
+      <c r="V3" s="730">
         <v>3</v>
       </c>
-      <c r="W3" s="726">
+      <c r="W3" s="718">
         <v>4</v>
       </c>
-      <c r="X3" s="727"/>
-      <c r="Y3" s="709">
+      <c r="X3" s="765"/>
+      <c r="Y3" s="730">
         <v>5</v>
       </c>
     </row>
@@ -13250,22 +13243,22 @@
       <c r="T4" s="142" t="s">
         <v>88</v>
       </c>
-      <c r="U4" s="747"/>
-      <c r="V4" s="747"/>
-      <c r="W4" s="728" t="s">
+      <c r="U4" s="731"/>
+      <c r="V4" s="731"/>
+      <c r="W4" s="766" t="s">
         <v>323</v>
       </c>
-      <c r="X4" s="729"/>
-      <c r="Y4" s="710"/>
+      <c r="X4" s="767"/>
+      <c r="Y4" s="749"/>
     </row>
     <row r="5" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L5" s="765" t="s">
+      <c r="L5" s="710" t="s">
         <v>111</v>
       </c>
-      <c r="M5" s="733" t="s">
+      <c r="M5" s="715" t="s">
         <v>113</v>
       </c>
-      <c r="N5" s="749" t="s">
+      <c r="N5" s="733" t="s">
         <v>327</v>
       </c>
       <c r="O5" s="61"/>
@@ -13278,26 +13271,26 @@
       <c r="T5" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="U5" s="741" t="s">
+      <c r="U5" s="724" t="s">
         <v>475</v>
       </c>
-      <c r="V5" s="744" t="s">
+      <c r="V5" s="727" t="s">
         <v>326</v>
       </c>
-      <c r="W5" s="720" t="s">
+      <c r="W5" s="759" t="s">
         <v>314</v>
       </c>
-      <c r="X5" s="724" t="s">
+      <c r="X5" s="763" t="s">
         <v>315</v>
       </c>
-      <c r="Y5" s="711" t="s">
+      <c r="Y5" s="750" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="6" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L6" s="766"/>
-      <c r="M6" s="734"/>
-      <c r="N6" s="750"/>
+      <c r="L6" s="711"/>
+      <c r="M6" s="716"/>
+      <c r="N6" s="734"/>
       <c r="O6" s="64"/>
       <c r="P6" s="65"/>
       <c r="Q6" s="65"/>
@@ -13306,16 +13299,16 @@
       <c r="T6" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U6" s="742"/>
-      <c r="V6" s="745"/>
-      <c r="W6" s="721"/>
-      <c r="X6" s="725"/>
-      <c r="Y6" s="712"/>
+      <c r="U6" s="725"/>
+      <c r="V6" s="728"/>
+      <c r="W6" s="760"/>
+      <c r="X6" s="764"/>
+      <c r="Y6" s="751"/>
     </row>
     <row r="7" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L7" s="766"/>
-      <c r="M7" s="734"/>
-      <c r="N7" s="751"/>
+      <c r="L7" s="711"/>
+      <c r="M7" s="716"/>
+      <c r="N7" s="735"/>
       <c r="O7" s="64"/>
       <c r="P7" s="65"/>
       <c r="Q7" s="65"/>
@@ -13324,18 +13317,18 @@
       <c r="T7" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U7" s="742"/>
-      <c r="V7" s="745"/>
-      <c r="W7" s="722"/>
-      <c r="X7" s="730" t="s">
+      <c r="U7" s="725"/>
+      <c r="V7" s="728"/>
+      <c r="W7" s="761"/>
+      <c r="X7" s="768" t="s">
         <v>320</v>
       </c>
-      <c r="Y7" s="712"/>
+      <c r="Y7" s="751"/>
     </row>
     <row r="8" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L8" s="767"/>
-      <c r="M8" s="734"/>
-      <c r="N8" s="754" t="s">
+      <c r="L8" s="712"/>
+      <c r="M8" s="716"/>
+      <c r="N8" s="738" t="s">
         <v>312</v>
       </c>
       <c r="O8" s="108"/>
@@ -13348,18 +13341,18 @@
       <c r="T8" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U8" s="742"/>
-      <c r="V8" s="745"/>
-      <c r="W8" s="722"/>
-      <c r="X8" s="731"/>
-      <c r="Y8" s="712"/>
+      <c r="U8" s="725"/>
+      <c r="V8" s="728"/>
+      <c r="W8" s="761"/>
+      <c r="X8" s="769"/>
+      <c r="Y8" s="751"/>
     </row>
     <row r="9" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L9" s="765" t="s">
+      <c r="L9" s="710" t="s">
         <v>110</v>
       </c>
-      <c r="M9" s="734"/>
-      <c r="N9" s="755"/>
+      <c r="M9" s="716"/>
+      <c r="N9" s="739"/>
       <c r="O9" s="61"/>
       <c r="P9" s="62"/>
       <c r="Q9" s="62"/>
@@ -13370,18 +13363,18 @@
       <c r="T9" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U9" s="742"/>
-      <c r="V9" s="745"/>
-      <c r="W9" s="722"/>
-      <c r="X9" s="725" t="s">
+      <c r="U9" s="725"/>
+      <c r="V9" s="728"/>
+      <c r="W9" s="761"/>
+      <c r="X9" s="764" t="s">
         <v>319</v>
       </c>
-      <c r="Y9" s="712"/>
+      <c r="Y9" s="751"/>
     </row>
     <row r="10" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L10" s="766"/>
-      <c r="M10" s="734"/>
-      <c r="N10" s="755"/>
+      <c r="L10" s="711"/>
+      <c r="M10" s="716"/>
+      <c r="N10" s="739"/>
       <c r="O10" s="64"/>
       <c r="P10" s="65"/>
       <c r="Q10" s="65"/>
@@ -13390,16 +13383,16 @@
       <c r="T10" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U10" s="742"/>
-      <c r="V10" s="745"/>
-      <c r="W10" s="722"/>
-      <c r="X10" s="732"/>
-      <c r="Y10" s="712"/>
+      <c r="U10" s="725"/>
+      <c r="V10" s="728"/>
+      <c r="W10" s="761"/>
+      <c r="X10" s="770"/>
+      <c r="Y10" s="751"/>
     </row>
     <row r="11" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L11" s="766"/>
-      <c r="M11" s="734"/>
-      <c r="N11" s="756"/>
+      <c r="L11" s="711"/>
+      <c r="M11" s="716"/>
+      <c r="N11" s="740"/>
       <c r="O11" s="64"/>
       <c r="P11" s="65"/>
       <c r="Q11" s="65"/>
@@ -13408,18 +13401,18 @@
       <c r="T11" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U11" s="742"/>
-      <c r="V11" s="745"/>
-      <c r="W11" s="722"/>
-      <c r="X11" s="730" t="s">
+      <c r="U11" s="725"/>
+      <c r="V11" s="728"/>
+      <c r="W11" s="761"/>
+      <c r="X11" s="768" t="s">
         <v>318</v>
       </c>
-      <c r="Y11" s="712"/>
+      <c r="Y11" s="751"/>
     </row>
     <row r="12" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L12" s="767"/>
-      <c r="M12" s="734"/>
-      <c r="N12" s="752" t="s">
+      <c r="L12" s="712"/>
+      <c r="M12" s="716"/>
+      <c r="N12" s="736" t="s">
         <v>311</v>
       </c>
       <c r="O12" s="80"/>
@@ -13432,19 +13425,19 @@
       <c r="T12" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U12" s="742"/>
-      <c r="V12" s="745"/>
-      <c r="W12" s="722"/>
-      <c r="X12" s="731"/>
-      <c r="Y12" s="712"/>
+      <c r="U12" s="725"/>
+      <c r="V12" s="728"/>
+      <c r="W12" s="761"/>
+      <c r="X12" s="769"/>
+      <c r="Y12" s="751"/>
       <c r="Z12" s="203"/>
     </row>
     <row r="13" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L13" s="765" t="s">
+      <c r="L13" s="710" t="s">
         <v>109</v>
       </c>
-      <c r="M13" s="734"/>
-      <c r="N13" s="753"/>
+      <c r="M13" s="716"/>
+      <c r="N13" s="737"/>
       <c r="O13" s="106"/>
       <c r="P13" s="107"/>
       <c r="Q13" s="107"/>
@@ -13455,18 +13448,18 @@
       <c r="T13" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U13" s="742"/>
-      <c r="V13" s="745"/>
-      <c r="W13" s="722"/>
-      <c r="X13" s="725" t="s">
+      <c r="U13" s="725"/>
+      <c r="V13" s="728"/>
+      <c r="W13" s="761"/>
+      <c r="X13" s="764" t="s">
         <v>317</v>
       </c>
-      <c r="Y13" s="712"/>
+      <c r="Y13" s="751"/>
       <c r="Z13" s="204"/>
     </row>
     <row r="14" spans="12:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L14" s="766"/>
-      <c r="M14" s="734"/>
+      <c r="L14" s="711"/>
+      <c r="M14" s="716"/>
       <c r="N14" s="208"/>
       <c r="O14" s="64"/>
       <c r="P14" s="65"/>
@@ -13476,16 +13469,16 @@
       <c r="T14" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U14" s="742"/>
-      <c r="V14" s="745"/>
-      <c r="W14" s="722"/>
-      <c r="X14" s="732"/>
-      <c r="Y14" s="712"/>
+      <c r="U14" s="725"/>
+      <c r="V14" s="728"/>
+      <c r="W14" s="761"/>
+      <c r="X14" s="770"/>
+      <c r="Y14" s="751"/>
       <c r="Z14" s="204"/>
     </row>
     <row r="15" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L15" s="766"/>
-      <c r="M15" s="734"/>
+      <c r="L15" s="711"/>
+      <c r="M15" s="716"/>
       <c r="N15" s="209"/>
       <c r="O15" s="64"/>
       <c r="P15" s="65"/>
@@ -13495,18 +13488,18 @@
       <c r="T15" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U15" s="742"/>
-      <c r="V15" s="745"/>
-      <c r="W15" s="722"/>
-      <c r="X15" s="730" t="s">
+      <c r="U15" s="725"/>
+      <c r="V15" s="728"/>
+      <c r="W15" s="761"/>
+      <c r="X15" s="768" t="s">
         <v>316</v>
       </c>
-      <c r="Y15" s="712"/>
+      <c r="Y15" s="751"/>
       <c r="Z15" s="204"/>
     </row>
     <row r="16" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L16" s="767"/>
-      <c r="M16" s="734"/>
+      <c r="L16" s="712"/>
+      <c r="M16" s="716"/>
       <c r="N16" s="209"/>
       <c r="O16" s="108"/>
       <c r="P16" s="109"/>
@@ -13518,18 +13511,18 @@
       <c r="T16" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U16" s="742"/>
-      <c r="V16" s="745"/>
-      <c r="W16" s="723"/>
-      <c r="X16" s="731"/>
-      <c r="Y16" s="712"/>
+      <c r="U16" s="725"/>
+      <c r="V16" s="728"/>
+      <c r="W16" s="762"/>
+      <c r="X16" s="769"/>
+      <c r="Y16" s="751"/>
       <c r="Z16" s="204"/>
     </row>
     <row r="17" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="L17" s="765" t="s">
+      <c r="L17" s="710" t="s">
         <v>108</v>
       </c>
-      <c r="M17" s="734"/>
+      <c r="M17" s="716"/>
       <c r="N17" s="209"/>
       <c r="O17" s="61"/>
       <c r="P17" s="62"/>
@@ -13541,18 +13534,18 @@
       <c r="T17" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U17" s="742"/>
-      <c r="V17" s="745"/>
-      <c r="W17" s="714" t="s">
+      <c r="U17" s="725"/>
+      <c r="V17" s="728"/>
+      <c r="W17" s="753" t="s">
         <v>321</v>
       </c>
-      <c r="X17" s="715"/>
-      <c r="Y17" s="712"/>
+      <c r="X17" s="754"/>
+      <c r="Y17" s="751"/>
       <c r="Z17" s="204"/>
     </row>
     <row r="18" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="L18" s="766"/>
-      <c r="M18" s="734"/>
+      <c r="L18" s="711"/>
+      <c r="M18" s="716"/>
       <c r="N18" s="209"/>
       <c r="O18" s="64"/>
       <c r="P18" s="65"/>
@@ -13562,16 +13555,16 @@
       <c r="T18" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U18" s="742"/>
-      <c r="V18" s="745"/>
-      <c r="W18" s="716"/>
-      <c r="X18" s="717"/>
-      <c r="Y18" s="712"/>
+      <c r="U18" s="725"/>
+      <c r="V18" s="728"/>
+      <c r="W18" s="755"/>
+      <c r="X18" s="756"/>
+      <c r="Y18" s="751"/>
       <c r="Z18" s="204"/>
     </row>
     <row r="19" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="L19" s="766"/>
-      <c r="M19" s="734"/>
+      <c r="L19" s="711"/>
+      <c r="M19" s="716"/>
       <c r="N19" s="209"/>
       <c r="O19" s="64"/>
       <c r="P19" s="65"/>
@@ -13581,16 +13574,16 @@
       <c r="T19" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U19" s="742"/>
-      <c r="V19" s="745"/>
-      <c r="W19" s="716"/>
-      <c r="X19" s="717"/>
-      <c r="Y19" s="712"/>
+      <c r="U19" s="725"/>
+      <c r="V19" s="728"/>
+      <c r="W19" s="755"/>
+      <c r="X19" s="756"/>
+      <c r="Y19" s="751"/>
       <c r="Z19" s="204"/>
     </row>
     <row r="20" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="L20" s="767"/>
-      <c r="M20" s="734"/>
+      <c r="L20" s="712"/>
+      <c r="M20" s="716"/>
       <c r="N20" s="209"/>
       <c r="O20" s="80" t="s">
         <v>73</v>
@@ -13606,18 +13599,18 @@
       <c r="T20" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="U20" s="742"/>
-      <c r="V20" s="745"/>
-      <c r="W20" s="716"/>
-      <c r="X20" s="717"/>
-      <c r="Y20" s="712"/>
+      <c r="U20" s="725"/>
+      <c r="V20" s="728"/>
+      <c r="W20" s="755"/>
+      <c r="X20" s="756"/>
+      <c r="Y20" s="751"/>
       <c r="Z20" s="204"/>
     </row>
     <row r="21" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L21" s="765" t="s">
+      <c r="L21" s="710" t="s">
         <v>107</v>
       </c>
-      <c r="M21" s="734"/>
+      <c r="M21" s="716"/>
       <c r="N21" s="209"/>
       <c r="O21" s="78"/>
       <c r="P21" s="79"/>
@@ -13629,11 +13622,11 @@
       <c r="T21" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="U21" s="742"/>
-      <c r="V21" s="745"/>
-      <c r="W21" s="716"/>
-      <c r="X21" s="717"/>
-      <c r="Y21" s="712"/>
+      <c r="U21" s="725"/>
+      <c r="V21" s="728"/>
+      <c r="W21" s="755"/>
+      <c r="X21" s="756"/>
+      <c r="Y21" s="751"/>
       <c r="Z21" s="204"/>
     </row>
     <row r="22" spans="2:26" x14ac:dyDescent="0.25">
@@ -13660,8 +13653,8 @@
         <v>7759</v>
       </c>
       <c r="J22" s="206"/>
-      <c r="L22" s="766"/>
-      <c r="M22" s="734"/>
+      <c r="L22" s="711"/>
+      <c r="M22" s="716"/>
       <c r="N22" s="209"/>
       <c r="O22" s="64"/>
       <c r="P22" s="65"/>
@@ -13671,19 +13664,19 @@
       <c r="T22" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U22" s="742"/>
-      <c r="V22" s="745"/>
-      <c r="W22" s="716"/>
-      <c r="X22" s="717"/>
-      <c r="Y22" s="712"/>
+      <c r="U22" s="725"/>
+      <c r="V22" s="728"/>
+      <c r="W22" s="755"/>
+      <c r="X22" s="756"/>
+      <c r="Y22" s="751"/>
     </row>
     <row r="23" spans="2:26" x14ac:dyDescent="0.25">
       <c r="D23" s="174" t="s">
         <v>60</v>
       </c>
       <c r="J23" s="207"/>
-      <c r="L23" s="766"/>
-      <c r="M23" s="734"/>
+      <c r="L23" s="711"/>
+      <c r="M23" s="716"/>
       <c r="N23" s="209"/>
       <c r="O23" s="80"/>
       <c r="P23" s="81"/>
@@ -13693,11 +13686,11 @@
       <c r="T23" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U23" s="742"/>
-      <c r="V23" s="745"/>
-      <c r="W23" s="716"/>
-      <c r="X23" s="717"/>
-      <c r="Y23" s="712"/>
+      <c r="U23" s="725"/>
+      <c r="V23" s="728"/>
+      <c r="W23" s="755"/>
+      <c r="X23" s="756"/>
+      <c r="Y23" s="751"/>
     </row>
     <row r="24" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B24" s="189" t="s">
@@ -13723,8 +13716,8 @@
         <v>305</v>
       </c>
       <c r="J24" s="199"/>
-      <c r="L24" s="767"/>
-      <c r="M24" s="734"/>
+      <c r="L24" s="712"/>
+      <c r="M24" s="716"/>
       <c r="N24" s="209"/>
       <c r="O24" s="108"/>
       <c r="P24" s="109"/>
@@ -13736,11 +13729,11 @@
       <c r="T24" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U24" s="742"/>
-      <c r="V24" s="745"/>
-      <c r="W24" s="716"/>
-      <c r="X24" s="717"/>
-      <c r="Y24" s="712"/>
+      <c r="U24" s="725"/>
+      <c r="V24" s="728"/>
+      <c r="W24" s="755"/>
+      <c r="X24" s="756"/>
+      <c r="Y24" s="751"/>
     </row>
     <row r="25" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B25" s="186" t="s">
@@ -13766,10 +13759,10 @@
         <v>30</v>
       </c>
       <c r="J25" s="294"/>
-      <c r="L25" s="765" t="s">
+      <c r="L25" s="710" t="s">
         <v>106</v>
       </c>
-      <c r="M25" s="734"/>
+      <c r="M25" s="716"/>
       <c r="N25" s="209"/>
       <c r="O25" s="61"/>
       <c r="P25" s="62"/>
@@ -13781,16 +13774,16 @@
       <c r="T25" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U25" s="742"/>
-      <c r="V25" s="745"/>
-      <c r="W25" s="716"/>
-      <c r="X25" s="717"/>
-      <c r="Y25" s="712"/>
+      <c r="U25" s="725"/>
+      <c r="V25" s="728"/>
+      <c r="W25" s="755"/>
+      <c r="X25" s="756"/>
+      <c r="Y25" s="751"/>
     </row>
     <row r="26" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="L26" s="766"/>
-      <c r="M26" s="734"/>
-      <c r="N26" s="762" t="s">
+      <c r="L26" s="711"/>
+      <c r="M26" s="716"/>
+      <c r="N26" s="746" t="s">
         <v>330</v>
       </c>
       <c r="O26" s="64"/>
@@ -13801,17 +13794,17 @@
       <c r="T26" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U26" s="742"/>
-      <c r="V26" s="745"/>
-      <c r="W26" s="716"/>
-      <c r="X26" s="717"/>
-      <c r="Y26" s="712"/>
+      <c r="U26" s="725"/>
+      <c r="V26" s="728"/>
+      <c r="W26" s="755"/>
+      <c r="X26" s="756"/>
+      <c r="Y26" s="751"/>
     </row>
     <row r="27" spans="2:26" x14ac:dyDescent="0.25">
       <c r="H27" s="199"/>
-      <c r="L27" s="766"/>
-      <c r="M27" s="734"/>
-      <c r="N27" s="763"/>
+      <c r="L27" s="711"/>
+      <c r="M27" s="716"/>
+      <c r="N27" s="747"/>
       <c r="O27" s="80"/>
       <c r="P27" s="81"/>
       <c r="Q27" s="81"/>
@@ -13820,17 +13813,17 @@
       <c r="T27" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U27" s="742"/>
-      <c r="V27" s="745"/>
-      <c r="W27" s="716"/>
-      <c r="X27" s="717"/>
-      <c r="Y27" s="712"/>
+      <c r="U27" s="725"/>
+      <c r="V27" s="728"/>
+      <c r="W27" s="755"/>
+      <c r="X27" s="756"/>
+      <c r="Y27" s="751"/>
     </row>
     <row r="28" spans="2:26" x14ac:dyDescent="0.25">
       <c r="H28" s="199"/>
-      <c r="L28" s="767"/>
-      <c r="M28" s="734"/>
-      <c r="N28" s="763"/>
+      <c r="L28" s="712"/>
+      <c r="M28" s="716"/>
+      <c r="N28" s="747"/>
       <c r="O28" s="80"/>
       <c r="P28" s="81"/>
       <c r="Q28" s="82" t="s">
@@ -13841,19 +13834,19 @@
       <c r="T28" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U28" s="742"/>
-      <c r="V28" s="745"/>
-      <c r="W28" s="716"/>
-      <c r="X28" s="717"/>
-      <c r="Y28" s="712"/>
+      <c r="U28" s="725"/>
+      <c r="V28" s="728"/>
+      <c r="W28" s="755"/>
+      <c r="X28" s="756"/>
+      <c r="Y28" s="751"/>
     </row>
     <row r="29" spans="2:26" x14ac:dyDescent="0.25">
       <c r="H29" s="144"/>
-      <c r="L29" s="765" t="s">
+      <c r="L29" s="710" t="s">
         <v>105</v>
       </c>
-      <c r="M29" s="734"/>
-      <c r="N29" s="763"/>
+      <c r="M29" s="716"/>
+      <c r="N29" s="747"/>
       <c r="O29" s="106"/>
       <c r="P29" s="107"/>
       <c r="Q29" s="107"/>
@@ -13864,16 +13857,16 @@
       <c r="T29" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U29" s="742"/>
-      <c r="V29" s="745"/>
-      <c r="W29" s="716"/>
-      <c r="X29" s="717"/>
-      <c r="Y29" s="712"/>
+      <c r="U29" s="725"/>
+      <c r="V29" s="728"/>
+      <c r="W29" s="755"/>
+      <c r="X29" s="756"/>
+      <c r="Y29" s="751"/>
     </row>
     <row r="30" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="L30" s="766"/>
-      <c r="M30" s="734"/>
-      <c r="N30" s="764"/>
+      <c r="L30" s="711"/>
+      <c r="M30" s="716"/>
+      <c r="N30" s="748"/>
       <c r="O30" s="64"/>
       <c r="P30" s="65"/>
       <c r="Q30" s="65"/>
@@ -13882,16 +13875,16 @@
       <c r="T30" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U30" s="742"/>
-      <c r="V30" s="745"/>
-      <c r="W30" s="716"/>
-      <c r="X30" s="717"/>
-      <c r="Y30" s="712"/>
+      <c r="U30" s="725"/>
+      <c r="V30" s="728"/>
+      <c r="W30" s="755"/>
+      <c r="X30" s="756"/>
+      <c r="Y30" s="751"/>
     </row>
     <row r="31" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="L31" s="766"/>
-      <c r="M31" s="734"/>
-      <c r="N31" s="761" t="s">
+      <c r="L31" s="711"/>
+      <c r="M31" s="716"/>
+      <c r="N31" s="745" t="s">
         <v>329</v>
       </c>
       <c r="O31" s="64"/>
@@ -13902,16 +13895,16 @@
       <c r="T31" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U31" s="742"/>
-      <c r="V31" s="745"/>
-      <c r="W31" s="716"/>
-      <c r="X31" s="717"/>
-      <c r="Y31" s="712"/>
+      <c r="U31" s="725"/>
+      <c r="V31" s="728"/>
+      <c r="W31" s="755"/>
+      <c r="X31" s="756"/>
+      <c r="Y31" s="751"/>
     </row>
     <row r="32" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="L32" s="767"/>
-      <c r="M32" s="734"/>
-      <c r="N32" s="755"/>
+      <c r="L32" s="712"/>
+      <c r="M32" s="716"/>
+      <c r="N32" s="739"/>
       <c r="O32" s="110"/>
       <c r="P32" s="111"/>
       <c r="Q32" s="112" t="s">
@@ -13922,18 +13915,18 @@
       <c r="T32" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U32" s="742"/>
-      <c r="V32" s="745"/>
-      <c r="W32" s="716"/>
-      <c r="X32" s="717"/>
-      <c r="Y32" s="712"/>
+      <c r="U32" s="725"/>
+      <c r="V32" s="728"/>
+      <c r="W32" s="755"/>
+      <c r="X32" s="756"/>
+      <c r="Y32" s="751"/>
     </row>
     <row r="33" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L33" s="765" t="s">
+      <c r="L33" s="710" t="s">
         <v>104</v>
       </c>
-      <c r="M33" s="734"/>
-      <c r="N33" s="755"/>
+      <c r="M33" s="716"/>
+      <c r="N33" s="739"/>
       <c r="O33" s="61"/>
       <c r="P33" s="62"/>
       <c r="Q33" s="62"/>
@@ -13944,17 +13937,17 @@
       <c r="T33" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U33" s="742"/>
-      <c r="V33" s="745"/>
-      <c r="W33" s="716"/>
-      <c r="X33" s="717"/>
-      <c r="Y33" s="712"/>
+      <c r="U33" s="725"/>
+      <c r="V33" s="728"/>
+      <c r="W33" s="755"/>
+      <c r="X33" s="756"/>
+      <c r="Y33" s="751"/>
       <c r="Z33" s="205"/>
     </row>
     <row r="34" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L34" s="766"/>
-      <c r="M34" s="734"/>
-      <c r="N34" s="756"/>
+      <c r="L34" s="711"/>
+      <c r="M34" s="716"/>
+      <c r="N34" s="740"/>
       <c r="O34" s="64"/>
       <c r="P34" s="65"/>
       <c r="Q34" s="65"/>
@@ -13963,17 +13956,17 @@
       <c r="T34" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U34" s="742"/>
-      <c r="V34" s="745"/>
-      <c r="W34" s="716"/>
-      <c r="X34" s="717"/>
-      <c r="Y34" s="712"/>
+      <c r="U34" s="725"/>
+      <c r="V34" s="728"/>
+      <c r="W34" s="755"/>
+      <c r="X34" s="756"/>
+      <c r="Y34" s="751"/>
       <c r="Z34" s="205"/>
     </row>
     <row r="35" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L35" s="766"/>
-      <c r="M35" s="734"/>
-      <c r="N35" s="760" t="s">
+      <c r="L35" s="711"/>
+      <c r="M35" s="716"/>
+      <c r="N35" s="744" t="s">
         <v>328</v>
       </c>
       <c r="O35" s="64"/>
@@ -13984,17 +13977,17 @@
       <c r="T35" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U35" s="742"/>
-      <c r="V35" s="745"/>
-      <c r="W35" s="716"/>
-      <c r="X35" s="717"/>
-      <c r="Y35" s="712"/>
+      <c r="U35" s="725"/>
+      <c r="V35" s="728"/>
+      <c r="W35" s="755"/>
+      <c r="X35" s="756"/>
+      <c r="Y35" s="751"/>
       <c r="Z35" s="203"/>
     </row>
     <row r="36" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L36" s="767"/>
-      <c r="M36" s="734"/>
-      <c r="N36" s="753"/>
+      <c r="L36" s="712"/>
+      <c r="M36" s="716"/>
+      <c r="N36" s="737"/>
       <c r="O36" s="67" t="s">
         <v>73</v>
       </c>
@@ -14009,19 +14002,19 @@
       <c r="T36" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="U36" s="742"/>
-      <c r="V36" s="745"/>
-      <c r="W36" s="716"/>
-      <c r="X36" s="717"/>
-      <c r="Y36" s="712"/>
+      <c r="U36" s="725"/>
+      <c r="V36" s="728"/>
+      <c r="W36" s="755"/>
+      <c r="X36" s="756"/>
+      <c r="Y36" s="751"/>
       <c r="Z36" s="204"/>
     </row>
     <row r="37" spans="12:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L37" s="765" t="s">
+      <c r="L37" s="710" t="s">
         <v>103</v>
       </c>
-      <c r="M37" s="734"/>
-      <c r="N37" s="757" t="s">
+      <c r="M37" s="716"/>
+      <c r="N37" s="741" t="s">
         <v>313</v>
       </c>
       <c r="O37" s="70"/>
@@ -14038,17 +14031,17 @@
       <c r="T37" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="U37" s="742"/>
-      <c r="V37" s="745"/>
-      <c r="W37" s="716"/>
-      <c r="X37" s="717"/>
-      <c r="Y37" s="712"/>
+      <c r="U37" s="725"/>
+      <c r="V37" s="728"/>
+      <c r="W37" s="755"/>
+      <c r="X37" s="756"/>
+      <c r="Y37" s="751"/>
       <c r="Z37" s="204"/>
     </row>
     <row r="38" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L38" s="766"/>
-      <c r="M38" s="734"/>
-      <c r="N38" s="758"/>
+      <c r="L38" s="711"/>
+      <c r="M38" s="716"/>
+      <c r="N38" s="742"/>
       <c r="O38" s="72"/>
       <c r="P38" s="73"/>
       <c r="Q38" s="74" t="s">
@@ -14061,17 +14054,17 @@
       <c r="T38" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U38" s="742"/>
-      <c r="V38" s="745"/>
-      <c r="W38" s="716"/>
-      <c r="X38" s="717"/>
-      <c r="Y38" s="712"/>
+      <c r="U38" s="725"/>
+      <c r="V38" s="728"/>
+      <c r="W38" s="755"/>
+      <c r="X38" s="756"/>
+      <c r="Y38" s="751"/>
       <c r="Z38" s="204"/>
     </row>
     <row r="39" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L39" s="766"/>
-      <c r="M39" s="734"/>
-      <c r="N39" s="758"/>
+      <c r="L39" s="711"/>
+      <c r="M39" s="716"/>
+      <c r="N39" s="742"/>
       <c r="O39" s="72"/>
       <c r="P39" s="73"/>
       <c r="Q39" s="74" t="s">
@@ -14084,17 +14077,17 @@
       <c r="T39" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U39" s="742"/>
-      <c r="V39" s="745"/>
-      <c r="W39" s="716"/>
-      <c r="X39" s="717"/>
-      <c r="Y39" s="712"/>
+      <c r="U39" s="725"/>
+      <c r="V39" s="728"/>
+      <c r="W39" s="755"/>
+      <c r="X39" s="756"/>
+      <c r="Y39" s="751"/>
       <c r="Z39" s="205"/>
     </row>
     <row r="40" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L40" s="767"/>
-      <c r="M40" s="734"/>
-      <c r="N40" s="758"/>
+      <c r="L40" s="712"/>
+      <c r="M40" s="716"/>
+      <c r="N40" s="742"/>
       <c r="O40" s="96"/>
       <c r="P40" s="97"/>
       <c r="Q40" s="170" t="s">
@@ -14109,19 +14102,19 @@
       <c r="T40" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U40" s="742"/>
-      <c r="V40" s="745"/>
-      <c r="W40" s="716"/>
-      <c r="X40" s="717"/>
-      <c r="Y40" s="712"/>
+      <c r="U40" s="725"/>
+      <c r="V40" s="728"/>
+      <c r="W40" s="755"/>
+      <c r="X40" s="756"/>
+      <c r="Y40" s="751"/>
       <c r="Z40" s="203"/>
     </row>
     <row r="41" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L41" s="765" t="s">
+      <c r="L41" s="710" t="s">
         <v>102</v>
       </c>
-      <c r="M41" s="734"/>
-      <c r="N41" s="758"/>
+      <c r="M41" s="716"/>
+      <c r="N41" s="742"/>
       <c r="O41" s="101"/>
       <c r="P41" s="102"/>
       <c r="Q41" s="103" t="s">
@@ -14136,17 +14129,17 @@
       <c r="T41" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U41" s="742"/>
-      <c r="V41" s="745"/>
-      <c r="W41" s="716"/>
-      <c r="X41" s="717"/>
-      <c r="Y41" s="712"/>
+      <c r="U41" s="725"/>
+      <c r="V41" s="728"/>
+      <c r="W41" s="755"/>
+      <c r="X41" s="756"/>
+      <c r="Y41" s="751"/>
       <c r="Z41" s="204"/>
     </row>
     <row r="42" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L42" s="766"/>
-      <c r="M42" s="734"/>
-      <c r="N42" s="758"/>
+      <c r="L42" s="711"/>
+      <c r="M42" s="716"/>
+      <c r="N42" s="742"/>
       <c r="O42" s="72"/>
       <c r="P42" s="73"/>
       <c r="Q42" s="74" t="s">
@@ -14159,17 +14152,17 @@
       <c r="T42" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U42" s="742"/>
-      <c r="V42" s="745"/>
-      <c r="W42" s="716"/>
-      <c r="X42" s="717"/>
-      <c r="Y42" s="712"/>
+      <c r="U42" s="725"/>
+      <c r="V42" s="728"/>
+      <c r="W42" s="755"/>
+      <c r="X42" s="756"/>
+      <c r="Y42" s="751"/>
       <c r="Z42" s="205"/>
     </row>
     <row r="43" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L43" s="766"/>
-      <c r="M43" s="734"/>
-      <c r="N43" s="758"/>
+      <c r="L43" s="711"/>
+      <c r="M43" s="716"/>
+      <c r="N43" s="742"/>
       <c r="O43" s="96"/>
       <c r="P43" s="97"/>
       <c r="Q43" s="170" t="s">
@@ -14182,17 +14175,17 @@
       <c r="T43" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U43" s="742"/>
-      <c r="V43" s="745"/>
-      <c r="W43" s="716"/>
-      <c r="X43" s="717"/>
-      <c r="Y43" s="712"/>
+      <c r="U43" s="725"/>
+      <c r="V43" s="728"/>
+      <c r="W43" s="755"/>
+      <c r="X43" s="756"/>
+      <c r="Y43" s="751"/>
       <c r="Z43" s="205"/>
     </row>
     <row r="44" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L44" s="767"/>
-      <c r="M44" s="734"/>
-      <c r="N44" s="758"/>
+      <c r="L44" s="712"/>
+      <c r="M44" s="716"/>
+      <c r="N44" s="742"/>
       <c r="O44" s="104"/>
       <c r="P44" s="105"/>
       <c r="Q44" s="171" t="s">
@@ -14205,19 +14198,19 @@
       <c r="T44" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U44" s="742"/>
-      <c r="V44" s="745"/>
-      <c r="W44" s="716"/>
-      <c r="X44" s="717"/>
-      <c r="Y44" s="712"/>
+      <c r="U44" s="725"/>
+      <c r="V44" s="728"/>
+      <c r="W44" s="755"/>
+      <c r="X44" s="756"/>
+      <c r="Y44" s="751"/>
       <c r="Z44" s="205"/>
     </row>
     <row r="45" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L45" s="765" t="s">
+      <c r="L45" s="710" t="s">
         <v>101</v>
       </c>
-      <c r="M45" s="734"/>
-      <c r="N45" s="758"/>
+      <c r="M45" s="716"/>
+      <c r="N45" s="742"/>
       <c r="O45" s="98"/>
       <c r="P45" s="99"/>
       <c r="Q45" s="100" t="s">
@@ -14230,16 +14223,16 @@
       <c r="T45" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U45" s="742"/>
-      <c r="V45" s="745"/>
-      <c r="W45" s="716"/>
-      <c r="X45" s="717"/>
-      <c r="Y45" s="712"/>
+      <c r="U45" s="725"/>
+      <c r="V45" s="728"/>
+      <c r="W45" s="755"/>
+      <c r="X45" s="756"/>
+      <c r="Y45" s="751"/>
     </row>
     <row r="46" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L46" s="768"/>
-      <c r="M46" s="734"/>
-      <c r="N46" s="758"/>
+      <c r="L46" s="713"/>
+      <c r="M46" s="716"/>
+      <c r="N46" s="742"/>
       <c r="O46" s="72"/>
       <c r="P46" s="73"/>
       <c r="Q46" s="74" t="s">
@@ -14252,16 +14245,16 @@
       <c r="T46" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U46" s="742"/>
-      <c r="V46" s="745"/>
-      <c r="W46" s="716"/>
-      <c r="X46" s="717"/>
-      <c r="Y46" s="712"/>
+      <c r="U46" s="725"/>
+      <c r="V46" s="728"/>
+      <c r="W46" s="755"/>
+      <c r="X46" s="756"/>
+      <c r="Y46" s="751"/>
     </row>
     <row r="47" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L47" s="768"/>
-      <c r="M47" s="734"/>
-      <c r="N47" s="758"/>
+      <c r="L47" s="713"/>
+      <c r="M47" s="716"/>
+      <c r="N47" s="742"/>
       <c r="O47" s="96"/>
       <c r="P47" s="97"/>
       <c r="Q47" s="170" t="s">
@@ -14274,16 +14267,16 @@
       <c r="T47" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U47" s="742"/>
-      <c r="V47" s="745"/>
-      <c r="W47" s="716"/>
-      <c r="X47" s="717"/>
-      <c r="Y47" s="712"/>
+      <c r="U47" s="725"/>
+      <c r="V47" s="728"/>
+      <c r="W47" s="755"/>
+      <c r="X47" s="756"/>
+      <c r="Y47" s="751"/>
     </row>
     <row r="48" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L48" s="769"/>
-      <c r="M48" s="734"/>
-      <c r="N48" s="758"/>
+      <c r="L48" s="714"/>
+      <c r="M48" s="716"/>
+      <c r="N48" s="742"/>
       <c r="O48" s="104"/>
       <c r="P48" s="105"/>
       <c r="Q48" s="171" t="s">
@@ -14296,18 +14289,18 @@
       <c r="T48" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U48" s="742"/>
-      <c r="V48" s="745"/>
-      <c r="W48" s="716"/>
-      <c r="X48" s="717"/>
-      <c r="Y48" s="712"/>
+      <c r="U48" s="725"/>
+      <c r="V48" s="728"/>
+      <c r="W48" s="755"/>
+      <c r="X48" s="756"/>
+      <c r="Y48" s="751"/>
     </row>
     <row r="49" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L49" s="765" t="s">
+      <c r="L49" s="710" t="s">
         <v>100</v>
       </c>
-      <c r="M49" s="734"/>
-      <c r="N49" s="758"/>
+      <c r="M49" s="716"/>
+      <c r="N49" s="742"/>
       <c r="O49" s="98"/>
       <c r="P49" s="99"/>
       <c r="Q49" s="100" t="s">
@@ -14320,16 +14313,16 @@
       <c r="T49" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U49" s="742"/>
-      <c r="V49" s="745"/>
-      <c r="W49" s="716"/>
-      <c r="X49" s="717"/>
-      <c r="Y49" s="712"/>
+      <c r="U49" s="725"/>
+      <c r="V49" s="728"/>
+      <c r="W49" s="755"/>
+      <c r="X49" s="756"/>
+      <c r="Y49" s="751"/>
     </row>
     <row r="50" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L50" s="766"/>
-      <c r="M50" s="734"/>
-      <c r="N50" s="758"/>
+      <c r="L50" s="711"/>
+      <c r="M50" s="716"/>
+      <c r="N50" s="742"/>
       <c r="O50" s="72"/>
       <c r="P50" s="73"/>
       <c r="Q50" s="74" t="s">
@@ -14338,22 +14331,22 @@
       <c r="R50" s="74" t="s">
         <v>92</v>
       </c>
-      <c r="S50" s="738" t="s">
+      <c r="S50" s="721" t="s">
         <v>115</v>
       </c>
       <c r="T50" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U50" s="742"/>
-      <c r="V50" s="745"/>
-      <c r="W50" s="716"/>
-      <c r="X50" s="717"/>
-      <c r="Y50" s="712"/>
+      <c r="U50" s="725"/>
+      <c r="V50" s="728"/>
+      <c r="W50" s="755"/>
+      <c r="X50" s="756"/>
+      <c r="Y50" s="751"/>
     </row>
     <row r="51" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L51" s="766"/>
-      <c r="M51" s="734"/>
-      <c r="N51" s="758"/>
+      <c r="L51" s="711"/>
+      <c r="M51" s="716"/>
+      <c r="N51" s="742"/>
       <c r="O51" s="72"/>
       <c r="P51" s="73"/>
       <c r="Q51" s="74" t="s">
@@ -14362,20 +14355,20 @@
       <c r="R51" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="S51" s="739"/>
+      <c r="S51" s="722"/>
       <c r="T51" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U51" s="742"/>
-      <c r="V51" s="745"/>
-      <c r="W51" s="716"/>
-      <c r="X51" s="717"/>
-      <c r="Y51" s="712"/>
+      <c r="U51" s="725"/>
+      <c r="V51" s="728"/>
+      <c r="W51" s="755"/>
+      <c r="X51" s="756"/>
+      <c r="Y51" s="751"/>
     </row>
     <row r="52" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L52" s="767"/>
-      <c r="M52" s="734"/>
-      <c r="N52" s="758"/>
+      <c r="L52" s="712"/>
+      <c r="M52" s="716"/>
+      <c r="N52" s="742"/>
       <c r="O52" s="75" t="s">
         <v>64</v>
       </c>
@@ -14386,22 +14379,22 @@
       <c r="R52" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="S52" s="740"/>
+      <c r="S52" s="723"/>
       <c r="T52" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="U52" s="742"/>
-      <c r="V52" s="745"/>
-      <c r="W52" s="716"/>
-      <c r="X52" s="717"/>
-      <c r="Y52" s="712"/>
+      <c r="U52" s="725"/>
+      <c r="V52" s="728"/>
+      <c r="W52" s="755"/>
+      <c r="X52" s="756"/>
+      <c r="Y52" s="751"/>
     </row>
     <row r="53" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L53" s="765" t="s">
+      <c r="L53" s="710" t="s">
         <v>99</v>
       </c>
-      <c r="M53" s="734"/>
-      <c r="N53" s="758"/>
+      <c r="M53" s="716"/>
+      <c r="N53" s="742"/>
       <c r="O53" s="83"/>
       <c r="P53" s="84"/>
       <c r="Q53" s="85" t="s">
@@ -14414,16 +14407,16 @@
       <c r="T53" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="U53" s="742"/>
-      <c r="V53" s="745"/>
-      <c r="W53" s="716"/>
-      <c r="X53" s="717"/>
-      <c r="Y53" s="712"/>
+      <c r="U53" s="725"/>
+      <c r="V53" s="728"/>
+      <c r="W53" s="755"/>
+      <c r="X53" s="756"/>
+      <c r="Y53" s="751"/>
     </row>
     <row r="54" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L54" s="766"/>
-      <c r="M54" s="734"/>
-      <c r="N54" s="758"/>
+      <c r="L54" s="711"/>
+      <c r="M54" s="716"/>
+      <c r="N54" s="742"/>
       <c r="O54" s="86"/>
       <c r="P54" s="87"/>
       <c r="Q54" s="88" t="s">
@@ -14436,16 +14429,16 @@
       <c r="T54" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U54" s="742"/>
-      <c r="V54" s="745"/>
-      <c r="W54" s="716"/>
-      <c r="X54" s="717"/>
-      <c r="Y54" s="712"/>
+      <c r="U54" s="725"/>
+      <c r="V54" s="728"/>
+      <c r="W54" s="755"/>
+      <c r="X54" s="756"/>
+      <c r="Y54" s="751"/>
     </row>
     <row r="55" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L55" s="766"/>
-      <c r="M55" s="734"/>
-      <c r="N55" s="758"/>
+      <c r="L55" s="711"/>
+      <c r="M55" s="716"/>
+      <c r="N55" s="742"/>
       <c r="O55" s="86"/>
       <c r="P55" s="87"/>
       <c r="Q55" s="88" t="s">
@@ -14458,16 +14451,16 @@
       <c r="T55" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U55" s="742"/>
-      <c r="V55" s="745"/>
-      <c r="W55" s="716"/>
-      <c r="X55" s="717"/>
-      <c r="Y55" s="712"/>
+      <c r="U55" s="725"/>
+      <c r="V55" s="728"/>
+      <c r="W55" s="755"/>
+      <c r="X55" s="756"/>
+      <c r="Y55" s="751"/>
     </row>
     <row r="56" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L56" s="767"/>
-      <c r="M56" s="734"/>
-      <c r="N56" s="758"/>
+      <c r="L56" s="712"/>
+      <c r="M56" s="716"/>
+      <c r="N56" s="742"/>
       <c r="O56" s="89" t="s">
         <v>54</v>
       </c>
@@ -14484,18 +14477,18 @@
       <c r="T56" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="U56" s="742"/>
-      <c r="V56" s="745"/>
-      <c r="W56" s="716"/>
-      <c r="X56" s="717"/>
-      <c r="Y56" s="712"/>
+      <c r="U56" s="725"/>
+      <c r="V56" s="728"/>
+      <c r="W56" s="755"/>
+      <c r="X56" s="756"/>
+      <c r="Y56" s="751"/>
     </row>
     <row r="57" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L57" s="765" t="s">
+      <c r="L57" s="710" t="s">
         <v>98</v>
       </c>
-      <c r="M57" s="734"/>
-      <c r="N57" s="758"/>
+      <c r="M57" s="716"/>
+      <c r="N57" s="742"/>
       <c r="O57" s="52"/>
       <c r="P57" s="53"/>
       <c r="Q57" s="54" t="s">
@@ -14508,16 +14501,16 @@
       <c r="T57" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="U57" s="742"/>
-      <c r="V57" s="745"/>
-      <c r="W57" s="716"/>
-      <c r="X57" s="717"/>
-      <c r="Y57" s="712"/>
+      <c r="U57" s="725"/>
+      <c r="V57" s="728"/>
+      <c r="W57" s="755"/>
+      <c r="X57" s="756"/>
+      <c r="Y57" s="751"/>
     </row>
     <row r="58" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L58" s="766"/>
-      <c r="M58" s="734"/>
-      <c r="N58" s="758"/>
+      <c r="L58" s="711"/>
+      <c r="M58" s="716"/>
+      <c r="N58" s="742"/>
       <c r="O58" s="55"/>
       <c r="P58" s="56"/>
       <c r="Q58" s="57" t="s">
@@ -14530,16 +14523,16 @@
       <c r="T58" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U58" s="742"/>
-      <c r="V58" s="745"/>
-      <c r="W58" s="716"/>
-      <c r="X58" s="717"/>
-      <c r="Y58" s="712"/>
+      <c r="U58" s="725"/>
+      <c r="V58" s="728"/>
+      <c r="W58" s="755"/>
+      <c r="X58" s="756"/>
+      <c r="Y58" s="751"/>
     </row>
     <row r="59" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L59" s="766"/>
-      <c r="M59" s="734"/>
-      <c r="N59" s="758"/>
+      <c r="L59" s="711"/>
+      <c r="M59" s="716"/>
+      <c r="N59" s="742"/>
       <c r="O59" s="55"/>
       <c r="P59" s="56"/>
       <c r="Q59" s="57" t="s">
@@ -14552,16 +14545,16 @@
       <c r="T59" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U59" s="742"/>
-      <c r="V59" s="745"/>
-      <c r="W59" s="716"/>
-      <c r="X59" s="717"/>
-      <c r="Y59" s="712"/>
+      <c r="U59" s="725"/>
+      <c r="V59" s="728"/>
+      <c r="W59" s="755"/>
+      <c r="X59" s="756"/>
+      <c r="Y59" s="751"/>
     </row>
     <row r="60" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L60" s="767"/>
-      <c r="M60" s="734"/>
-      <c r="N60" s="758"/>
+      <c r="L60" s="712"/>
+      <c r="M60" s="716"/>
+      <c r="N60" s="742"/>
       <c r="O60" s="55"/>
       <c r="P60" s="56"/>
       <c r="Q60" s="57" t="s">
@@ -14574,18 +14567,18 @@
       <c r="T60" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U60" s="742"/>
-      <c r="V60" s="745"/>
-      <c r="W60" s="716"/>
-      <c r="X60" s="717"/>
-      <c r="Y60" s="712"/>
+      <c r="U60" s="725"/>
+      <c r="V60" s="728"/>
+      <c r="W60" s="755"/>
+      <c r="X60" s="756"/>
+      <c r="Y60" s="751"/>
     </row>
     <row r="61" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L61" s="765" t="s">
+      <c r="L61" s="710" t="s">
         <v>97</v>
       </c>
-      <c r="M61" s="734"/>
-      <c r="N61" s="758"/>
+      <c r="M61" s="716"/>
+      <c r="N61" s="742"/>
       <c r="O61" s="55"/>
       <c r="P61" s="56"/>
       <c r="Q61" s="57" t="s">
@@ -14598,16 +14591,16 @@
       <c r="T61" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U61" s="742"/>
-      <c r="V61" s="745"/>
-      <c r="W61" s="716"/>
-      <c r="X61" s="717"/>
-      <c r="Y61" s="712"/>
+      <c r="U61" s="725"/>
+      <c r="V61" s="728"/>
+      <c r="W61" s="755"/>
+      <c r="X61" s="756"/>
+      <c r="Y61" s="751"/>
     </row>
     <row r="62" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L62" s="766"/>
-      <c r="M62" s="734"/>
-      <c r="N62" s="758"/>
+      <c r="L62" s="711"/>
+      <c r="M62" s="716"/>
+      <c r="N62" s="742"/>
       <c r="O62" s="55"/>
       <c r="P62" s="56"/>
       <c r="Q62" s="57" t="s">
@@ -14620,16 +14613,16 @@
       <c r="T62" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U62" s="742"/>
-      <c r="V62" s="745"/>
-      <c r="W62" s="716"/>
-      <c r="X62" s="717"/>
-      <c r="Y62" s="712"/>
+      <c r="U62" s="725"/>
+      <c r="V62" s="728"/>
+      <c r="W62" s="755"/>
+      <c r="X62" s="756"/>
+      <c r="Y62" s="751"/>
     </row>
     <row r="63" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L63" s="766"/>
-      <c r="M63" s="734"/>
-      <c r="N63" s="758"/>
+      <c r="L63" s="711"/>
+      <c r="M63" s="716"/>
+      <c r="N63" s="742"/>
       <c r="O63" s="55"/>
       <c r="P63" s="56"/>
       <c r="Q63" s="57" t="s">
@@ -14642,16 +14635,16 @@
       <c r="T63" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U63" s="742"/>
-      <c r="V63" s="745"/>
-      <c r="W63" s="716"/>
-      <c r="X63" s="717"/>
-      <c r="Y63" s="712"/>
+      <c r="U63" s="725"/>
+      <c r="V63" s="728"/>
+      <c r="W63" s="755"/>
+      <c r="X63" s="756"/>
+      <c r="Y63" s="751"/>
     </row>
     <row r="64" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L64" s="767"/>
-      <c r="M64" s="734"/>
-      <c r="N64" s="758"/>
+      <c r="L64" s="712"/>
+      <c r="M64" s="716"/>
+      <c r="N64" s="742"/>
       <c r="O64" s="58" t="s">
         <v>36</v>
       </c>
@@ -14668,18 +14661,18 @@
       <c r="T64" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="U64" s="742"/>
-      <c r="V64" s="745"/>
-      <c r="W64" s="716"/>
-      <c r="X64" s="717"/>
-      <c r="Y64" s="712"/>
+      <c r="U64" s="725"/>
+      <c r="V64" s="728"/>
+      <c r="W64" s="755"/>
+      <c r="X64" s="756"/>
+      <c r="Y64" s="751"/>
     </row>
     <row r="65" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L65" s="765" t="s">
+      <c r="L65" s="710" t="s">
         <v>96</v>
       </c>
-      <c r="M65" s="734"/>
-      <c r="N65" s="758"/>
+      <c r="M65" s="716"/>
+      <c r="N65" s="742"/>
       <c r="O65" s="61"/>
       <c r="P65" s="62"/>
       <c r="Q65" s="63" t="s">
@@ -14692,16 +14685,16 @@
       <c r="T65" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="U65" s="742"/>
-      <c r="V65" s="745"/>
-      <c r="W65" s="716"/>
-      <c r="X65" s="717"/>
-      <c r="Y65" s="712"/>
+      <c r="U65" s="725"/>
+      <c r="V65" s="728"/>
+      <c r="W65" s="755"/>
+      <c r="X65" s="756"/>
+      <c r="Y65" s="751"/>
     </row>
     <row r="66" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L66" s="766"/>
-      <c r="M66" s="734"/>
-      <c r="N66" s="758"/>
+      <c r="L66" s="711"/>
+      <c r="M66" s="716"/>
+      <c r="N66" s="742"/>
       <c r="O66" s="64"/>
       <c r="P66" s="65"/>
       <c r="Q66" s="66" t="s">
@@ -14714,16 +14707,16 @@
       <c r="T66" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U66" s="742"/>
-      <c r="V66" s="745"/>
-      <c r="W66" s="716"/>
-      <c r="X66" s="717"/>
-      <c r="Y66" s="712"/>
+      <c r="U66" s="725"/>
+      <c r="V66" s="728"/>
+      <c r="W66" s="755"/>
+      <c r="X66" s="756"/>
+      <c r="Y66" s="751"/>
     </row>
     <row r="67" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L67" s="766"/>
-      <c r="M67" s="734"/>
-      <c r="N67" s="758"/>
+      <c r="L67" s="711"/>
+      <c r="M67" s="716"/>
+      <c r="N67" s="742"/>
       <c r="O67" s="64"/>
       <c r="P67" s="65"/>
       <c r="Q67" s="66" t="s">
@@ -14736,16 +14729,16 @@
       <c r="T67" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U67" s="742"/>
-      <c r="V67" s="745"/>
-      <c r="W67" s="716"/>
-      <c r="X67" s="717"/>
-      <c r="Y67" s="712"/>
+      <c r="U67" s="725"/>
+      <c r="V67" s="728"/>
+      <c r="W67" s="755"/>
+      <c r="X67" s="756"/>
+      <c r="Y67" s="751"/>
     </row>
     <row r="68" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L68" s="767"/>
-      <c r="M68" s="735"/>
-      <c r="N68" s="759"/>
+      <c r="L68" s="712"/>
+      <c r="M68" s="717"/>
+      <c r="N68" s="743"/>
       <c r="O68" s="67" t="s">
         <v>25</v>
       </c>
@@ -14762,11 +14755,11 @@
       <c r="T68" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="U68" s="743"/>
-      <c r="V68" s="746"/>
-      <c r="W68" s="718"/>
-      <c r="X68" s="719"/>
-      <c r="Y68" s="713"/>
+      <c r="U68" s="726"/>
+      <c r="V68" s="729"/>
+      <c r="W68" s="757"/>
+      <c r="X68" s="758"/>
+      <c r="Y68" s="752"/>
     </row>
     <row r="69" spans="12:25" x14ac:dyDescent="0.25">
       <c r="N69" s="210"/>
@@ -14774,6 +14767,34 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="Y5:Y68"/>
+    <mergeCell ref="W17:X67"/>
+    <mergeCell ref="W68:X68"/>
+    <mergeCell ref="W5:W16"/>
+    <mergeCell ref="X5:X6"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="X15:X16"/>
+    <mergeCell ref="M5:M68"/>
+    <mergeCell ref="O3:T3"/>
+    <mergeCell ref="S50:S52"/>
+    <mergeCell ref="U5:U68"/>
+    <mergeCell ref="V5:V68"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="N5:N7"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="N8:N11"/>
+    <mergeCell ref="N37:N68"/>
+    <mergeCell ref="N35:N36"/>
+    <mergeCell ref="N31:N34"/>
+    <mergeCell ref="N26:N30"/>
     <mergeCell ref="L65:L68"/>
     <mergeCell ref="L61:L64"/>
     <mergeCell ref="L57:L60"/>
@@ -14790,34 +14811,6 @@
     <mergeCell ref="L49:L52"/>
     <mergeCell ref="L45:L48"/>
     <mergeCell ref="L41:L44"/>
-    <mergeCell ref="M5:M68"/>
-    <mergeCell ref="O3:T3"/>
-    <mergeCell ref="S50:S52"/>
-    <mergeCell ref="U5:U68"/>
-    <mergeCell ref="V5:V68"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="N5:N7"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="N8:N11"/>
-    <mergeCell ref="N37:N68"/>
-    <mergeCell ref="N35:N36"/>
-    <mergeCell ref="N31:N34"/>
-    <mergeCell ref="N26:N30"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="Y5:Y68"/>
-    <mergeCell ref="W17:X67"/>
-    <mergeCell ref="W68:X68"/>
-    <mergeCell ref="W5:W16"/>
-    <mergeCell ref="X5:X6"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="X15:X16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -14844,13 +14837,13 @@
       <c r="C4" s="476" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="770" t="s">
+      <c r="D4" s="786" t="s">
         <v>119</v>
       </c>
-      <c r="E4" s="771"/>
-      <c r="F4" s="771"/>
-      <c r="G4" s="771"/>
-      <c r="H4" s="771"/>
+      <c r="E4" s="787"/>
+      <c r="F4" s="787"/>
+      <c r="G4" s="787"/>
+      <c r="H4" s="787"/>
       <c r="I4" s="492"/>
     </row>
     <row r="5" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14877,7 +14870,7 @@
       </c>
     </row>
     <row r="6" spans="3:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="772" t="s">
+      <c r="C6" s="788" t="s">
         <v>111</v>
       </c>
       <c r="D6" s="483"/>
@@ -14889,12 +14882,12 @@
       <c r="H6" s="490" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="779" t="s">
+      <c r="I6" s="771" t="s">
         <v>876</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="773"/>
+      <c r="C7" s="777"/>
       <c r="D7" s="443"/>
       <c r="E7" s="65"/>
       <c r="F7" s="65"/>
@@ -14902,10 +14895,10 @@
       <c r="H7" s="457" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="780"/>
+      <c r="I7" s="772"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="773"/>
+      <c r="C8" s="777"/>
       <c r="D8" s="443"/>
       <c r="E8" s="65"/>
       <c r="F8" s="65"/>
@@ -14913,10 +14906,10 @@
       <c r="H8" s="457" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="780"/>
+      <c r="I8" s="772"/>
     </row>
     <row r="9" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="774"/>
+      <c r="C9" s="778"/>
       <c r="D9" s="444" t="s">
         <v>73</v>
       </c>
@@ -14930,10 +14923,10 @@
       <c r="H9" s="478" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="786"/>
+      <c r="I9" s="773"/>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="775" t="s">
+      <c r="C10" s="776" t="s">
         <v>110</v>
       </c>
       <c r="D10" s="488"/>
@@ -14945,12 +14938,12 @@
       <c r="H10" s="503" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="777" t="s">
+      <c r="I10" s="774" t="s">
         <v>879</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="773"/>
+      <c r="C11" s="777"/>
       <c r="D11" s="72"/>
       <c r="E11" s="73"/>
       <c r="F11" s="65"/>
@@ -14958,10 +14951,10 @@
       <c r="H11" s="456" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="777"/>
+      <c r="I11" s="774"/>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="773"/>
+      <c r="C12" s="777"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="65"/>
@@ -14969,10 +14962,10 @@
       <c r="H12" s="456" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="777"/>
+      <c r="I12" s="774"/>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="774"/>
+      <c r="C13" s="778"/>
       <c r="D13" s="96"/>
       <c r="E13" s="97"/>
       <c r="F13" s="82" t="s">
@@ -14982,10 +14975,10 @@
       <c r="H13" s="501" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="777"/>
+      <c r="I13" s="774"/>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="775" t="s">
+      <c r="C14" s="776" t="s">
         <v>109</v>
       </c>
       <c r="D14" s="101"/>
@@ -14997,10 +14990,10 @@
       <c r="H14" s="505" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="777"/>
+      <c r="I14" s="774"/>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="773"/>
+      <c r="C15" s="777"/>
       <c r="D15" s="72"/>
       <c r="E15" s="73"/>
       <c r="F15" s="65"/>
@@ -15008,10 +15001,10 @@
       <c r="H15" s="456" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="777"/>
+      <c r="I15" s="774"/>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="773"/>
+      <c r="C16" s="777"/>
       <c r="D16" s="96"/>
       <c r="E16" s="97"/>
       <c r="F16" s="65"/>
@@ -15019,10 +15012,10 @@
       <c r="H16" s="456" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="777"/>
+      <c r="I16" s="774"/>
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C17" s="774"/>
+      <c r="C17" s="778"/>
       <c r="D17" s="104"/>
       <c r="E17" s="105"/>
       <c r="F17" s="113" t="s">
@@ -15032,10 +15025,10 @@
       <c r="H17" s="501" t="s">
         <v>32</v>
       </c>
-      <c r="I17" s="777"/>
+      <c r="I17" s="774"/>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C18" s="775" t="s">
+      <c r="C18" s="776" t="s">
         <v>108</v>
       </c>
       <c r="D18" s="98"/>
@@ -15047,10 +15040,10 @@
       <c r="H18" s="505" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="777"/>
+      <c r="I18" s="774"/>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C19" s="773"/>
+      <c r="C19" s="777"/>
       <c r="D19" s="72"/>
       <c r="E19" s="73"/>
       <c r="F19" s="65"/>
@@ -15058,10 +15051,10 @@
       <c r="H19" s="456" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="777"/>
+      <c r="I19" s="774"/>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C20" s="773"/>
+      <c r="C20" s="777"/>
       <c r="D20" s="96"/>
       <c r="E20" s="97"/>
       <c r="F20" s="65"/>
@@ -15069,10 +15062,10 @@
       <c r="H20" s="456" t="s">
         <v>32</v>
       </c>
-      <c r="I20" s="777"/>
+      <c r="I20" s="774"/>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C21" s="774"/>
+      <c r="C21" s="778"/>
       <c r="D21" s="104"/>
       <c r="E21" s="105"/>
       <c r="F21" s="82" t="s">
@@ -15082,10 +15075,10 @@
       <c r="H21" s="506" t="s">
         <v>32</v>
       </c>
-      <c r="I21" s="777"/>
+      <c r="I21" s="774"/>
     </row>
     <row r="22" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C22" s="775" t="s">
+      <c r="C22" s="776" t="s">
         <v>107</v>
       </c>
       <c r="D22" s="98"/>
@@ -15097,10 +15090,10 @@
       <c r="H22" s="504" t="s">
         <v>32</v>
       </c>
-      <c r="I22" s="777"/>
+      <c r="I22" s="774"/>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C23" s="773"/>
+      <c r="C23" s="777"/>
       <c r="D23" s="72"/>
       <c r="E23" s="73"/>
       <c r="F23" s="65"/>
@@ -15108,10 +15101,10 @@
       <c r="H23" s="456" t="s">
         <v>32</v>
       </c>
-      <c r="I23" s="777"/>
+      <c r="I23" s="774"/>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C24" s="773"/>
+      <c r="C24" s="777"/>
       <c r="D24" s="72"/>
       <c r="E24" s="73"/>
       <c r="F24" s="81"/>
@@ -15119,10 +15112,10 @@
       <c r="H24" s="456" t="s">
         <v>32</v>
       </c>
-      <c r="I24" s="777"/>
+      <c r="I24" s="774"/>
     </row>
     <row r="25" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="774"/>
+      <c r="C25" s="778"/>
       <c r="D25" s="96" t="s">
         <v>64</v>
       </c>
@@ -15136,10 +15129,10 @@
       <c r="H25" s="501" t="s">
         <v>32</v>
       </c>
-      <c r="I25" s="778"/>
+      <c r="I25" s="775"/>
     </row>
     <row r="26" spans="3:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="775" t="s">
+      <c r="C26" s="776" t="s">
         <v>106</v>
       </c>
       <c r="D26" s="484" t="s">
@@ -15162,7 +15155,7 @@
       </c>
     </row>
     <row r="27" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="773"/>
+      <c r="C27" s="777"/>
       <c r="D27" s="447"/>
       <c r="E27" s="448"/>
       <c r="F27" s="62"/>
@@ -15172,12 +15165,12 @@
       <c r="H27" s="477" t="s">
         <v>33</v>
       </c>
-      <c r="I27" s="787" t="s">
+      <c r="I27" s="779" t="s">
         <v>896</v>
       </c>
     </row>
     <row r="28" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="773"/>
+      <c r="C28" s="777"/>
       <c r="D28" s="445"/>
       <c r="E28" s="446"/>
       <c r="F28" s="81"/>
@@ -15185,10 +15178,10 @@
       <c r="H28" s="457" t="s">
         <v>33</v>
       </c>
-      <c r="I28" s="780"/>
+      <c r="I28" s="772"/>
     </row>
     <row r="29" spans="3:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="774"/>
+      <c r="C29" s="778"/>
       <c r="D29" s="445"/>
       <c r="E29" s="446"/>
       <c r="F29" s="82" t="s">
@@ -15198,7 +15191,7 @@
       <c r="H29" s="478" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="781"/>
+      <c r="I29" s="780"/>
       <c r="J29" s="497" t="s">
         <v>84</v>
       </c>
@@ -15219,7 +15212,7 @@
       </c>
     </row>
     <row r="30" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="775" t="s">
+      <c r="C30" s="776" t="s">
         <v>105</v>
       </c>
       <c r="D30" s="449"/>
@@ -15242,12 +15235,12 @@
       <c r="N30" s="462" t="s">
         <v>32</v>
       </c>
-      <c r="O30" s="779" t="s">
+      <c r="O30" s="771" t="s">
         <v>894</v>
       </c>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C31" s="773"/>
+      <c r="C31" s="777"/>
       <c r="D31" s="64"/>
       <c r="E31" s="65"/>
       <c r="F31" s="65"/>
@@ -15266,10 +15259,10 @@
       <c r="N31" s="456" t="s">
         <v>32</v>
       </c>
-      <c r="O31" s="780"/>
+      <c r="O31" s="772"/>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C32" s="773"/>
+      <c r="C32" s="777"/>
       <c r="D32" s="64"/>
       <c r="E32" s="65"/>
       <c r="F32" s="65"/>
@@ -15288,10 +15281,10 @@
       <c r="N32" s="456" t="s">
         <v>32</v>
       </c>
-      <c r="O32" s="780"/>
+      <c r="O32" s="772"/>
     </row>
     <row r="33" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="774"/>
+      <c r="C33" s="778"/>
       <c r="D33" s="452" t="s">
         <v>73</v>
       </c>
@@ -15316,10 +15309,10 @@
       <c r="N33" s="456" t="s">
         <v>32</v>
       </c>
-      <c r="O33" s="780"/>
+      <c r="O33" s="772"/>
     </row>
     <row r="34" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C34" s="775" t="s">
+      <c r="C34" s="776" t="s">
         <v>104</v>
       </c>
       <c r="D34" s="61"/>
@@ -15342,10 +15335,10 @@
       <c r="N34" s="456" t="s">
         <v>32</v>
       </c>
-      <c r="O34" s="780"/>
+      <c r="O34" s="772"/>
     </row>
     <row r="35" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C35" s="773"/>
+      <c r="C35" s="777"/>
       <c r="D35" s="64"/>
       <c r="E35" s="65"/>
       <c r="F35" s="65"/>
@@ -15364,10 +15357,10 @@
       <c r="N35" s="456" t="s">
         <v>32</v>
       </c>
-      <c r="O35" s="780"/>
+      <c r="O35" s="772"/>
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C36" s="773"/>
+      <c r="C36" s="777"/>
       <c r="D36" s="64"/>
       <c r="E36" s="65"/>
       <c r="F36" s="65"/>
@@ -15386,10 +15379,10 @@
       <c r="N36" s="457" t="s">
         <v>33</v>
       </c>
-      <c r="O36" s="780"/>
+      <c r="O36" s="772"/>
     </row>
     <row r="37" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="774"/>
+      <c r="C37" s="778"/>
       <c r="D37" s="80" t="s">
         <v>73</v>
       </c>
@@ -15418,10 +15411,10 @@
       <c r="N37" s="458" t="s">
         <v>33</v>
       </c>
-      <c r="O37" s="781"/>
+      <c r="O37" s="780"/>
     </row>
     <row r="38" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="775" t="s">
+      <c r="C38" s="776" t="s">
         <v>103</v>
       </c>
       <c r="D38" s="449"/>
@@ -15437,7 +15430,7 @@
       </c>
     </row>
     <row r="39" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C39" s="773"/>
+      <c r="C39" s="777"/>
       <c r="D39" s="64"/>
       <c r="E39" s="65"/>
       <c r="F39" s="66" t="s">
@@ -15451,7 +15444,7 @@
       </c>
     </row>
     <row r="40" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C40" s="773"/>
+      <c r="C40" s="777"/>
       <c r="D40" s="64"/>
       <c r="E40" s="65"/>
       <c r="F40" s="66" t="s">
@@ -15465,7 +15458,7 @@
       </c>
     </row>
     <row r="41" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C41" s="774"/>
+      <c r="C41" s="778"/>
       <c r="D41" s="108"/>
       <c r="E41" s="109"/>
       <c r="F41" s="82" t="s">
@@ -15479,7 +15472,7 @@
       </c>
     </row>
     <row r="42" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C42" s="775" t="s">
+      <c r="C42" s="776" t="s">
         <v>102</v>
       </c>
       <c r="D42" s="61"/>
@@ -15495,7 +15488,7 @@
       </c>
     </row>
     <row r="43" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C43" s="773"/>
+      <c r="C43" s="777"/>
       <c r="D43" s="64"/>
       <c r="E43" s="65"/>
       <c r="F43" s="66" t="s">
@@ -15509,7 +15502,7 @@
       </c>
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C44" s="773"/>
+      <c r="C44" s="777"/>
       <c r="D44" s="64"/>
       <c r="E44" s="65"/>
       <c r="F44" s="82" t="s">
@@ -15523,7 +15516,7 @@
       </c>
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C45" s="774"/>
+      <c r="C45" s="778"/>
       <c r="D45" s="80"/>
       <c r="E45" s="81"/>
       <c r="F45" s="113" t="s">
@@ -15537,7 +15530,7 @@
       </c>
     </row>
     <row r="46" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C46" s="775" t="s">
+      <c r="C46" s="776" t="s">
         <v>101</v>
       </c>
       <c r="D46" s="106"/>
@@ -15595,7 +15588,7 @@
       </c>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C50" s="775" t="s">
+      <c r="C50" s="776" t="s">
         <v>100</v>
       </c>
       <c r="D50" s="61"/>
@@ -15611,7 +15604,7 @@
       </c>
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C51" s="773"/>
+      <c r="C51" s="777"/>
       <c r="D51" s="64"/>
       <c r="E51" s="65"/>
       <c r="F51" s="66" t="s">
@@ -15625,7 +15618,7 @@
       </c>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C52" s="773"/>
+      <c r="C52" s="777"/>
       <c r="D52" s="64"/>
       <c r="E52" s="65"/>
       <c r="F52" s="66" t="s">
@@ -15639,7 +15632,7 @@
       </c>
     </row>
     <row r="53" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="774"/>
+      <c r="C53" s="778"/>
       <c r="D53" s="452" t="s">
         <v>73</v>
       </c>
@@ -15657,7 +15650,7 @@
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C54" s="775" t="s">
+      <c r="C54" s="776" t="s">
         <v>99</v>
       </c>
       <c r="D54" s="61"/>
@@ -15673,7 +15666,7 @@
       </c>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C55" s="773"/>
+      <c r="C55" s="777"/>
       <c r="D55" s="64"/>
       <c r="E55" s="65"/>
       <c r="F55" s="66" t="s">
@@ -15687,7 +15680,7 @@
       </c>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C56" s="773"/>
+      <c r="C56" s="777"/>
       <c r="D56" s="80"/>
       <c r="E56" s="81"/>
       <c r="F56" s="66" t="s">
@@ -15701,7 +15694,7 @@
       </c>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C57" s="774"/>
+      <c r="C57" s="778"/>
       <c r="D57" s="108"/>
       <c r="E57" s="109"/>
       <c r="F57" s="82" t="s">
@@ -15715,7 +15708,7 @@
       </c>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C58" s="775" t="s">
+      <c r="C58" s="776" t="s">
         <v>98</v>
       </c>
       <c r="D58" s="61"/>
@@ -15731,7 +15724,7 @@
       </c>
     </row>
     <row r="59" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C59" s="773"/>
+      <c r="C59" s="777"/>
       <c r="D59" s="64"/>
       <c r="E59" s="65"/>
       <c r="F59" s="66" t="s">
@@ -15745,7 +15738,7 @@
       </c>
     </row>
     <row r="60" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C60" s="773"/>
+      <c r="C60" s="777"/>
       <c r="D60" s="80"/>
       <c r="E60" s="81"/>
       <c r="F60" s="66" t="s">
@@ -15759,7 +15752,7 @@
       </c>
     </row>
     <row r="61" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C61" s="774"/>
+      <c r="C61" s="778"/>
       <c r="D61" s="80"/>
       <c r="E61" s="81"/>
       <c r="F61" s="82" t="s">
@@ -15773,7 +15766,7 @@
       </c>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C62" s="775" t="s">
+      <c r="C62" s="776" t="s">
         <v>97</v>
       </c>
       <c r="D62" s="106"/>
@@ -15789,7 +15782,7 @@
       </c>
     </row>
     <row r="63" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C63" s="773"/>
+      <c r="C63" s="777"/>
       <c r="D63" s="64"/>
       <c r="E63" s="65"/>
       <c r="F63" s="66" t="s">
@@ -15803,7 +15796,7 @@
       </c>
     </row>
     <row r="64" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C64" s="773"/>
+      <c r="C64" s="777"/>
       <c r="D64" s="64"/>
       <c r="E64" s="65"/>
       <c r="F64" s="66" t="s">
@@ -15817,7 +15810,7 @@
       </c>
     </row>
     <row r="65" spans="3:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C65" s="774"/>
+      <c r="C65" s="778"/>
       <c r="D65" s="110"/>
       <c r="E65" s="109"/>
       <c r="F65" s="113" t="s">
@@ -15849,7 +15842,7 @@
       </c>
     </row>
     <row r="66" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C66" s="775" t="s">
+      <c r="C66" s="776" t="s">
         <v>96</v>
       </c>
       <c r="D66" s="61"/>
@@ -15875,12 +15868,12 @@
       <c r="N66" s="475" t="s">
         <v>33</v>
       </c>
-      <c r="O66" s="776" t="s">
+      <c r="O66" s="781" t="s">
         <v>874</v>
       </c>
     </row>
     <row r="67" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C67" s="773"/>
+      <c r="C67" s="777"/>
       <c r="D67" s="64"/>
       <c r="E67" s="65"/>
       <c r="F67" s="66" t="s">
@@ -15904,10 +15897,10 @@
       <c r="N67" s="471" t="s">
         <v>32</v>
       </c>
-      <c r="O67" s="777"/>
+      <c r="O67" s="774"/>
     </row>
     <row r="68" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C68" s="773"/>
+      <c r="C68" s="777"/>
       <c r="D68" s="64"/>
       <c r="E68" s="65"/>
       <c r="F68" s="66" t="s">
@@ -15931,7 +15924,7 @@
       <c r="N68" s="471" t="s">
         <v>32</v>
       </c>
-      <c r="O68" s="777"/>
+      <c r="O68" s="774"/>
     </row>
     <row r="69" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C69" s="784"/>
@@ -15966,16 +15959,16 @@
       <c r="N69" s="472" t="s">
         <v>32</v>
       </c>
-      <c r="O69" s="778"/>
+      <c r="O69" s="775"/>
     </row>
     <row r="70" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="I6:I9"/>
-    <mergeCell ref="I10:I25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C18:C21"/>
     <mergeCell ref="O66:O69"/>
     <mergeCell ref="O30:O37"/>
     <mergeCell ref="C38:C41"/>
@@ -15989,11 +15982,11 @@
     <mergeCell ref="C62:C65"/>
     <mergeCell ref="C66:C69"/>
     <mergeCell ref="I66:I69"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="I6:I9"/>
+    <mergeCell ref="I10:I25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="I27:I29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17448,16 +17441,16 @@
     <row r="2" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" s="514"/>
       <c r="C2" s="515"/>
-      <c r="D2" s="788" t="s">
+      <c r="D2" s="789" t="s">
         <v>900</v>
       </c>
-      <c r="E2" s="789"/>
+      <c r="E2" s="790"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="790" t="s">
+      <c r="B3" s="791" t="s">
         <v>897</v>
       </c>
-      <c r="C3" s="791"/>
+      <c r="C3" s="792"/>
       <c r="D3" s="516" t="s">
         <v>902</v>
       </c>
@@ -17838,7 +17831,7 @@
       <c r="B3" s="511" t="s">
         <v>919</v>
       </c>
-      <c r="C3" s="792" t="s">
+      <c r="C3" s="793" t="s">
         <v>932</v>
       </c>
     </row>
@@ -17846,13 +17839,13 @@
       <c r="B4" s="512" t="s">
         <v>920</v>
       </c>
-      <c r="C4" s="793"/>
+      <c r="C4" s="794"/>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B5" s="512" t="s">
         <v>921</v>
       </c>
-      <c r="C5" s="793"/>
+      <c r="C5" s="794"/>
       <c r="F5" s="527" t="s">
         <v>196</v>
       </c>
@@ -17907,7 +17900,7 @@
       <c r="B6" s="512" t="s">
         <v>922</v>
       </c>
-      <c r="C6" s="793"/>
+      <c r="C6" s="794"/>
       <c r="F6" s="526"/>
       <c r="G6" s="528" t="s">
         <v>962</v>
@@ -17964,7 +17957,7 @@
       <c r="B7" s="512" t="s">
         <v>923</v>
       </c>
-      <c r="C7" s="793"/>
+      <c r="C7" s="794"/>
       <c r="F7" s="526"/>
       <c r="G7" s="526"/>
       <c r="H7" s="528" t="s">
@@ -18021,7 +18014,7 @@
       <c r="B8" s="512" t="s">
         <v>933</v>
       </c>
-      <c r="C8" s="793"/>
+      <c r="C8" s="794"/>
       <c r="F8" s="526"/>
       <c r="G8" s="527" t="s">
         <v>216</v>
@@ -18076,13 +18069,13 @@
       <c r="B9" s="512" t="s">
         <v>924</v>
       </c>
-      <c r="C9" s="793"/>
+      <c r="C9" s="794"/>
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" s="512" t="s">
         <v>925</v>
       </c>
-      <c r="C10" s="793"/>
+      <c r="C10" s="794"/>
       <c r="F10" s="530" t="s">
         <v>97</v>
       </c>
@@ -18137,7 +18130,7 @@
       <c r="B11" s="512" t="s">
         <v>926</v>
       </c>
-      <c r="C11" s="793"/>
+      <c r="C11" s="794"/>
       <c r="F11" s="526"/>
       <c r="G11" s="528" t="s">
         <v>943</v>
@@ -18245,7 +18238,7 @@
       <c r="B13" s="512" t="s">
         <v>927</v>
       </c>
-      <c r="C13" s="794" t="s">
+      <c r="C13" s="795" t="s">
         <v>931</v>
       </c>
       <c r="F13" s="526"/>
@@ -18302,19 +18295,19 @@
       <c r="B14" s="512" t="s">
         <v>928</v>
       </c>
-      <c r="C14" s="795"/>
+      <c r="C14" s="796"/>
     </row>
     <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B15" s="512" t="s">
         <v>929</v>
       </c>
-      <c r="C15" s="795"/>
+      <c r="C15" s="796"/>
     </row>
     <row r="16" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="513" t="s">
         <v>930</v>
       </c>
-      <c r="C16" s="796"/>
+      <c r="C16" s="797"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -19248,10 +19241,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="797" t="s">
+      <c r="B1" s="798" t="s">
         <v>648</v>
       </c>
-      <c r="C1" s="798"/>
+      <c r="C1" s="799"/>
       <c r="D1" s="337" t="s">
         <v>657</v>
       </c>
@@ -20609,15 +20602,15 @@
       <c r="D5" s="179" t="s">
         <v>266</v>
       </c>
-      <c r="E5" s="799" t="s">
+      <c r="E5" s="800" t="s">
         <v>270</v>
       </c>
-      <c r="F5" s="800"/>
-      <c r="G5" s="801" t="s">
+      <c r="F5" s="801"/>
+      <c r="G5" s="802" t="s">
         <v>271</v>
       </c>
-      <c r="H5" s="801"/>
-      <c r="I5" s="800"/>
+      <c r="H5" s="802"/>
+      <c r="I5" s="801"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -20719,58 +20712,58 @@
       <c r="M9" s="181"/>
       <c r="N9" s="181"/>
       <c r="O9" s="181"/>
-      <c r="P9" s="799" t="s">
+      <c r="P9" s="800" t="s">
         <v>285</v>
       </c>
-      <c r="Q9" s="802"/>
-      <c r="R9" s="799" t="s">
+      <c r="Q9" s="803"/>
+      <c r="R9" s="800" t="s">
         <v>270</v>
       </c>
-      <c r="S9" s="802"/>
+      <c r="S9" s="803"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C10" s="174" t="s">
         <v>286</v>
       </c>
-      <c r="D10" s="803" t="s">
+      <c r="D10" s="804" t="s">
         <v>271</v>
       </c>
-      <c r="E10" s="804"/>
-      <c r="F10" s="804"/>
-      <c r="G10" s="804"/>
-      <c r="H10" s="804"/>
-      <c r="I10" s="804"/>
-      <c r="J10" s="804"/>
-      <c r="K10" s="804"/>
-      <c r="L10" s="804"/>
-      <c r="M10" s="804"/>
-      <c r="N10" s="804"/>
-      <c r="O10" s="804"/>
-      <c r="P10" s="804"/>
-      <c r="Q10" s="804"/>
-      <c r="R10" s="804"/>
-      <c r="S10" s="727"/>
+      <c r="E10" s="805"/>
+      <c r="F10" s="805"/>
+      <c r="G10" s="805"/>
+      <c r="H10" s="805"/>
+      <c r="I10" s="805"/>
+      <c r="J10" s="805"/>
+      <c r="K10" s="805"/>
+      <c r="L10" s="805"/>
+      <c r="M10" s="805"/>
+      <c r="N10" s="805"/>
+      <c r="O10" s="805"/>
+      <c r="P10" s="805"/>
+      <c r="Q10" s="805"/>
+      <c r="R10" s="805"/>
+      <c r="S10" s="765"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>268</v>
       </c>
-      <c r="D11" s="805"/>
-      <c r="E11" s="806"/>
-      <c r="F11" s="806"/>
-      <c r="G11" s="806"/>
-      <c r="H11" s="806"/>
-      <c r="I11" s="806"/>
-      <c r="J11" s="806"/>
-      <c r="K11" s="806"/>
-      <c r="L11" s="806"/>
-      <c r="M11" s="806"/>
-      <c r="N11" s="806"/>
-      <c r="O11" s="806"/>
-      <c r="P11" s="806"/>
-      <c r="Q11" s="806"/>
-      <c r="R11" s="806"/>
-      <c r="S11" s="729"/>
+      <c r="D11" s="806"/>
+      <c r="E11" s="807"/>
+      <c r="F11" s="807"/>
+      <c r="G11" s="807"/>
+      <c r="H11" s="807"/>
+      <c r="I11" s="807"/>
+      <c r="J11" s="807"/>
+      <c r="K11" s="807"/>
+      <c r="L11" s="807"/>
+      <c r="M11" s="807"/>
+      <c r="N11" s="807"/>
+      <c r="O11" s="807"/>
+      <c r="P11" s="807"/>
+      <c r="Q11" s="807"/>
+      <c r="R11" s="807"/>
+      <c r="S11" s="767"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
@@ -20873,94 +20866,94 @@
       <c r="D19" s="180" t="s">
         <v>292</v>
       </c>
-      <c r="E19" s="810" t="s">
+      <c r="E19" s="811" t="s">
         <v>294</v>
       </c>
-      <c r="F19" s="811"/>
-      <c r="G19" s="811"/>
-      <c r="H19" s="811"/>
-      <c r="I19" s="811"/>
-      <c r="J19" s="811"/>
-      <c r="K19" s="811"/>
-      <c r="L19" s="811"/>
-      <c r="M19" s="811"/>
-      <c r="N19" s="811"/>
-      <c r="O19" s="811"/>
-      <c r="P19" s="811"/>
-      <c r="Q19" s="811"/>
-      <c r="R19" s="811"/>
-      <c r="S19" s="748"/>
+      <c r="F19" s="812"/>
+      <c r="G19" s="812"/>
+      <c r="H19" s="812"/>
+      <c r="I19" s="812"/>
+      <c r="J19" s="812"/>
+      <c r="K19" s="812"/>
+      <c r="L19" s="812"/>
+      <c r="M19" s="812"/>
+      <c r="N19" s="812"/>
+      <c r="O19" s="812"/>
+      <c r="P19" s="812"/>
+      <c r="Q19" s="812"/>
+      <c r="R19" s="812"/>
+      <c r="S19" s="732"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C20" s="174" t="s">
         <v>272</v>
       </c>
-      <c r="D20" s="807" t="s">
+      <c r="D20" s="808" t="s">
         <v>295</v>
       </c>
-      <c r="E20" s="808"/>
-      <c r="F20" s="808"/>
-      <c r="G20" s="808"/>
-      <c r="H20" s="808"/>
-      <c r="I20" s="808"/>
-      <c r="J20" s="808"/>
-      <c r="K20" s="808"/>
-      <c r="L20" s="808"/>
-      <c r="M20" s="808"/>
-      <c r="N20" s="808"/>
-      <c r="O20" s="808"/>
-      <c r="P20" s="809"/>
+      <c r="E20" s="809"/>
+      <c r="F20" s="809"/>
+      <c r="G20" s="809"/>
+      <c r="H20" s="809"/>
+      <c r="I20" s="809"/>
+      <c r="J20" s="809"/>
+      <c r="K20" s="809"/>
+      <c r="L20" s="809"/>
+      <c r="M20" s="809"/>
+      <c r="N20" s="809"/>
+      <c r="O20" s="809"/>
+      <c r="P20" s="810"/>
       <c r="Q20" s="183" t="s">
         <v>112</v>
       </c>
-      <c r="R20" s="799" t="s">
+      <c r="R20" s="800" t="s">
         <v>270</v>
       </c>
-      <c r="S20" s="802"/>
+      <c r="S20" s="803"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C21" s="174" t="s">
         <v>286</v>
       </c>
-      <c r="D21" s="803" t="s">
+      <c r="D21" s="804" t="s">
         <v>271</v>
       </c>
-      <c r="E21" s="804"/>
-      <c r="F21" s="804"/>
-      <c r="G21" s="804"/>
-      <c r="H21" s="804"/>
-      <c r="I21" s="804"/>
-      <c r="J21" s="804"/>
-      <c r="K21" s="804"/>
-      <c r="L21" s="804"/>
-      <c r="M21" s="804"/>
-      <c r="N21" s="804"/>
-      <c r="O21" s="804"/>
-      <c r="P21" s="804"/>
-      <c r="Q21" s="804"/>
-      <c r="R21" s="804"/>
-      <c r="S21" s="727"/>
+      <c r="E21" s="805"/>
+      <c r="F21" s="805"/>
+      <c r="G21" s="805"/>
+      <c r="H21" s="805"/>
+      <c r="I21" s="805"/>
+      <c r="J21" s="805"/>
+      <c r="K21" s="805"/>
+      <c r="L21" s="805"/>
+      <c r="M21" s="805"/>
+      <c r="N21" s="805"/>
+      <c r="O21" s="805"/>
+      <c r="P21" s="805"/>
+      <c r="Q21" s="805"/>
+      <c r="R21" s="805"/>
+      <c r="S21" s="765"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>268</v>
       </c>
-      <c r="D22" s="805"/>
-      <c r="E22" s="806"/>
-      <c r="F22" s="806"/>
-      <c r="G22" s="806"/>
-      <c r="H22" s="806"/>
-      <c r="I22" s="806"/>
-      <c r="J22" s="806"/>
-      <c r="K22" s="806"/>
-      <c r="L22" s="806"/>
-      <c r="M22" s="806"/>
-      <c r="N22" s="806"/>
-      <c r="O22" s="806"/>
-      <c r="P22" s="806"/>
-      <c r="Q22" s="806"/>
-      <c r="R22" s="806"/>
-      <c r="S22" s="729"/>
+      <c r="D22" s="806"/>
+      <c r="E22" s="807"/>
+      <c r="F22" s="807"/>
+      <c r="G22" s="807"/>
+      <c r="H22" s="807"/>
+      <c r="I22" s="807"/>
+      <c r="J22" s="807"/>
+      <c r="K22" s="807"/>
+      <c r="L22" s="807"/>
+      <c r="M22" s="807"/>
+      <c r="N22" s="807"/>
+      <c r="O22" s="807"/>
+      <c r="P22" s="807"/>
+      <c r="Q22" s="807"/>
+      <c r="R22" s="807"/>
+      <c r="S22" s="767"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="K24" t="s">

</xml_diff>

<commit_message>
1) phys. Tastatur Korrektur für ',' 2) Speicher löschen über gesamten Speicher
</commit_message>
<xml_diff>
--- a/DOC/DEG2000.xlsx
+++ b/DOC/DEG2000.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\devel\1 DEG2000\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2F0F48-EC52-43AB-8077-5ADA2BA63B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCEFADC-CFAA-4035-B4C9-C159D45E48F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="7125" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{F91C61BF-F393-4C13-9000-551DF6FEF055}"/>
+    <workbookView xWindow="22110" yWindow="5325" windowWidth="30900" windowHeight="25815" activeTab="1" xr2:uid="{F91C61BF-F393-4C13-9000-551DF6FEF055}"/>
   </bookViews>
   <sheets>
     <sheet name="DataGridView" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2815" uniqueCount="1520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2831" uniqueCount="1534">
   <si>
     <t>cpuStatus</t>
   </si>
@@ -4716,6 +4716,48 @@
   </si>
   <si>
     <t>128</t>
+  </si>
+  <si>
+    <t>sbios1</t>
+  </si>
+  <si>
+    <t>opsmac</t>
+  </si>
+  <si>
+    <t>op12</t>
+  </si>
+  <si>
+    <t>abios1</t>
+  </si>
+  <si>
+    <t>gosys1</t>
+  </si>
+  <si>
+    <t>abios2</t>
+  </si>
+  <si>
+    <t>gosys2</t>
+  </si>
+  <si>
+    <t>gosys3</t>
+  </si>
+  <si>
+    <t>18E5</t>
+  </si>
+  <si>
+    <t>13A4</t>
+  </si>
+  <si>
+    <t>out</t>
+  </si>
+  <si>
+    <t>541</t>
+  </si>
+  <si>
+    <t>setla:</t>
+  </si>
+  <si>
+    <t>resla:</t>
   </si>
 </sst>
 </file>
@@ -11257,41 +11299,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="315" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="81" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="123" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="316" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="317" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="68" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="320" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="321" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="322" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="137" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -11301,9 +11380,6 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -11336,9 +11412,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="18" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -11392,72 +11465,61 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="81" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="68" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="315" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="123" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="316" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="317" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="320" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="321" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="322" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="137" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="183" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="184" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="186" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="187" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="189" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="185" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="187" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="185" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="327" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -11503,15 +11565,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="332" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="186" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="187" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="185" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="329" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -11527,45 +11580,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="328" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="183" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="191" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="184" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="175" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="189" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="179" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="187" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="185" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="180" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="199" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="177" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="178" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="177" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="200" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="179" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="180" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="202" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="178" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="175" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="177" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="191" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="215" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -15616,7 +15658,7 @@
       <c r="P6" s="1102"/>
       <c r="Q6" s="1102"/>
       <c r="R6" s="1102"/>
-      <c r="S6" s="1042"/>
+      <c r="S6" s="997"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
@@ -15637,7 +15679,7 @@
       <c r="P7" s="1104"/>
       <c r="Q7" s="1104"/>
       <c r="R7" s="1104"/>
-      <c r="S7" s="1044"/>
+      <c r="S7" s="999"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -15810,7 +15852,7 @@
       <c r="P15" s="1102"/>
       <c r="Q15" s="1102"/>
       <c r="R15" s="1102"/>
-      <c r="S15" s="1042"/>
+      <c r="S15" s="997"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
@@ -15831,7 +15873,7 @@
       <c r="P16" s="1104"/>
       <c r="Q16" s="1104"/>
       <c r="R16" s="1104"/>
-      <c r="S16" s="1044"/>
+      <c r="S16" s="999"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
@@ -15950,7 +15992,7 @@
       <c r="P24" s="1115"/>
       <c r="Q24" s="1115"/>
       <c r="R24" s="1115"/>
-      <c r="S24" s="1009"/>
+      <c r="S24" s="1018"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C25" s="173" t="s">
@@ -16000,7 +16042,7 @@
       <c r="P26" s="1102"/>
       <c r="Q26" s="1102"/>
       <c r="R26" s="1102"/>
-      <c r="S26" s="1042"/>
+      <c r="S26" s="997"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
@@ -16021,7 +16063,7 @@
       <c r="P27" s="1104"/>
       <c r="Q27" s="1104"/>
       <c r="R27" s="1104"/>
-      <c r="S27" s="1044"/>
+      <c r="S27" s="999"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="K29" t="s">
@@ -19813,15 +19855,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7213ADEA-A0ED-4772-BDDF-F43C00D4300A}">
-  <dimension ref="B3:AK69"/>
+  <dimension ref="A3:AK69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:T68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="5.85546875" customWidth="1"/>
     <col min="5" max="6" width="6.85546875" customWidth="1"/>
     <col min="7" max="7" width="5.28515625" bestFit="1" customWidth="1"/>
@@ -19838,42 +19880,42 @@
       <c r="L3" s="115" t="s">
         <v>112</v>
       </c>
-      <c r="M3" s="995">
+      <c r="M3" s="996">
         <v>0</v>
       </c>
-      <c r="N3" s="1009"/>
-      <c r="O3" s="995" t="s">
+      <c r="N3" s="1018"/>
+      <c r="O3" s="996" t="s">
         <v>119</v>
       </c>
-      <c r="P3" s="996"/>
-      <c r="Q3" s="996"/>
-      <c r="R3" s="996"/>
-      <c r="S3" s="996"/>
-      <c r="T3" s="997"/>
-      <c r="U3" s="1007">
+      <c r="P3" s="1006"/>
+      <c r="Q3" s="1006"/>
+      <c r="R3" s="1006"/>
+      <c r="S3" s="1006"/>
+      <c r="T3" s="1007"/>
+      <c r="U3" s="979">
         <v>2</v>
       </c>
-      <c r="V3" s="1007">
+      <c r="V3" s="979">
         <v>3</v>
       </c>
-      <c r="W3" s="995">
+      <c r="W3" s="996">
         <v>4</v>
       </c>
-      <c r="X3" s="1042"/>
-      <c r="Y3" s="1007">
+      <c r="X3" s="997"/>
+      <c r="Y3" s="979">
         <v>5</v>
       </c>
-      <c r="AC3" s="986" t="s">
+      <c r="AC3" s="1047" t="s">
         <v>1438</v>
       </c>
-      <c r="AD3" s="986"/>
-      <c r="AE3" s="986"/>
-      <c r="AF3" s="986"/>
-      <c r="AG3" s="986"/>
-      <c r="AH3" s="986"/>
-      <c r="AI3" s="986"/>
-      <c r="AJ3" s="986"/>
-      <c r="AK3" s="986"/>
+      <c r="AD3" s="1047"/>
+      <c r="AE3" s="1047"/>
+      <c r="AF3" s="1047"/>
+      <c r="AG3" s="1047"/>
+      <c r="AH3" s="1047"/>
+      <c r="AI3" s="1047"/>
+      <c r="AJ3" s="1047"/>
+      <c r="AK3" s="1047"/>
     </row>
     <row r="4" spans="12:37" x14ac:dyDescent="0.25">
       <c r="L4" s="114" t="s">
@@ -19899,40 +19941,40 @@
       <c r="T4" s="142" t="s">
         <v>88</v>
       </c>
-      <c r="U4" s="1008"/>
-      <c r="V4" s="1008"/>
-      <c r="W4" s="1043" t="s">
+      <c r="U4" s="1017"/>
+      <c r="V4" s="1017"/>
+      <c r="W4" s="998" t="s">
         <v>320</v>
       </c>
-      <c r="X4" s="1044"/>
-      <c r="Y4" s="1026"/>
+      <c r="X4" s="999"/>
+      <c r="Y4" s="980"/>
       <c r="AB4" s="898"/>
-      <c r="AC4" s="979" t="s">
+      <c r="AC4" s="1040" t="s">
         <v>1389</v>
       </c>
-      <c r="AD4" s="980"/>
-      <c r="AE4" s="981" t="s">
+      <c r="AD4" s="1041"/>
+      <c r="AE4" s="1042" t="s">
         <v>1388</v>
       </c>
-      <c r="AF4" s="982"/>
-      <c r="AG4" s="979" t="s">
+      <c r="AF4" s="1043"/>
+      <c r="AG4" s="1040" t="s">
         <v>1390</v>
       </c>
-      <c r="AH4" s="982"/>
-      <c r="AI4" s="983" t="s">
+      <c r="AH4" s="1043"/>
+      <c r="AI4" s="1044" t="s">
         <v>1437</v>
       </c>
-      <c r="AJ4" s="984"/>
-      <c r="AK4" s="985"/>
+      <c r="AJ4" s="1045"/>
+      <c r="AK4" s="1046"/>
     </row>
     <row r="5" spans="12:37" x14ac:dyDescent="0.25">
-      <c r="L5" s="987" t="s">
+      <c r="L5" s="1035" t="s">
         <v>111</v>
       </c>
-      <c r="M5" s="992" t="s">
+      <c r="M5" s="1003" t="s">
         <v>113</v>
       </c>
-      <c r="N5" s="1010" t="s">
+      <c r="N5" s="1019" t="s">
         <v>324</v>
       </c>
       <c r="O5" s="61"/>
@@ -19945,19 +19987,19 @@
       <c r="T5" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="U5" s="1001" t="s">
+      <c r="U5" s="1011" t="s">
         <v>470</v>
       </c>
-      <c r="V5" s="1004" t="s">
+      <c r="V5" s="1014" t="s">
         <v>323</v>
       </c>
-      <c r="W5" s="1036" t="s">
+      <c r="W5" s="990" t="s">
         <v>311</v>
       </c>
-      <c r="X5" s="1040" t="s">
+      <c r="X5" s="994" t="s">
         <v>312</v>
       </c>
-      <c r="Y5" s="1027" t="s">
+      <c r="Y5" s="981" t="s">
         <v>114</v>
       </c>
       <c r="AB5" s="911">
@@ -19990,9 +20032,9 @@
       <c r="AK5" s="902"/>
     </row>
     <row r="6" spans="12:37" x14ac:dyDescent="0.25">
-      <c r="L6" s="988"/>
-      <c r="M6" s="993"/>
-      <c r="N6" s="1011"/>
+      <c r="L6" s="1036"/>
+      <c r="M6" s="1004"/>
+      <c r="N6" s="1020"/>
       <c r="O6" s="64"/>
       <c r="P6" s="65"/>
       <c r="Q6" s="65"/>
@@ -20001,11 +20043,11 @@
       <c r="T6" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U6" s="1002"/>
-      <c r="V6" s="1005"/>
-      <c r="W6" s="1037"/>
-      <c r="X6" s="1041"/>
-      <c r="Y6" s="1028"/>
+      <c r="U6" s="1012"/>
+      <c r="V6" s="1015"/>
+      <c r="W6" s="991"/>
+      <c r="X6" s="995"/>
+      <c r="Y6" s="982"/>
       <c r="AB6" s="279">
         <v>2</v>
       </c>
@@ -20036,9 +20078,9 @@
       <c r="AK6" s="215"/>
     </row>
     <row r="7" spans="12:37" x14ac:dyDescent="0.25">
-      <c r="L7" s="988"/>
-      <c r="M7" s="993"/>
-      <c r="N7" s="1012"/>
+      <c r="L7" s="1036"/>
+      <c r="M7" s="1004"/>
+      <c r="N7" s="1021"/>
       <c r="O7" s="64"/>
       <c r="P7" s="65"/>
       <c r="Q7" s="65"/>
@@ -20047,13 +20089,13 @@
       <c r="T7" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U7" s="1002"/>
-      <c r="V7" s="1005"/>
-      <c r="W7" s="1038"/>
-      <c r="X7" s="1045" t="s">
+      <c r="U7" s="1012"/>
+      <c r="V7" s="1015"/>
+      <c r="W7" s="992"/>
+      <c r="X7" s="1000" t="s">
         <v>317</v>
       </c>
-      <c r="Y7" s="1028"/>
+      <c r="Y7" s="982"/>
       <c r="AB7" s="279">
         <v>3</v>
       </c>
@@ -20084,9 +20126,9 @@
       <c r="AK7" s="215"/>
     </row>
     <row r="8" spans="12:37" x14ac:dyDescent="0.25">
-      <c r="L8" s="989"/>
-      <c r="M8" s="993"/>
-      <c r="N8" s="1015" t="s">
+      <c r="L8" s="1037"/>
+      <c r="M8" s="1004"/>
+      <c r="N8" s="1024" t="s">
         <v>309</v>
       </c>
       <c r="O8" s="108"/>
@@ -20099,11 +20141,11 @@
       <c r="T8" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U8" s="1002"/>
-      <c r="V8" s="1005"/>
-      <c r="W8" s="1038"/>
-      <c r="X8" s="1046"/>
-      <c r="Y8" s="1028"/>
+      <c r="U8" s="1012"/>
+      <c r="V8" s="1015"/>
+      <c r="W8" s="992"/>
+      <c r="X8" s="1001"/>
+      <c r="Y8" s="982"/>
       <c r="AB8" s="279">
         <v>4</v>
       </c>
@@ -20134,11 +20176,11 @@
       <c r="AK8" s="215"/>
     </row>
     <row r="9" spans="12:37" x14ac:dyDescent="0.25">
-      <c r="L9" s="987" t="s">
+      <c r="L9" s="1035" t="s">
         <v>110</v>
       </c>
-      <c r="M9" s="993"/>
-      <c r="N9" s="1016"/>
+      <c r="M9" s="1004"/>
+      <c r="N9" s="1025"/>
       <c r="O9" s="61"/>
       <c r="P9" s="62"/>
       <c r="Q9" s="62"/>
@@ -20149,13 +20191,13 @@
       <c r="T9" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U9" s="1002"/>
-      <c r="V9" s="1005"/>
-      <c r="W9" s="1038"/>
-      <c r="X9" s="1041" t="s">
+      <c r="U9" s="1012"/>
+      <c r="V9" s="1015"/>
+      <c r="W9" s="992"/>
+      <c r="X9" s="995" t="s">
         <v>316</v>
       </c>
-      <c r="Y9" s="1028"/>
+      <c r="Y9" s="982"/>
       <c r="AB9" s="279">
         <v>5</v>
       </c>
@@ -20188,9 +20230,9 @@
       </c>
     </row>
     <row r="10" spans="12:37" x14ac:dyDescent="0.25">
-      <c r="L10" s="988"/>
-      <c r="M10" s="993"/>
-      <c r="N10" s="1016"/>
+      <c r="L10" s="1036"/>
+      <c r="M10" s="1004"/>
+      <c r="N10" s="1025"/>
       <c r="O10" s="64"/>
       <c r="P10" s="65"/>
       <c r="Q10" s="65"/>
@@ -20199,11 +20241,11 @@
       <c r="T10" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U10" s="1002"/>
-      <c r="V10" s="1005"/>
-      <c r="W10" s="1038"/>
-      <c r="X10" s="1047"/>
-      <c r="Y10" s="1028"/>
+      <c r="U10" s="1012"/>
+      <c r="V10" s="1015"/>
+      <c r="W10" s="992"/>
+      <c r="X10" s="1002"/>
+      <c r="Y10" s="982"/>
       <c r="AB10" s="279">
         <v>6</v>
       </c>
@@ -20234,9 +20276,9 @@
       <c r="AK10" s="917"/>
     </row>
     <row r="11" spans="12:37" x14ac:dyDescent="0.25">
-      <c r="L11" s="988"/>
-      <c r="M11" s="993"/>
-      <c r="N11" s="1017"/>
+      <c r="L11" s="1036"/>
+      <c r="M11" s="1004"/>
+      <c r="N11" s="1026"/>
       <c r="O11" s="64"/>
       <c r="P11" s="65"/>
       <c r="Q11" s="65"/>
@@ -20245,13 +20287,13 @@
       <c r="T11" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U11" s="1002"/>
-      <c r="V11" s="1005"/>
-      <c r="W11" s="1038"/>
-      <c r="X11" s="1045" t="s">
+      <c r="U11" s="1012"/>
+      <c r="V11" s="1015"/>
+      <c r="W11" s="992"/>
+      <c r="X11" s="1000" t="s">
         <v>315</v>
       </c>
-      <c r="Y11" s="1028"/>
+      <c r="Y11" s="982"/>
       <c r="AB11" s="279">
         <v>7</v>
       </c>
@@ -20282,9 +20324,9 @@
       <c r="AK11" s="215"/>
     </row>
     <row r="12" spans="12:37" x14ac:dyDescent="0.25">
-      <c r="L12" s="989"/>
-      <c r="M12" s="993"/>
-      <c r="N12" s="1013" t="s">
+      <c r="L12" s="1037"/>
+      <c r="M12" s="1004"/>
+      <c r="N12" s="1022" t="s">
         <v>308</v>
       </c>
       <c r="O12" s="80"/>
@@ -20297,11 +20339,11 @@
       <c r="T12" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U12" s="1002"/>
-      <c r="V12" s="1005"/>
-      <c r="W12" s="1038"/>
-      <c r="X12" s="1046"/>
-      <c r="Y12" s="1028"/>
+      <c r="U12" s="1012"/>
+      <c r="V12" s="1015"/>
+      <c r="W12" s="992"/>
+      <c r="X12" s="1001"/>
+      <c r="Y12" s="982"/>
       <c r="Z12" s="201"/>
       <c r="AB12" s="279">
         <v>8</v>
@@ -20333,11 +20375,11 @@
       <c r="AK12" s="215"/>
     </row>
     <row r="13" spans="12:37" x14ac:dyDescent="0.25">
-      <c r="L13" s="987" t="s">
+      <c r="L13" s="1035" t="s">
         <v>109</v>
       </c>
-      <c r="M13" s="993"/>
-      <c r="N13" s="1014"/>
+      <c r="M13" s="1004"/>
+      <c r="N13" s="1023"/>
       <c r="O13" s="106"/>
       <c r="P13" s="107"/>
       <c r="Q13" s="107"/>
@@ -20348,13 +20390,13 @@
       <c r="T13" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U13" s="1002"/>
-      <c r="V13" s="1005"/>
-      <c r="W13" s="1038"/>
-      <c r="X13" s="1041" t="s">
+      <c r="U13" s="1012"/>
+      <c r="V13" s="1015"/>
+      <c r="W13" s="992"/>
+      <c r="X13" s="995" t="s">
         <v>314</v>
       </c>
-      <c r="Y13" s="1028"/>
+      <c r="Y13" s="982"/>
       <c r="Z13" s="202"/>
       <c r="AB13" s="279">
         <v>9</v>
@@ -20386,8 +20428,8 @@
       <c r="AK13" s="215"/>
     </row>
     <row r="14" spans="12:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L14" s="988"/>
-      <c r="M14" s="993"/>
+      <c r="L14" s="1036"/>
+      <c r="M14" s="1004"/>
       <c r="N14" s="203"/>
       <c r="O14" s="64"/>
       <c r="P14" s="65"/>
@@ -20397,11 +20439,11 @@
       <c r="T14" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U14" s="1002"/>
-      <c r="V14" s="1005"/>
-      <c r="W14" s="1038"/>
-      <c r="X14" s="1047"/>
-      <c r="Y14" s="1028"/>
+      <c r="U14" s="1012"/>
+      <c r="V14" s="1015"/>
+      <c r="W14" s="992"/>
+      <c r="X14" s="1002"/>
+      <c r="Y14" s="982"/>
       <c r="Z14" s="202"/>
       <c r="AB14" s="279">
         <v>10</v>
@@ -20433,8 +20475,8 @@
       <c r="AK14" s="215"/>
     </row>
     <row r="15" spans="12:37" x14ac:dyDescent="0.25">
-      <c r="L15" s="988"/>
-      <c r="M15" s="993"/>
+      <c r="L15" s="1036"/>
+      <c r="M15" s="1004"/>
       <c r="N15" s="204"/>
       <c r="O15" s="64"/>
       <c r="P15" s="65"/>
@@ -20444,13 +20486,13 @@
       <c r="T15" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U15" s="1002"/>
-      <c r="V15" s="1005"/>
-      <c r="W15" s="1038"/>
-      <c r="X15" s="1045" t="s">
+      <c r="U15" s="1012"/>
+      <c r="V15" s="1015"/>
+      <c r="W15" s="992"/>
+      <c r="X15" s="1000" t="s">
         <v>313</v>
       </c>
-      <c r="Y15" s="1028"/>
+      <c r="Y15" s="982"/>
       <c r="Z15" s="202"/>
       <c r="AB15" s="279">
         <v>11</v>
@@ -20482,8 +20524,8 @@
       <c r="AK15" s="215"/>
     </row>
     <row r="16" spans="12:37" x14ac:dyDescent="0.25">
-      <c r="L16" s="989"/>
-      <c r="M16" s="993"/>
+      <c r="L16" s="1037"/>
+      <c r="M16" s="1004"/>
       <c r="N16" s="204"/>
       <c r="O16" s="108"/>
       <c r="P16" s="109"/>
@@ -20495,11 +20537,11 @@
       <c r="T16" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U16" s="1002"/>
-      <c r="V16" s="1005"/>
-      <c r="W16" s="1039"/>
-      <c r="X16" s="1046"/>
-      <c r="Y16" s="1028"/>
+      <c r="U16" s="1012"/>
+      <c r="V16" s="1015"/>
+      <c r="W16" s="993"/>
+      <c r="X16" s="1001"/>
+      <c r="Y16" s="982"/>
       <c r="Z16" s="202"/>
       <c r="AB16" s="279">
         <v>12</v>
@@ -20531,10 +20573,10 @@
       <c r="AK16" s="215"/>
     </row>
     <row r="17" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="L17" s="987" t="s">
+      <c r="L17" s="1035" t="s">
         <v>108</v>
       </c>
-      <c r="M17" s="993"/>
+      <c r="M17" s="1004"/>
       <c r="N17" s="204"/>
       <c r="O17" s="61"/>
       <c r="P17" s="62"/>
@@ -20546,13 +20588,13 @@
       <c r="T17" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U17" s="1002"/>
-      <c r="V17" s="1005"/>
-      <c r="W17" s="1030" t="s">
+      <c r="U17" s="1012"/>
+      <c r="V17" s="1015"/>
+      <c r="W17" s="984" t="s">
         <v>318</v>
       </c>
-      <c r="X17" s="1031"/>
-      <c r="Y17" s="1028"/>
+      <c r="X17" s="985"/>
+      <c r="Y17" s="982"/>
       <c r="Z17" s="202"/>
       <c r="AB17" s="279">
         <v>13</v>
@@ -20584,8 +20626,8 @@
       <c r="AK17" s="215"/>
     </row>
     <row r="18" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="L18" s="988"/>
-      <c r="M18" s="993"/>
+      <c r="L18" s="1036"/>
+      <c r="M18" s="1004"/>
       <c r="N18" s="204"/>
       <c r="O18" s="64"/>
       <c r="P18" s="65"/>
@@ -20595,11 +20637,11 @@
       <c r="T18" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U18" s="1002"/>
-      <c r="V18" s="1005"/>
-      <c r="W18" s="1032"/>
-      <c r="X18" s="1033"/>
-      <c r="Y18" s="1028"/>
+      <c r="U18" s="1012"/>
+      <c r="V18" s="1015"/>
+      <c r="W18" s="986"/>
+      <c r="X18" s="987"/>
+      <c r="Y18" s="982"/>
       <c r="Z18" s="202"/>
       <c r="AB18" s="279">
         <v>14</v>
@@ -20631,8 +20673,8 @@
       <c r="AK18" s="215"/>
     </row>
     <row r="19" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="L19" s="988"/>
-      <c r="M19" s="993"/>
+      <c r="L19" s="1036"/>
+      <c r="M19" s="1004"/>
       <c r="N19" s="204"/>
       <c r="O19" s="64"/>
       <c r="P19" s="65"/>
@@ -20642,11 +20684,11 @@
       <c r="T19" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U19" s="1002"/>
-      <c r="V19" s="1005"/>
-      <c r="W19" s="1032"/>
-      <c r="X19" s="1033"/>
-      <c r="Y19" s="1028"/>
+      <c r="U19" s="1012"/>
+      <c r="V19" s="1015"/>
+      <c r="W19" s="986"/>
+      <c r="X19" s="987"/>
+      <c r="Y19" s="982"/>
       <c r="Z19" s="202"/>
       <c r="AB19" s="279">
         <v>15</v>
@@ -20678,8 +20720,8 @@
       <c r="AK19" s="207"/>
     </row>
     <row r="20" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="L20" s="989"/>
-      <c r="M20" s="993"/>
+      <c r="L20" s="1037"/>
+      <c r="M20" s="1004"/>
       <c r="N20" s="204"/>
       <c r="O20" s="80" t="s">
         <v>73</v>
@@ -20695,11 +20737,11 @@
       <c r="T20" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="U20" s="1002"/>
-      <c r="V20" s="1005"/>
-      <c r="W20" s="1032"/>
-      <c r="X20" s="1033"/>
-      <c r="Y20" s="1028"/>
+      <c r="U20" s="1012"/>
+      <c r="V20" s="1015"/>
+      <c r="W20" s="986"/>
+      <c r="X20" s="987"/>
+      <c r="Y20" s="982"/>
       <c r="Z20" s="202"/>
       <c r="AB20" s="279">
         <v>16</v>
@@ -20731,10 +20773,10 @@
       <c r="AK20" s="207"/>
     </row>
     <row r="21" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L21" s="987" t="s">
+      <c r="L21" s="1035" t="s">
         <v>107</v>
       </c>
-      <c r="M21" s="993"/>
+      <c r="M21" s="1004"/>
       <c r="N21" s="204"/>
       <c r="O21" s="78"/>
       <c r="P21" s="79"/>
@@ -20746,11 +20788,11 @@
       <c r="T21" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="U21" s="1002"/>
-      <c r="V21" s="1005"/>
-      <c r="W21" s="1032"/>
-      <c r="X21" s="1033"/>
-      <c r="Y21" s="1028"/>
+      <c r="U21" s="1012"/>
+      <c r="V21" s="1015"/>
+      <c r="W21" s="986"/>
+      <c r="X21" s="987"/>
+      <c r="Y21" s="982"/>
       <c r="Z21" s="202"/>
       <c r="AB21" s="279">
         <v>17</v>
@@ -20806,8 +20848,8 @@
       <c r="I22" s="193">
         <v>7759</v>
       </c>
-      <c r="L22" s="988"/>
-      <c r="M22" s="993"/>
+      <c r="L22" s="1036"/>
+      <c r="M22" s="1004"/>
       <c r="N22" s="204"/>
       <c r="O22" s="64"/>
       <c r="P22" s="65"/>
@@ -20817,11 +20859,11 @@
       <c r="T22" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U22" s="1002"/>
-      <c r="V22" s="1005"/>
-      <c r="W22" s="1032"/>
-      <c r="X22" s="1033"/>
-      <c r="Y22" s="1028"/>
+      <c r="U22" s="1012"/>
+      <c r="V22" s="1015"/>
+      <c r="W22" s="986"/>
+      <c r="X22" s="987"/>
+      <c r="Y22" s="982"/>
       <c r="AB22" s="279">
         <v>18</v>
       </c>
@@ -20855,8 +20897,8 @@
       <c r="D23" s="173" t="s">
         <v>60</v>
       </c>
-      <c r="L23" s="988"/>
-      <c r="M23" s="993"/>
+      <c r="L23" s="1036"/>
+      <c r="M23" s="1004"/>
       <c r="N23" s="204"/>
       <c r="O23" s="80"/>
       <c r="P23" s="81"/>
@@ -20866,11 +20908,11 @@
       <c r="T23" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U23" s="1002"/>
-      <c r="V23" s="1005"/>
-      <c r="W23" s="1032"/>
-      <c r="X23" s="1033"/>
-      <c r="Y23" s="1028"/>
+      <c r="U23" s="1012"/>
+      <c r="V23" s="1015"/>
+      <c r="W23" s="986"/>
+      <c r="X23" s="987"/>
+      <c r="Y23" s="982"/>
       <c r="AB23" s="279">
         <v>19</v>
       </c>
@@ -20924,8 +20966,8 @@
         <v>302</v>
       </c>
       <c r="J24" s="173"/>
-      <c r="L24" s="989"/>
-      <c r="M24" s="993"/>
+      <c r="L24" s="1037"/>
+      <c r="M24" s="1004"/>
       <c r="N24" s="204"/>
       <c r="O24" s="108"/>
       <c r="P24" s="109"/>
@@ -20937,11 +20979,11 @@
       <c r="T24" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U24" s="1002"/>
-      <c r="V24" s="1005"/>
-      <c r="W24" s="1032"/>
-      <c r="X24" s="1033"/>
-      <c r="Y24" s="1028"/>
+      <c r="U24" s="1012"/>
+      <c r="V24" s="1015"/>
+      <c r="W24" s="986"/>
+      <c r="X24" s="987"/>
+      <c r="Y24" s="982"/>
       <c r="AB24" s="279">
         <v>20</v>
       </c>
@@ -20995,10 +21037,10 @@
         <v>30</v>
       </c>
       <c r="J25" s="288"/>
-      <c r="L25" s="987" t="s">
+      <c r="L25" s="1035" t="s">
         <v>106</v>
       </c>
-      <c r="M25" s="993"/>
+      <c r="M25" s="1004"/>
       <c r="N25" s="204"/>
       <c r="O25" s="61"/>
       <c r="P25" s="62"/>
@@ -21010,11 +21052,11 @@
       <c r="T25" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U25" s="1002"/>
-      <c r="V25" s="1005"/>
-      <c r="W25" s="1032"/>
-      <c r="X25" s="1033"/>
-      <c r="Y25" s="1028"/>
+      <c r="U25" s="1012"/>
+      <c r="V25" s="1015"/>
+      <c r="W25" s="986"/>
+      <c r="X25" s="987"/>
+      <c r="Y25" s="982"/>
       <c r="AB25" s="912">
         <v>21</v>
       </c>
@@ -21033,9 +21075,9 @@
       <c r="AK25" s="210"/>
     </row>
     <row r="26" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="L26" s="988"/>
-      <c r="M26" s="993"/>
-      <c r="N26" s="1023" t="s">
+      <c r="L26" s="1036"/>
+      <c r="M26" s="1004"/>
+      <c r="N26" s="1032" t="s">
         <v>327</v>
       </c>
       <c r="O26" s="64"/>
@@ -21046,17 +21088,17 @@
       <c r="T26" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U26" s="1002"/>
-      <c r="V26" s="1005"/>
-      <c r="W26" s="1032"/>
-      <c r="X26" s="1033"/>
-      <c r="Y26" s="1028"/>
+      <c r="U26" s="1012"/>
+      <c r="V26" s="1015"/>
+      <c r="W26" s="986"/>
+      <c r="X26" s="987"/>
+      <c r="Y26" s="982"/>
     </row>
     <row r="27" spans="2:37" x14ac:dyDescent="0.25">
       <c r="H27" s="173"/>
-      <c r="L27" s="988"/>
-      <c r="M27" s="993"/>
-      <c r="N27" s="1024"/>
+      <c r="L27" s="1036"/>
+      <c r="M27" s="1004"/>
+      <c r="N27" s="1033"/>
       <c r="O27" s="80"/>
       <c r="P27" s="81"/>
       <c r="Q27" s="81"/>
@@ -21065,17 +21107,17 @@
       <c r="T27" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U27" s="1002"/>
-      <c r="V27" s="1005"/>
-      <c r="W27" s="1032"/>
-      <c r="X27" s="1033"/>
-      <c r="Y27" s="1028"/>
+      <c r="U27" s="1012"/>
+      <c r="V27" s="1015"/>
+      <c r="W27" s="986"/>
+      <c r="X27" s="987"/>
+      <c r="Y27" s="982"/>
     </row>
     <row r="28" spans="2:37" x14ac:dyDescent="0.25">
       <c r="H28" s="173"/>
-      <c r="L28" s="989"/>
-      <c r="M28" s="993"/>
-      <c r="N28" s="1024"/>
+      <c r="L28" s="1037"/>
+      <c r="M28" s="1004"/>
+      <c r="N28" s="1033"/>
       <c r="O28" s="80"/>
       <c r="P28" s="81"/>
       <c r="Q28" s="82" t="s">
@@ -21086,18 +21128,18 @@
       <c r="T28" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U28" s="1002"/>
-      <c r="V28" s="1005"/>
-      <c r="W28" s="1032"/>
-      <c r="X28" s="1033"/>
-      <c r="Y28" s="1028"/>
+      <c r="U28" s="1012"/>
+      <c r="V28" s="1015"/>
+      <c r="W28" s="986"/>
+      <c r="X28" s="987"/>
+      <c r="Y28" s="982"/>
     </row>
     <row r="29" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="L29" s="987" t="s">
+      <c r="L29" s="1035" t="s">
         <v>105</v>
       </c>
-      <c r="M29" s="993"/>
-      <c r="N29" s="1024"/>
+      <c r="M29" s="1004"/>
+      <c r="N29" s="1033"/>
       <c r="O29" s="106"/>
       <c r="P29" s="107"/>
       <c r="Q29" s="107"/>
@@ -21108,16 +21150,16 @@
       <c r="T29" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U29" s="1002"/>
-      <c r="V29" s="1005"/>
-      <c r="W29" s="1032"/>
-      <c r="X29" s="1033"/>
-      <c r="Y29" s="1028"/>
+      <c r="U29" s="1012"/>
+      <c r="V29" s="1015"/>
+      <c r="W29" s="986"/>
+      <c r="X29" s="987"/>
+      <c r="Y29" s="982"/>
     </row>
     <row r="30" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="L30" s="988"/>
-      <c r="M30" s="993"/>
-      <c r="N30" s="1025"/>
+      <c r="L30" s="1036"/>
+      <c r="M30" s="1004"/>
+      <c r="N30" s="1034"/>
       <c r="O30" s="64"/>
       <c r="P30" s="65"/>
       <c r="Q30" s="65"/>
@@ -21126,16 +21168,16 @@
       <c r="T30" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U30" s="1002"/>
-      <c r="V30" s="1005"/>
-      <c r="W30" s="1032"/>
-      <c r="X30" s="1033"/>
-      <c r="Y30" s="1028"/>
+      <c r="U30" s="1012"/>
+      <c r="V30" s="1015"/>
+      <c r="W30" s="986"/>
+      <c r="X30" s="987"/>
+      <c r="Y30" s="982"/>
     </row>
     <row r="31" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="L31" s="988"/>
-      <c r="M31" s="993"/>
-      <c r="N31" s="1022" t="s">
+      <c r="L31" s="1036"/>
+      <c r="M31" s="1004"/>
+      <c r="N31" s="1031" t="s">
         <v>326</v>
       </c>
       <c r="O31" s="64"/>
@@ -21146,16 +21188,16 @@
       <c r="T31" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U31" s="1002"/>
-      <c r="V31" s="1005"/>
-      <c r="W31" s="1032"/>
-      <c r="X31" s="1033"/>
-      <c r="Y31" s="1028"/>
+      <c r="U31" s="1012"/>
+      <c r="V31" s="1015"/>
+      <c r="W31" s="986"/>
+      <c r="X31" s="987"/>
+      <c r="Y31" s="982"/>
     </row>
     <row r="32" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="L32" s="989"/>
-      <c r="M32" s="993"/>
-      <c r="N32" s="1016"/>
+      <c r="L32" s="1037"/>
+      <c r="M32" s="1004"/>
+      <c r="N32" s="1025"/>
       <c r="O32" s="110"/>
       <c r="P32" s="111"/>
       <c r="Q32" s="112" t="s">
@@ -21166,18 +21208,18 @@
       <c r="T32" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U32" s="1002"/>
-      <c r="V32" s="1005"/>
-      <c r="W32" s="1032"/>
-      <c r="X32" s="1033"/>
-      <c r="Y32" s="1028"/>
-    </row>
-    <row r="33" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L33" s="987" t="s">
+      <c r="U32" s="1012"/>
+      <c r="V32" s="1015"/>
+      <c r="W32" s="986"/>
+      <c r="X32" s="987"/>
+      <c r="Y32" s="982"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L33" s="1035" t="s">
         <v>104</v>
       </c>
-      <c r="M33" s="993"/>
-      <c r="N33" s="1016"/>
+      <c r="M33" s="1004"/>
+      <c r="N33" s="1025"/>
       <c r="O33" s="61"/>
       <c r="P33" s="62"/>
       <c r="Q33" s="62"/>
@@ -21188,16 +21230,16 @@
       <c r="T33" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U33" s="1002"/>
-      <c r="V33" s="1005"/>
-      <c r="W33" s="1032"/>
-      <c r="X33" s="1033"/>
-      <c r="Y33" s="1028"/>
-    </row>
-    <row r="34" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L34" s="988"/>
-      <c r="M34" s="993"/>
-      <c r="N34" s="1017"/>
+      <c r="U33" s="1012"/>
+      <c r="V33" s="1015"/>
+      <c r="W33" s="986"/>
+      <c r="X33" s="987"/>
+      <c r="Y33" s="982"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L34" s="1036"/>
+      <c r="M34" s="1004"/>
+      <c r="N34" s="1026"/>
       <c r="O34" s="64"/>
       <c r="P34" s="65"/>
       <c r="Q34" s="65"/>
@@ -21206,16 +21248,19 @@
       <c r="T34" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U34" s="1002"/>
-      <c r="V34" s="1005"/>
-      <c r="W34" s="1032"/>
-      <c r="X34" s="1033"/>
-      <c r="Y34" s="1028"/>
-    </row>
-    <row r="35" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L35" s="988"/>
-      <c r="M35" s="993"/>
-      <c r="N35" s="1021" t="s">
+      <c r="U34" s="1012"/>
+      <c r="V34" s="1015"/>
+      <c r="W34" s="986"/>
+      <c r="X34" s="987"/>
+      <c r="Y34" s="982"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1520</v>
+      </c>
+      <c r="L35" s="1036"/>
+      <c r="M35" s="1004"/>
+      <c r="N35" s="1030" t="s">
         <v>325</v>
       </c>
       <c r="O35" s="64"/>
@@ -21226,17 +21271,20 @@
       <c r="T35" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U35" s="1002"/>
-      <c r="V35" s="1005"/>
-      <c r="W35" s="1032"/>
-      <c r="X35" s="1033"/>
-      <c r="Y35" s="1028"/>
+      <c r="U35" s="1012"/>
+      <c r="V35" s="1015"/>
+      <c r="W35" s="986"/>
+      <c r="X35" s="987"/>
+      <c r="Y35" s="982"/>
       <c r="Z35" s="201"/>
     </row>
-    <row r="36" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L36" s="989"/>
-      <c r="M36" s="993"/>
-      <c r="N36" s="1014"/>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1523</v>
+      </c>
+      <c r="L36" s="1037"/>
+      <c r="M36" s="1004"/>
+      <c r="N36" s="1023"/>
       <c r="O36" s="67" t="s">
         <v>73</v>
       </c>
@@ -21251,19 +21299,22 @@
       <c r="T36" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="U36" s="1002"/>
-      <c r="V36" s="1005"/>
-      <c r="W36" s="1032"/>
-      <c r="X36" s="1033"/>
-      <c r="Y36" s="1028"/>
+      <c r="U36" s="1012"/>
+      <c r="V36" s="1015"/>
+      <c r="W36" s="986"/>
+      <c r="X36" s="987"/>
+      <c r="Y36" s="982"/>
       <c r="Z36" s="202"/>
     </row>
-    <row r="37" spans="12:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L37" s="987" t="s">
+    <row r="37" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1522</v>
+      </c>
+      <c r="L37" s="1035" t="s">
         <v>103</v>
       </c>
-      <c r="M37" s="993"/>
-      <c r="N37" s="1018" t="s">
+      <c r="M37" s="1004"/>
+      <c r="N37" s="1027" t="s">
         <v>310</v>
       </c>
       <c r="O37" s="70"/>
@@ -21280,17 +21331,17 @@
       <c r="T37" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="U37" s="1002"/>
-      <c r="V37" s="1005"/>
-      <c r="W37" s="1032"/>
-      <c r="X37" s="1033"/>
-      <c r="Y37" s="1028"/>
+      <c r="U37" s="1012"/>
+      <c r="V37" s="1015"/>
+      <c r="W37" s="986"/>
+      <c r="X37" s="987"/>
+      <c r="Y37" s="982"/>
       <c r="Z37" s="202"/>
     </row>
-    <row r="38" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L38" s="988"/>
-      <c r="M38" s="993"/>
-      <c r="N38" s="1019"/>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L38" s="1036"/>
+      <c r="M38" s="1004"/>
+      <c r="N38" s="1028"/>
       <c r="O38" s="72"/>
       <c r="P38" s="73"/>
       <c r="Q38" s="74" t="s">
@@ -21303,17 +21354,20 @@
       <c r="T38" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U38" s="1002"/>
-      <c r="V38" s="1005"/>
-      <c r="W38" s="1032"/>
-      <c r="X38" s="1033"/>
-      <c r="Y38" s="1028"/>
+      <c r="U38" s="1012"/>
+      <c r="V38" s="1015"/>
+      <c r="W38" s="986"/>
+      <c r="X38" s="987"/>
+      <c r="Y38" s="982"/>
       <c r="Z38" s="202"/>
     </row>
-    <row r="39" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L39" s="988"/>
-      <c r="M39" s="993"/>
-      <c r="N39" s="1019"/>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1526</v>
+      </c>
+      <c r="L39" s="1036"/>
+      <c r="M39" s="1004"/>
+      <c r="N39" s="1028"/>
       <c r="O39" s="72"/>
       <c r="P39" s="73"/>
       <c r="Q39" s="74" t="s">
@@ -21326,16 +21380,19 @@
       <c r="T39" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U39" s="1002"/>
-      <c r="V39" s="1005"/>
-      <c r="W39" s="1032"/>
-      <c r="X39" s="1033"/>
-      <c r="Y39" s="1028"/>
-    </row>
-    <row r="40" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L40" s="989"/>
-      <c r="M40" s="993"/>
-      <c r="N40" s="1019"/>
+      <c r="U39" s="1012"/>
+      <c r="V39" s="1015"/>
+      <c r="W39" s="986"/>
+      <c r="X39" s="987"/>
+      <c r="Y39" s="982"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1527</v>
+      </c>
+      <c r="L40" s="1037"/>
+      <c r="M40" s="1004"/>
+      <c r="N40" s="1028"/>
       <c r="O40" s="96"/>
       <c r="P40" s="97"/>
       <c r="Q40" s="169" t="s">
@@ -21350,19 +21407,19 @@
       <c r="T40" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U40" s="1002"/>
-      <c r="V40" s="1005"/>
-      <c r="W40" s="1032"/>
-      <c r="X40" s="1033"/>
-      <c r="Y40" s="1028"/>
+      <c r="U40" s="1012"/>
+      <c r="V40" s="1015"/>
+      <c r="W40" s="986"/>
+      <c r="X40" s="987"/>
+      <c r="Y40" s="982"/>
       <c r="Z40" s="201"/>
     </row>
-    <row r="41" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L41" s="987" t="s">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L41" s="1035" t="s">
         <v>102</v>
       </c>
-      <c r="M41" s="993"/>
-      <c r="N41" s="1019"/>
+      <c r="M41" s="1004"/>
+      <c r="N41" s="1028"/>
       <c r="O41" s="101"/>
       <c r="P41" s="102"/>
       <c r="Q41" s="103" t="s">
@@ -21377,17 +21434,20 @@
       <c r="T41" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U41" s="1002"/>
-      <c r="V41" s="1005"/>
-      <c r="W41" s="1032"/>
-      <c r="X41" s="1033"/>
-      <c r="Y41" s="1028"/>
+      <c r="U41" s="1012"/>
+      <c r="V41" s="1015"/>
+      <c r="W41" s="986"/>
+      <c r="X41" s="987"/>
+      <c r="Y41" s="982"/>
       <c r="Z41" s="202"/>
     </row>
-    <row r="42" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L42" s="988"/>
-      <c r="M42" s="993"/>
-      <c r="N42" s="1019"/>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1521</v>
+      </c>
+      <c r="L42" s="1036"/>
+      <c r="M42" s="1004"/>
+      <c r="N42" s="1028"/>
       <c r="O42" s="72"/>
       <c r="P42" s="73"/>
       <c r="Q42" s="74" t="s">
@@ -21400,16 +21460,19 @@
       <c r="T42" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U42" s="1002"/>
-      <c r="V42" s="1005"/>
-      <c r="W42" s="1032"/>
-      <c r="X42" s="1033"/>
-      <c r="Y42" s="1028"/>
-    </row>
-    <row r="43" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L43" s="988"/>
-      <c r="M43" s="993"/>
-      <c r="N43" s="1019"/>
+      <c r="U42" s="1012"/>
+      <c r="V42" s="1015"/>
+      <c r="W42" s="986"/>
+      <c r="X42" s="987"/>
+      <c r="Y42" s="982"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1524</v>
+      </c>
+      <c r="L43" s="1036"/>
+      <c r="M43" s="1004"/>
+      <c r="N43" s="1028"/>
       <c r="O43" s="96"/>
       <c r="P43" s="97"/>
       <c r="Q43" s="169" t="s">
@@ -21422,16 +21485,16 @@
       <c r="T43" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U43" s="1002"/>
-      <c r="V43" s="1005"/>
-      <c r="W43" s="1032"/>
-      <c r="X43" s="1033"/>
-      <c r="Y43" s="1028"/>
-    </row>
-    <row r="44" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L44" s="989"/>
-      <c r="M44" s="993"/>
-      <c r="N44" s="1019"/>
+      <c r="U43" s="1012"/>
+      <c r="V43" s="1015"/>
+      <c r="W43" s="986"/>
+      <c r="X43" s="987"/>
+      <c r="Y43" s="982"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L44" s="1037"/>
+      <c r="M44" s="1004"/>
+      <c r="N44" s="1028"/>
       <c r="O44" s="104"/>
       <c r="P44" s="105"/>
       <c r="Q44" s="170" t="s">
@@ -21444,18 +21507,27 @@
       <c r="T44" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U44" s="1002"/>
-      <c r="V44" s="1005"/>
-      <c r="W44" s="1032"/>
-      <c r="X44" s="1033"/>
-      <c r="Y44" s="1028"/>
-    </row>
-    <row r="45" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L45" s="987" t="s">
+      <c r="U44" s="1012"/>
+      <c r="V44" s="1015"/>
+      <c r="W44" s="986"/>
+      <c r="X44" s="987"/>
+      <c r="Y44" s="982"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1525</v>
+      </c>
+      <c r="B45" s="288" t="s">
+        <v>1528</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1530</v>
+      </c>
+      <c r="L45" s="1035" t="s">
         <v>101</v>
       </c>
-      <c r="M45" s="993"/>
-      <c r="N45" s="1019"/>
+      <c r="M45" s="1004"/>
+      <c r="N45" s="1028"/>
       <c r="O45" s="98"/>
       <c r="P45" s="99"/>
       <c r="Q45" s="100" t="s">
@@ -21468,16 +21540,28 @@
       <c r="T45" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U45" s="1002"/>
-      <c r="V45" s="1005"/>
-      <c r="W45" s="1032"/>
-      <c r="X45" s="1033"/>
-      <c r="Y45" s="1028"/>
-    </row>
-    <row r="46" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L46" s="990"/>
-      <c r="M46" s="993"/>
-      <c r="N46" s="1019"/>
+      <c r="U45" s="1012"/>
+      <c r="V45" s="1015"/>
+      <c r="W45" s="986"/>
+      <c r="X45" s="987"/>
+      <c r="Y45" s="982"/>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B46" s="173" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1530</v>
+      </c>
+      <c r="D46" s="173" t="s">
+        <v>1531</v>
+      </c>
+      <c r="L46" s="1038"/>
+      <c r="M46" s="1004"/>
+      <c r="N46" s="1028"/>
       <c r="O46" s="72"/>
       <c r="P46" s="73"/>
       <c r="Q46" s="74" t="s">
@@ -21490,16 +21574,16 @@
       <c r="T46" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U46" s="1002"/>
-      <c r="V46" s="1005"/>
-      <c r="W46" s="1032"/>
-      <c r="X46" s="1033"/>
-      <c r="Y46" s="1028"/>
-    </row>
-    <row r="47" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L47" s="990"/>
-      <c r="M47" s="993"/>
-      <c r="N47" s="1019"/>
+      <c r="U46" s="1012"/>
+      <c r="V46" s="1015"/>
+      <c r="W46" s="986"/>
+      <c r="X46" s="987"/>
+      <c r="Y46" s="982"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L47" s="1038"/>
+      <c r="M47" s="1004"/>
+      <c r="N47" s="1028"/>
       <c r="O47" s="96"/>
       <c r="P47" s="97"/>
       <c r="Q47" s="169" t="s">
@@ -21512,16 +21596,16 @@
       <c r="T47" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U47" s="1002"/>
-      <c r="V47" s="1005"/>
-      <c r="W47" s="1032"/>
-      <c r="X47" s="1033"/>
-      <c r="Y47" s="1028"/>
-    </row>
-    <row r="48" spans="12:26" x14ac:dyDescent="0.25">
-      <c r="L48" s="991"/>
-      <c r="M48" s="993"/>
-      <c r="N48" s="1019"/>
+      <c r="U47" s="1012"/>
+      <c r="V47" s="1015"/>
+      <c r="W47" s="986"/>
+      <c r="X47" s="987"/>
+      <c r="Y47" s="982"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L48" s="1039"/>
+      <c r="M48" s="1004"/>
+      <c r="N48" s="1028"/>
       <c r="O48" s="104"/>
       <c r="P48" s="105"/>
       <c r="Q48" s="170" t="s">
@@ -21534,18 +21618,18 @@
       <c r="T48" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U48" s="1002"/>
-      <c r="V48" s="1005"/>
-      <c r="W48" s="1032"/>
-      <c r="X48" s="1033"/>
-      <c r="Y48" s="1028"/>
-    </row>
-    <row r="49" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L49" s="987" t="s">
+      <c r="U48" s="1012"/>
+      <c r="V48" s="1015"/>
+      <c r="W48" s="986"/>
+      <c r="X48" s="987"/>
+      <c r="Y48" s="982"/>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="L49" s="1035" t="s">
         <v>100</v>
       </c>
-      <c r="M49" s="993"/>
-      <c r="N49" s="1019"/>
+      <c r="M49" s="1004"/>
+      <c r="N49" s="1028"/>
       <c r="O49" s="98"/>
       <c r="P49" s="99"/>
       <c r="Q49" s="100" t="s">
@@ -21558,16 +21642,16 @@
       <c r="T49" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U49" s="1002"/>
-      <c r="V49" s="1005"/>
-      <c r="W49" s="1032"/>
-      <c r="X49" s="1033"/>
-      <c r="Y49" s="1028"/>
-    </row>
-    <row r="50" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L50" s="988"/>
-      <c r="M50" s="993"/>
-      <c r="N50" s="1019"/>
+      <c r="U49" s="1012"/>
+      <c r="V49" s="1015"/>
+      <c r="W49" s="986"/>
+      <c r="X49" s="987"/>
+      <c r="Y49" s="982"/>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="L50" s="1036"/>
+      <c r="M50" s="1004"/>
+      <c r="N50" s="1028"/>
       <c r="O50" s="72"/>
       <c r="P50" s="73"/>
       <c r="Q50" s="74" t="s">
@@ -21576,22 +21660,25 @@
       <c r="R50" s="74" t="s">
         <v>92</v>
       </c>
-      <c r="S50" s="998" t="s">
+      <c r="S50" s="1008" t="s">
         <v>115</v>
       </c>
       <c r="T50" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U50" s="1002"/>
-      <c r="V50" s="1005"/>
-      <c r="W50" s="1032"/>
-      <c r="X50" s="1033"/>
-      <c r="Y50" s="1028"/>
-    </row>
-    <row r="51" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L51" s="988"/>
-      <c r="M51" s="993"/>
-      <c r="N51" s="1019"/>
+      <c r="U50" s="1012"/>
+      <c r="V50" s="1015"/>
+      <c r="W50" s="986"/>
+      <c r="X50" s="987"/>
+      <c r="Y50" s="982"/>
+    </row>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1532</v>
+      </c>
+      <c r="L51" s="1036"/>
+      <c r="M51" s="1004"/>
+      <c r="N51" s="1028"/>
       <c r="O51" s="72"/>
       <c r="P51" s="73"/>
       <c r="Q51" s="74" t="s">
@@ -21600,20 +21687,23 @@
       <c r="R51" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="S51" s="999"/>
+      <c r="S51" s="1009"/>
       <c r="T51" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U51" s="1002"/>
-      <c r="V51" s="1005"/>
-      <c r="W51" s="1032"/>
-      <c r="X51" s="1033"/>
-      <c r="Y51" s="1028"/>
-    </row>
-    <row r="52" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L52" s="989"/>
-      <c r="M52" s="993"/>
-      <c r="N52" s="1019"/>
+      <c r="U51" s="1012"/>
+      <c r="V51" s="1015"/>
+      <c r="W51" s="986"/>
+      <c r="X51" s="987"/>
+      <c r="Y51" s="982"/>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>1533</v>
+      </c>
+      <c r="L52" s="1037"/>
+      <c r="M52" s="1004"/>
+      <c r="N52" s="1028"/>
       <c r="O52" s="75" t="s">
         <v>64</v>
       </c>
@@ -21624,22 +21714,22 @@
       <c r="R52" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="S52" s="1000"/>
+      <c r="S52" s="1010"/>
       <c r="T52" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="U52" s="1002"/>
-      <c r="V52" s="1005"/>
-      <c r="W52" s="1032"/>
-      <c r="X52" s="1033"/>
-      <c r="Y52" s="1028"/>
-    </row>
-    <row r="53" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L53" s="987" t="s">
+      <c r="U52" s="1012"/>
+      <c r="V52" s="1015"/>
+      <c r="W52" s="986"/>
+      <c r="X52" s="987"/>
+      <c r="Y52" s="982"/>
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="L53" s="1035" t="s">
         <v>99</v>
       </c>
-      <c r="M53" s="993"/>
-      <c r="N53" s="1019"/>
+      <c r="M53" s="1004"/>
+      <c r="N53" s="1028"/>
       <c r="O53" s="83"/>
       <c r="P53" s="84"/>
       <c r="Q53" s="85" t="s">
@@ -21652,16 +21742,16 @@
       <c r="T53" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="U53" s="1002"/>
-      <c r="V53" s="1005"/>
-      <c r="W53" s="1032"/>
-      <c r="X53" s="1033"/>
-      <c r="Y53" s="1028"/>
-    </row>
-    <row r="54" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L54" s="988"/>
-      <c r="M54" s="993"/>
-      <c r="N54" s="1019"/>
+      <c r="U53" s="1012"/>
+      <c r="V53" s="1015"/>
+      <c r="W53" s="986"/>
+      <c r="X53" s="987"/>
+      <c r="Y53" s="982"/>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="L54" s="1036"/>
+      <c r="M54" s="1004"/>
+      <c r="N54" s="1028"/>
       <c r="O54" s="86"/>
       <c r="P54" s="87"/>
       <c r="Q54" s="88" t="s">
@@ -21674,16 +21764,16 @@
       <c r="T54" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U54" s="1002"/>
-      <c r="V54" s="1005"/>
-      <c r="W54" s="1032"/>
-      <c r="X54" s="1033"/>
-      <c r="Y54" s="1028"/>
-    </row>
-    <row r="55" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L55" s="988"/>
-      <c r="M55" s="993"/>
-      <c r="N55" s="1019"/>
+      <c r="U54" s="1012"/>
+      <c r="V54" s="1015"/>
+      <c r="W54" s="986"/>
+      <c r="X54" s="987"/>
+      <c r="Y54" s="982"/>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="L55" s="1036"/>
+      <c r="M55" s="1004"/>
+      <c r="N55" s="1028"/>
       <c r="O55" s="86"/>
       <c r="P55" s="87"/>
       <c r="Q55" s="88" t="s">
@@ -21696,16 +21786,16 @@
       <c r="T55" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U55" s="1002"/>
-      <c r="V55" s="1005"/>
-      <c r="W55" s="1032"/>
-      <c r="X55" s="1033"/>
-      <c r="Y55" s="1028"/>
-    </row>
-    <row r="56" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L56" s="989"/>
-      <c r="M56" s="993"/>
-      <c r="N56" s="1019"/>
+      <c r="U55" s="1012"/>
+      <c r="V55" s="1015"/>
+      <c r="W55" s="986"/>
+      <c r="X55" s="987"/>
+      <c r="Y55" s="982"/>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="L56" s="1037"/>
+      <c r="M56" s="1004"/>
+      <c r="N56" s="1028"/>
       <c r="O56" s="89" t="s">
         <v>54</v>
       </c>
@@ -21722,18 +21812,18 @@
       <c r="T56" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="U56" s="1002"/>
-      <c r="V56" s="1005"/>
-      <c r="W56" s="1032"/>
-      <c r="X56" s="1033"/>
-      <c r="Y56" s="1028"/>
-    </row>
-    <row r="57" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L57" s="987" t="s">
+      <c r="U56" s="1012"/>
+      <c r="V56" s="1015"/>
+      <c r="W56" s="986"/>
+      <c r="X56" s="987"/>
+      <c r="Y56" s="982"/>
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="L57" s="1035" t="s">
         <v>98</v>
       </c>
-      <c r="M57" s="993"/>
-      <c r="N57" s="1019"/>
+      <c r="M57" s="1004"/>
+      <c r="N57" s="1028"/>
       <c r="O57" s="52"/>
       <c r="P57" s="53"/>
       <c r="Q57" s="54" t="s">
@@ -21746,16 +21836,16 @@
       <c r="T57" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="U57" s="1002"/>
-      <c r="V57" s="1005"/>
-      <c r="W57" s="1032"/>
-      <c r="X57" s="1033"/>
-      <c r="Y57" s="1028"/>
-    </row>
-    <row r="58" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L58" s="988"/>
-      <c r="M58" s="993"/>
-      <c r="N58" s="1019"/>
+      <c r="U57" s="1012"/>
+      <c r="V57" s="1015"/>
+      <c r="W57" s="986"/>
+      <c r="X57" s="987"/>
+      <c r="Y57" s="982"/>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="L58" s="1036"/>
+      <c r="M58" s="1004"/>
+      <c r="N58" s="1028"/>
       <c r="O58" s="55"/>
       <c r="P58" s="56"/>
       <c r="Q58" s="57" t="s">
@@ -21768,16 +21858,16 @@
       <c r="T58" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="U58" s="1002"/>
-      <c r="V58" s="1005"/>
-      <c r="W58" s="1032"/>
-      <c r="X58" s="1033"/>
-      <c r="Y58" s="1028"/>
-    </row>
-    <row r="59" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L59" s="988"/>
-      <c r="M59" s="993"/>
-      <c r="N59" s="1019"/>
+      <c r="U58" s="1012"/>
+      <c r="V58" s="1015"/>
+      <c r="W58" s="986"/>
+      <c r="X58" s="987"/>
+      <c r="Y58" s="982"/>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="L59" s="1036"/>
+      <c r="M59" s="1004"/>
+      <c r="N59" s="1028"/>
       <c r="O59" s="55"/>
       <c r="P59" s="56"/>
       <c r="Q59" s="57" t="s">
@@ -21790,16 +21880,16 @@
       <c r="T59" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U59" s="1002"/>
-      <c r="V59" s="1005"/>
-      <c r="W59" s="1032"/>
-      <c r="X59" s="1033"/>
-      <c r="Y59" s="1028"/>
-    </row>
-    <row r="60" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L60" s="989"/>
-      <c r="M60" s="993"/>
-      <c r="N60" s="1019"/>
+      <c r="U59" s="1012"/>
+      <c r="V59" s="1015"/>
+      <c r="W59" s="986"/>
+      <c r="X59" s="987"/>
+      <c r="Y59" s="982"/>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="L60" s="1037"/>
+      <c r="M60" s="1004"/>
+      <c r="N60" s="1028"/>
       <c r="O60" s="55"/>
       <c r="P60" s="56"/>
       <c r="Q60" s="57" t="s">
@@ -21812,18 +21902,18 @@
       <c r="T60" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U60" s="1002"/>
-      <c r="V60" s="1005"/>
-      <c r="W60" s="1032"/>
-      <c r="X60" s="1033"/>
-      <c r="Y60" s="1028"/>
-    </row>
-    <row r="61" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L61" s="987" t="s">
+      <c r="U60" s="1012"/>
+      <c r="V60" s="1015"/>
+      <c r="W60" s="986"/>
+      <c r="X60" s="987"/>
+      <c r="Y60" s="982"/>
+    </row>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="L61" s="1035" t="s">
         <v>97</v>
       </c>
-      <c r="M61" s="993"/>
-      <c r="N61" s="1019"/>
+      <c r="M61" s="1004"/>
+      <c r="N61" s="1028"/>
       <c r="O61" s="55"/>
       <c r="P61" s="56"/>
       <c r="Q61" s="57" t="s">
@@ -21836,16 +21926,16 @@
       <c r="T61" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U61" s="1002"/>
-      <c r="V61" s="1005"/>
-      <c r="W61" s="1032"/>
-      <c r="X61" s="1033"/>
-      <c r="Y61" s="1028"/>
-    </row>
-    <row r="62" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L62" s="988"/>
-      <c r="M62" s="993"/>
-      <c r="N62" s="1019"/>
+      <c r="U61" s="1012"/>
+      <c r="V61" s="1015"/>
+      <c r="W61" s="986"/>
+      <c r="X61" s="987"/>
+      <c r="Y61" s="982"/>
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="L62" s="1036"/>
+      <c r="M62" s="1004"/>
+      <c r="N62" s="1028"/>
       <c r="O62" s="55"/>
       <c r="P62" s="56"/>
       <c r="Q62" s="57" t="s">
@@ -21858,16 +21948,16 @@
       <c r="T62" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U62" s="1002"/>
-      <c r="V62" s="1005"/>
-      <c r="W62" s="1032"/>
-      <c r="X62" s="1033"/>
-      <c r="Y62" s="1028"/>
-    </row>
-    <row r="63" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L63" s="988"/>
-      <c r="M63" s="993"/>
-      <c r="N63" s="1019"/>
+      <c r="U62" s="1012"/>
+      <c r="V62" s="1015"/>
+      <c r="W62" s="986"/>
+      <c r="X62" s="987"/>
+      <c r="Y62" s="982"/>
+    </row>
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="L63" s="1036"/>
+      <c r="M63" s="1004"/>
+      <c r="N63" s="1028"/>
       <c r="O63" s="55"/>
       <c r="P63" s="56"/>
       <c r="Q63" s="57" t="s">
@@ -21880,16 +21970,16 @@
       <c r="T63" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U63" s="1002"/>
-      <c r="V63" s="1005"/>
-      <c r="W63" s="1032"/>
-      <c r="X63" s="1033"/>
-      <c r="Y63" s="1028"/>
-    </row>
-    <row r="64" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L64" s="989"/>
-      <c r="M64" s="993"/>
-      <c r="N64" s="1019"/>
+      <c r="U63" s="1012"/>
+      <c r="V63" s="1015"/>
+      <c r="W63" s="986"/>
+      <c r="X63" s="987"/>
+      <c r="Y63" s="982"/>
+    </row>
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="L64" s="1037"/>
+      <c r="M64" s="1004"/>
+      <c r="N64" s="1028"/>
       <c r="O64" s="58" t="s">
         <v>36</v>
       </c>
@@ -21906,18 +21996,18 @@
       <c r="T64" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="U64" s="1002"/>
-      <c r="V64" s="1005"/>
-      <c r="W64" s="1032"/>
-      <c r="X64" s="1033"/>
-      <c r="Y64" s="1028"/>
+      <c r="U64" s="1012"/>
+      <c r="V64" s="1015"/>
+      <c r="W64" s="986"/>
+      <c r="X64" s="987"/>
+      <c r="Y64" s="982"/>
     </row>
     <row r="65" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L65" s="987" t="s">
+      <c r="L65" s="1035" t="s">
         <v>96</v>
       </c>
-      <c r="M65" s="993"/>
-      <c r="N65" s="1019"/>
+      <c r="M65" s="1004"/>
+      <c r="N65" s="1028"/>
       <c r="O65" s="61"/>
       <c r="P65" s="62"/>
       <c r="Q65" s="63" t="s">
@@ -21930,16 +22020,16 @@
       <c r="T65" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="U65" s="1002"/>
-      <c r="V65" s="1005"/>
-      <c r="W65" s="1032"/>
-      <c r="X65" s="1033"/>
-      <c r="Y65" s="1028"/>
+      <c r="U65" s="1012"/>
+      <c r="V65" s="1015"/>
+      <c r="W65" s="986"/>
+      <c r="X65" s="987"/>
+      <c r="Y65" s="982"/>
     </row>
     <row r="66" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L66" s="988"/>
-      <c r="M66" s="993"/>
-      <c r="N66" s="1019"/>
+      <c r="L66" s="1036"/>
+      <c r="M66" s="1004"/>
+      <c r="N66" s="1028"/>
       <c r="O66" s="64"/>
       <c r="P66" s="65"/>
       <c r="Q66" s="66" t="s">
@@ -21952,16 +22042,16 @@
       <c r="T66" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U66" s="1002"/>
-      <c r="V66" s="1005"/>
-      <c r="W66" s="1032"/>
-      <c r="X66" s="1033"/>
-      <c r="Y66" s="1028"/>
+      <c r="U66" s="1012"/>
+      <c r="V66" s="1015"/>
+      <c r="W66" s="986"/>
+      <c r="X66" s="987"/>
+      <c r="Y66" s="982"/>
     </row>
     <row r="67" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L67" s="988"/>
-      <c r="M67" s="993"/>
-      <c r="N67" s="1019"/>
+      <c r="L67" s="1036"/>
+      <c r="M67" s="1004"/>
+      <c r="N67" s="1028"/>
       <c r="O67" s="64"/>
       <c r="P67" s="65"/>
       <c r="Q67" s="66" t="s">
@@ -21974,16 +22064,16 @@
       <c r="T67" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="U67" s="1002"/>
-      <c r="V67" s="1005"/>
-      <c r="W67" s="1032"/>
-      <c r="X67" s="1033"/>
-      <c r="Y67" s="1028"/>
+      <c r="U67" s="1012"/>
+      <c r="V67" s="1015"/>
+      <c r="W67" s="986"/>
+      <c r="X67" s="987"/>
+      <c r="Y67" s="982"/>
     </row>
     <row r="68" spans="12:25" x14ac:dyDescent="0.25">
-      <c r="L68" s="989"/>
-      <c r="M68" s="994"/>
-      <c r="N68" s="1020"/>
+      <c r="L68" s="1037"/>
+      <c r="M68" s="1005"/>
+      <c r="N68" s="1029"/>
       <c r="O68" s="67" t="s">
         <v>25</v>
       </c>
@@ -22000,11 +22090,11 @@
       <c r="T68" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="U68" s="1003"/>
-      <c r="V68" s="1006"/>
-      <c r="W68" s="1034"/>
-      <c r="X68" s="1035"/>
-      <c r="Y68" s="1029"/>
+      <c r="U68" s="1013"/>
+      <c r="V68" s="1016"/>
+      <c r="W68" s="988"/>
+      <c r="X68" s="989"/>
+      <c r="Y68" s="983"/>
     </row>
     <row r="69" spans="12:25" x14ac:dyDescent="0.25">
       <c r="N69" s="205"/>
@@ -22012,34 +22102,11 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="Y5:Y68"/>
-    <mergeCell ref="W17:X67"/>
-    <mergeCell ref="W68:X68"/>
-    <mergeCell ref="W5:W16"/>
-    <mergeCell ref="X5:X6"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="X15:X16"/>
-    <mergeCell ref="M5:M68"/>
-    <mergeCell ref="O3:T3"/>
-    <mergeCell ref="S50:S52"/>
-    <mergeCell ref="U5:U68"/>
-    <mergeCell ref="V5:V68"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="N5:N7"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="N8:N11"/>
-    <mergeCell ref="N37:N68"/>
-    <mergeCell ref="N35:N36"/>
-    <mergeCell ref="N31:N34"/>
-    <mergeCell ref="N26:N30"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AI4:AK4"/>
+    <mergeCell ref="AC3:AK3"/>
     <mergeCell ref="L65:L68"/>
     <mergeCell ref="L61:L64"/>
     <mergeCell ref="L57:L60"/>
@@ -22056,11 +22123,34 @@
     <mergeCell ref="L49:L52"/>
     <mergeCell ref="L45:L48"/>
     <mergeCell ref="L41:L44"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AI4:AK4"/>
-    <mergeCell ref="AC3:AK3"/>
+    <mergeCell ref="M5:M68"/>
+    <mergeCell ref="O3:T3"/>
+    <mergeCell ref="S50:S52"/>
+    <mergeCell ref="U5:U68"/>
+    <mergeCell ref="V5:V68"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="N5:N7"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="N8:N11"/>
+    <mergeCell ref="N37:N68"/>
+    <mergeCell ref="N35:N36"/>
+    <mergeCell ref="N31:N34"/>
+    <mergeCell ref="N26:N30"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="Y5:Y68"/>
+    <mergeCell ref="W17:X67"/>
+    <mergeCell ref="W68:X68"/>
+    <mergeCell ref="W5:W16"/>
+    <mergeCell ref="X5:X6"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="X15:X16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -22085,18 +22175,18 @@
       <c r="E3" s="466" t="s">
         <v>112</v>
       </c>
-      <c r="F3" s="1071" t="s">
+      <c r="F3" s="1048" t="s">
         <v>119</v>
       </c>
-      <c r="G3" s="1072"/>
-      <c r="H3" s="1072"/>
-      <c r="I3" s="1072"/>
-      <c r="J3" s="1072"/>
-      <c r="K3" s="1072"/>
-      <c r="L3" s="1059">
+      <c r="G3" s="1049"/>
+      <c r="H3" s="1049"/>
+      <c r="I3" s="1049"/>
+      <c r="J3" s="1049"/>
+      <c r="K3" s="1049"/>
+      <c r="L3" s="1067">
         <v>2</v>
       </c>
-      <c r="M3" s="1061">
+      <c r="M3" s="1069">
         <v>5</v>
       </c>
     </row>
@@ -22120,11 +22210,11 @@
       <c r="K4" s="141" t="s">
         <v>88</v>
       </c>
-      <c r="L4" s="1060"/>
-      <c r="M4" s="1062"/>
+      <c r="L4" s="1068"/>
+      <c r="M4" s="1070"/>
     </row>
     <row r="5" spans="5:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="1063" t="s">
+      <c r="E5" s="1050" t="s">
         <v>111</v>
       </c>
       <c r="F5" s="920"/>
@@ -22135,13 +22225,13 @@
       <c r="K5" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="1048" t="s">
+      <c r="L5" s="1056" t="s">
         <v>1447</v>
       </c>
       <c r="M5" s="954"/>
     </row>
     <row r="6" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E6" s="1064"/>
+      <c r="E6" s="1051"/>
       <c r="F6" s="406"/>
       <c r="G6" s="924"/>
       <c r="H6" s="924"/>
@@ -22150,11 +22240,11 @@
       <c r="K6" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="1049"/>
+      <c r="L6" s="1057"/>
       <c r="M6" s="955"/>
     </row>
     <row r="7" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E7" s="1064"/>
+      <c r="E7" s="1051"/>
       <c r="F7" s="406"/>
       <c r="G7" s="924"/>
       <c r="H7" s="924"/>
@@ -22163,11 +22253,11 @@
       <c r="K7" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L7" s="1049"/>
+      <c r="L7" s="1057"/>
       <c r="M7" s="955"/>
     </row>
     <row r="8" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E8" s="1065"/>
+      <c r="E8" s="1053"/>
       <c r="F8" s="925"/>
       <c r="G8" s="926"/>
       <c r="H8" s="927"/>
@@ -22176,11 +22266,11 @@
       <c r="K8" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="1049"/>
+      <c r="L8" s="1057"/>
       <c r="M8" s="955"/>
     </row>
     <row r="9" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E9" s="1063" t="s">
+      <c r="E9" s="1050" t="s">
         <v>110</v>
       </c>
       <c r="F9" s="920"/>
@@ -22191,11 +22281,11 @@
       <c r="K9" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L9" s="1049"/>
+      <c r="L9" s="1057"/>
       <c r="M9" s="955"/>
     </row>
     <row r="10" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E10" s="1064"/>
+      <c r="E10" s="1051"/>
       <c r="F10" s="406"/>
       <c r="G10" s="924"/>
       <c r="H10" s="924"/>
@@ -22204,11 +22294,11 @@
       <c r="K10" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="1049"/>
+      <c r="L10" s="1057"/>
       <c r="M10" s="955"/>
     </row>
     <row r="11" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E11" s="1064"/>
+      <c r="E11" s="1051"/>
       <c r="F11" s="406"/>
       <c r="G11" s="924"/>
       <c r="H11" s="924"/>
@@ -22217,11 +22307,11 @@
       <c r="K11" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L11" s="1049"/>
+      <c r="L11" s="1057"/>
       <c r="M11" s="955"/>
     </row>
     <row r="12" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E12" s="1065"/>
+      <c r="E12" s="1053"/>
       <c r="F12" s="930"/>
       <c r="G12" s="931"/>
       <c r="H12" s="932"/>
@@ -22230,11 +22320,11 @@
       <c r="K12" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L12" s="1049"/>
+      <c r="L12" s="1057"/>
       <c r="M12" s="955"/>
     </row>
     <row r="13" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E13" s="1063" t="s">
+      <c r="E13" s="1050" t="s">
         <v>109</v>
       </c>
       <c r="F13" s="933"/>
@@ -22245,11 +22335,11 @@
       <c r="K13" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L13" s="1049"/>
+      <c r="L13" s="1057"/>
       <c r="M13" s="955"/>
     </row>
     <row r="14" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E14" s="1064"/>
+      <c r="E14" s="1051"/>
       <c r="F14" s="406"/>
       <c r="G14" s="924"/>
       <c r="H14" s="924"/>
@@ -22258,11 +22348,11 @@
       <c r="K14" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L14" s="1049"/>
+      <c r="L14" s="1057"/>
       <c r="M14" s="955"/>
     </row>
     <row r="15" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E15" s="1064"/>
+      <c r="E15" s="1051"/>
       <c r="F15" s="406"/>
       <c r="G15" s="924"/>
       <c r="H15" s="924"/>
@@ -22271,11 +22361,11 @@
       <c r="K15" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L15" s="1049"/>
+      <c r="L15" s="1057"/>
       <c r="M15" s="955"/>
     </row>
     <row r="16" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E16" s="1065"/>
+      <c r="E16" s="1053"/>
       <c r="F16" s="925"/>
       <c r="G16" s="926"/>
       <c r="H16" s="927"/>
@@ -22284,11 +22374,11 @@
       <c r="K16" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L16" s="1049"/>
+      <c r="L16" s="1057"/>
       <c r="M16" s="955"/>
     </row>
     <row r="17" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E17" s="1063" t="s">
+      <c r="E17" s="1050" t="s">
         <v>108</v>
       </c>
       <c r="F17" s="920"/>
@@ -22299,11 +22389,11 @@
       <c r="K17" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L17" s="1049"/>
+      <c r="L17" s="1057"/>
       <c r="M17" s="955"/>
     </row>
     <row r="18" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E18" s="1064"/>
+      <c r="E18" s="1051"/>
       <c r="F18" s="406"/>
       <c r="G18" s="924"/>
       <c r="H18" s="924"/>
@@ -22312,11 +22402,11 @@
       <c r="K18" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L18" s="1049"/>
+      <c r="L18" s="1057"/>
       <c r="M18" s="955"/>
     </row>
     <row r="19" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E19" s="1064"/>
+      <c r="E19" s="1051"/>
       <c r="F19" s="406"/>
       <c r="G19" s="924"/>
       <c r="H19" s="924"/>
@@ -22325,11 +22415,11 @@
       <c r="K19" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L19" s="1049"/>
+      <c r="L19" s="1057"/>
       <c r="M19" s="955"/>
     </row>
     <row r="20" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E20" s="1065"/>
+      <c r="E20" s="1053"/>
       <c r="F20" s="930"/>
       <c r="G20" s="931"/>
       <c r="H20" s="932"/>
@@ -22338,11 +22428,11 @@
       <c r="K20" s="688" t="s">
         <v>33</v>
       </c>
-      <c r="L20" s="1049"/>
+      <c r="L20" s="1057"/>
       <c r="M20" s="955"/>
     </row>
     <row r="21" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E21" s="1063" t="s">
+      <c r="E21" s="1050" t="s">
         <v>107</v>
       </c>
       <c r="F21" s="936"/>
@@ -22353,13 +22443,13 @@
       <c r="K21" s="901" t="s">
         <v>33</v>
       </c>
-      <c r="L21" s="1068" t="s">
+      <c r="L21" s="1073" t="s">
         <v>1452</v>
       </c>
       <c r="M21" s="955"/>
     </row>
     <row r="22" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E22" s="1064"/>
+      <c r="E22" s="1051"/>
       <c r="F22" s="406"/>
       <c r="G22" s="924"/>
       <c r="H22" s="924"/>
@@ -22368,11 +22458,11 @@
       <c r="K22" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L22" s="1069"/>
+      <c r="L22" s="1074"/>
       <c r="M22" s="955"/>
     </row>
     <row r="23" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E23" s="1064"/>
+      <c r="E23" s="1051"/>
       <c r="F23" s="930"/>
       <c r="G23" s="931"/>
       <c r="H23" s="931"/>
@@ -22381,11 +22471,11 @@
       <c r="K23" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L23" s="1069"/>
+      <c r="L23" s="1074"/>
       <c r="M23" s="955"/>
     </row>
     <row r="24" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E24" s="1065"/>
+      <c r="E24" s="1053"/>
       <c r="F24" s="925"/>
       <c r="G24" s="926"/>
       <c r="H24" s="927"/>
@@ -22394,11 +22484,11 @@
       <c r="K24" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L24" s="1069"/>
+      <c r="L24" s="1074"/>
       <c r="M24" s="955"/>
     </row>
     <row r="25" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E25" s="1063" t="s">
+      <c r="E25" s="1050" t="s">
         <v>106</v>
       </c>
       <c r="F25" s="920"/>
@@ -22409,11 +22499,11 @@
       <c r="K25" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="1069"/>
+      <c r="L25" s="1074"/>
       <c r="M25" s="955"/>
     </row>
     <row r="26" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E26" s="1064"/>
+      <c r="E26" s="1051"/>
       <c r="F26" s="406"/>
       <c r="G26" s="924"/>
       <c r="H26" s="924"/>
@@ -22422,11 +22512,11 @@
       <c r="K26" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L26" s="1070"/>
+      <c r="L26" s="1075"/>
       <c r="M26" s="955"/>
     </row>
     <row r="27" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E27" s="1064"/>
+      <c r="E27" s="1051"/>
       <c r="F27" s="930"/>
       <c r="G27" s="931"/>
       <c r="H27" s="932" t="s">
@@ -22439,13 +22529,13 @@
       <c r="K27" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L27" s="1066" t="s">
+      <c r="L27" s="1071" t="s">
         <v>1448</v>
       </c>
       <c r="M27" s="955"/>
     </row>
     <row r="28" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E28" s="1065"/>
+      <c r="E28" s="1053"/>
       <c r="F28" s="930"/>
       <c r="G28" s="931"/>
       <c r="H28" s="932" t="s">
@@ -22458,11 +22548,11 @@
       <c r="K28" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L28" s="1067"/>
+      <c r="L28" s="1072"/>
       <c r="M28" s="955"/>
     </row>
     <row r="29" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E29" s="1063" t="s">
+      <c r="E29" s="1050" t="s">
         <v>105</v>
       </c>
       <c r="F29" s="933"/>
@@ -22473,13 +22563,13 @@
       <c r="K29" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L29" s="1050" t="s">
+      <c r="L29" s="1058" t="s">
         <v>1450</v>
       </c>
       <c r="M29" s="955"/>
     </row>
     <row r="30" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E30" s="1064"/>
+      <c r="E30" s="1051"/>
       <c r="F30" s="406"/>
       <c r="G30" s="924"/>
       <c r="H30" s="924"/>
@@ -22488,11 +22578,11 @@
       <c r="K30" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L30" s="1051"/>
+      <c r="L30" s="1059"/>
       <c r="M30" s="955"/>
     </row>
     <row r="31" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E31" s="1064"/>
+      <c r="E31" s="1051"/>
       <c r="F31" s="406"/>
       <c r="G31" s="924"/>
       <c r="H31" s="924"/>
@@ -22501,11 +22591,11 @@
       <c r="K31" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L31" s="1051"/>
+      <c r="L31" s="1059"/>
       <c r="M31" s="955"/>
     </row>
     <row r="32" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E32" s="1065"/>
+      <c r="E32" s="1053"/>
       <c r="F32" s="941"/>
       <c r="G32" s="942"/>
       <c r="H32" s="943"/>
@@ -22514,11 +22604,11 @@
       <c r="K32" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L32" s="1051"/>
+      <c r="L32" s="1059"/>
       <c r="M32" s="955"/>
     </row>
     <row r="33" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E33" s="1063" t="s">
+      <c r="E33" s="1050" t="s">
         <v>104</v>
       </c>
       <c r="F33" s="920"/>
@@ -22529,11 +22619,11 @@
       <c r="K33" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L33" s="1051"/>
+      <c r="L33" s="1059"/>
       <c r="M33" s="955"/>
     </row>
     <row r="34" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E34" s="1064"/>
+      <c r="E34" s="1051"/>
       <c r="F34" s="406"/>
       <c r="G34" s="924"/>
       <c r="H34" s="924"/>
@@ -22542,11 +22632,11 @@
       <c r="K34" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L34" s="1051"/>
+      <c r="L34" s="1059"/>
       <c r="M34" s="955"/>
     </row>
     <row r="35" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E35" s="1064"/>
+      <c r="E35" s="1051"/>
       <c r="F35" s="406"/>
       <c r="G35" s="924"/>
       <c r="H35" s="924"/>
@@ -22555,11 +22645,11 @@
       <c r="K35" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L35" s="1051"/>
+      <c r="L35" s="1059"/>
       <c r="M35" s="955"/>
     </row>
     <row r="36" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E36" s="1065"/>
+      <c r="E36" s="1053"/>
       <c r="F36" s="945"/>
       <c r="G36" s="946"/>
       <c r="H36" s="947"/>
@@ -22568,11 +22658,11 @@
       <c r="K36" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="L36" s="1052"/>
+      <c r="L36" s="1060"/>
       <c r="M36" s="955"/>
     </row>
     <row r="37" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E37" s="1063" t="s">
+      <c r="E37" s="1050" t="s">
         <v>103</v>
       </c>
       <c r="F37" s="70"/>
@@ -22589,15 +22679,15 @@
       <c r="K37" s="138" t="s">
         <v>32</v>
       </c>
-      <c r="L37" s="1053" t="s">
+      <c r="L37" s="1061" t="s">
         <v>1451</v>
       </c>
-      <c r="M37" s="1056" t="s">
+      <c r="M37" s="1064" t="s">
         <v>1449</v>
       </c>
     </row>
     <row r="38" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E38" s="1064"/>
+      <c r="E38" s="1051"/>
       <c r="F38" s="72"/>
       <c r="G38" s="73"/>
       <c r="H38" s="74" t="s">
@@ -22610,11 +22700,11 @@
       <c r="K38" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L38" s="1054"/>
-      <c r="M38" s="1057"/>
+      <c r="L38" s="1062"/>
+      <c r="M38" s="1065"/>
     </row>
     <row r="39" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E39" s="1064"/>
+      <c r="E39" s="1051"/>
       <c r="F39" s="72"/>
       <c r="G39" s="73"/>
       <c r="H39" s="74" t="s">
@@ -22627,11 +22717,11 @@
       <c r="K39" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L39" s="1054"/>
-      <c r="M39" s="1057"/>
+      <c r="L39" s="1062"/>
+      <c r="M39" s="1065"/>
     </row>
     <row r="40" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E40" s="1065"/>
+      <c r="E40" s="1053"/>
       <c r="F40" s="96"/>
       <c r="G40" s="97"/>
       <c r="H40" s="169" t="s">
@@ -22646,11 +22736,11 @@
       <c r="K40" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L40" s="1054"/>
-      <c r="M40" s="1057"/>
+      <c r="L40" s="1062"/>
+      <c r="M40" s="1065"/>
     </row>
     <row r="41" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E41" s="1063" t="s">
+      <c r="E41" s="1050" t="s">
         <v>102</v>
       </c>
       <c r="F41" s="101"/>
@@ -22667,11 +22757,11 @@
       <c r="K41" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L41" s="1054"/>
-      <c r="M41" s="1057"/>
+      <c r="L41" s="1062"/>
+      <c r="M41" s="1065"/>
     </row>
     <row r="42" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E42" s="1064"/>
+      <c r="E42" s="1051"/>
       <c r="F42" s="72"/>
       <c r="G42" s="73"/>
       <c r="H42" s="74" t="s">
@@ -22684,11 +22774,11 @@
       <c r="K42" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L42" s="1054"/>
-      <c r="M42" s="1057"/>
+      <c r="L42" s="1062"/>
+      <c r="M42" s="1065"/>
     </row>
     <row r="43" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E43" s="1064"/>
+      <c r="E43" s="1051"/>
       <c r="F43" s="96"/>
       <c r="G43" s="97"/>
       <c r="H43" s="169" t="s">
@@ -22701,11 +22791,11 @@
       <c r="K43" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L43" s="1054"/>
-      <c r="M43" s="1057"/>
+      <c r="L43" s="1062"/>
+      <c r="M43" s="1065"/>
     </row>
     <row r="44" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E44" s="1065"/>
+      <c r="E44" s="1053"/>
       <c r="F44" s="104"/>
       <c r="G44" s="105"/>
       <c r="H44" s="170" t="s">
@@ -22718,11 +22808,11 @@
       <c r="K44" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L44" s="1054"/>
-      <c r="M44" s="1057"/>
+      <c r="L44" s="1062"/>
+      <c r="M44" s="1065"/>
     </row>
     <row r="45" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E45" s="1063" t="s">
+      <c r="E45" s="1050" t="s">
         <v>101</v>
       </c>
       <c r="F45" s="98"/>
@@ -22737,11 +22827,11 @@
       <c r="K45" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L45" s="1054"/>
-      <c r="M45" s="1057"/>
+      <c r="L45" s="1062"/>
+      <c r="M45" s="1065"/>
     </row>
     <row r="46" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E46" s="1074"/>
+      <c r="E46" s="1054"/>
       <c r="F46" s="72"/>
       <c r="G46" s="73"/>
       <c r="H46" s="74" t="s">
@@ -22754,11 +22844,11 @@
       <c r="K46" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L46" s="1054"/>
-      <c r="M46" s="1057"/>
+      <c r="L46" s="1062"/>
+      <c r="M46" s="1065"/>
     </row>
     <row r="47" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E47" s="1074"/>
+      <c r="E47" s="1054"/>
       <c r="F47" s="96"/>
       <c r="G47" s="97"/>
       <c r="H47" s="169" t="s">
@@ -22771,11 +22861,11 @@
       <c r="K47" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L47" s="1054"/>
-      <c r="M47" s="1057"/>
+      <c r="L47" s="1062"/>
+      <c r="M47" s="1065"/>
     </row>
     <row r="48" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E48" s="1075"/>
+      <c r="E48" s="1055"/>
       <c r="F48" s="104"/>
       <c r="G48" s="105"/>
       <c r="H48" s="170" t="s">
@@ -22788,11 +22878,11 @@
       <c r="K48" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L48" s="1054"/>
-      <c r="M48" s="1057"/>
+      <c r="L48" s="1062"/>
+      <c r="M48" s="1065"/>
     </row>
     <row r="49" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E49" s="1063" t="s">
+      <c r="E49" s="1050" t="s">
         <v>100</v>
       </c>
       <c r="F49" s="98"/>
@@ -22807,11 +22897,11 @@
       <c r="K49" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L49" s="1054"/>
-      <c r="M49" s="1057"/>
+      <c r="L49" s="1062"/>
+      <c r="M49" s="1065"/>
     </row>
     <row r="50" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E50" s="1064"/>
+      <c r="E50" s="1051"/>
       <c r="F50" s="72"/>
       <c r="G50" s="73"/>
       <c r="H50" s="74" t="s">
@@ -22820,17 +22910,17 @@
       <c r="I50" s="74" t="s">
         <v>92</v>
       </c>
-      <c r="J50" s="998" t="s">
+      <c r="J50" s="1008" t="s">
         <v>115</v>
       </c>
       <c r="K50" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L50" s="1054"/>
-      <c r="M50" s="1057"/>
+      <c r="L50" s="1062"/>
+      <c r="M50" s="1065"/>
     </row>
     <row r="51" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E51" s="1064"/>
+      <c r="E51" s="1051"/>
       <c r="F51" s="72"/>
       <c r="G51" s="73"/>
       <c r="H51" s="74" t="s">
@@ -22839,15 +22929,15 @@
       <c r="I51" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="J51" s="999"/>
+      <c r="J51" s="1009"/>
       <c r="K51" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L51" s="1054"/>
-      <c r="M51" s="1057"/>
+      <c r="L51" s="1062"/>
+      <c r="M51" s="1065"/>
     </row>
     <row r="52" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E52" s="1065"/>
+      <c r="E52" s="1053"/>
       <c r="F52" s="75" t="s">
         <v>64</v>
       </c>
@@ -22858,15 +22948,15 @@
       <c r="I52" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="J52" s="1000"/>
+      <c r="J52" s="1010"/>
       <c r="K52" s="951" t="s">
         <v>32</v>
       </c>
-      <c r="L52" s="1054"/>
-      <c r="M52" s="1057"/>
+      <c r="L52" s="1062"/>
+      <c r="M52" s="1065"/>
     </row>
     <row r="53" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E53" s="1063" t="s">
+      <c r="E53" s="1050" t="s">
         <v>99</v>
       </c>
       <c r="F53" s="83"/>
@@ -22881,11 +22971,11 @@
       <c r="K53" s="901" t="s">
         <v>33</v>
       </c>
-      <c r="L53" s="1054"/>
-      <c r="M53" s="1057"/>
+      <c r="L53" s="1062"/>
+      <c r="M53" s="1065"/>
     </row>
     <row r="54" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E54" s="1064"/>
+      <c r="E54" s="1051"/>
       <c r="F54" s="86"/>
       <c r="G54" s="87"/>
       <c r="H54" s="88" t="s">
@@ -22898,11 +22988,11 @@
       <c r="K54" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L54" s="1054"/>
-      <c r="M54" s="1057"/>
+      <c r="L54" s="1062"/>
+      <c r="M54" s="1065"/>
     </row>
     <row r="55" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E55" s="1064"/>
+      <c r="E55" s="1051"/>
       <c r="F55" s="86"/>
       <c r="G55" s="87"/>
       <c r="H55" s="88" t="s">
@@ -22915,11 +23005,11 @@
       <c r="K55" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L55" s="1054"/>
-      <c r="M55" s="1057"/>
+      <c r="L55" s="1062"/>
+      <c r="M55" s="1065"/>
     </row>
     <row r="56" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E56" s="1065"/>
+      <c r="E56" s="1053"/>
       <c r="F56" s="89" t="s">
         <v>54</v>
       </c>
@@ -22936,11 +23026,11 @@
       <c r="K56" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="L56" s="1054"/>
-      <c r="M56" s="1057"/>
+      <c r="L56" s="1062"/>
+      <c r="M56" s="1065"/>
     </row>
     <row r="57" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E57" s="1063" t="s">
+      <c r="E57" s="1050" t="s">
         <v>98</v>
       </c>
       <c r="F57" s="52"/>
@@ -22955,11 +23045,11 @@
       <c r="K57" s="901" t="s">
         <v>33</v>
       </c>
-      <c r="L57" s="1054"/>
-      <c r="M57" s="1057"/>
+      <c r="L57" s="1062"/>
+      <c r="M57" s="1065"/>
     </row>
     <row r="58" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E58" s="1064"/>
+      <c r="E58" s="1051"/>
       <c r="F58" s="55"/>
       <c r="G58" s="56"/>
       <c r="H58" s="57" t="s">
@@ -22972,11 +23062,11 @@
       <c r="K58" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L58" s="1054"/>
-      <c r="M58" s="1057"/>
+      <c r="L58" s="1062"/>
+      <c r="M58" s="1065"/>
     </row>
     <row r="59" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E59" s="1064"/>
+      <c r="E59" s="1051"/>
       <c r="F59" s="55"/>
       <c r="G59" s="56"/>
       <c r="H59" s="57" t="s">
@@ -22989,11 +23079,11 @@
       <c r="K59" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L59" s="1054"/>
-      <c r="M59" s="1057"/>
+      <c r="L59" s="1062"/>
+      <c r="M59" s="1065"/>
     </row>
     <row r="60" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E60" s="1065"/>
+      <c r="E60" s="1053"/>
       <c r="F60" s="55"/>
       <c r="G60" s="56"/>
       <c r="H60" s="57" t="s">
@@ -23006,11 +23096,11 @@
       <c r="K60" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L60" s="1054"/>
-      <c r="M60" s="1057"/>
+      <c r="L60" s="1062"/>
+      <c r="M60" s="1065"/>
     </row>
     <row r="61" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E61" s="1063" t="s">
+      <c r="E61" s="1050" t="s">
         <v>97</v>
       </c>
       <c r="F61" s="55"/>
@@ -23025,11 +23115,11 @@
       <c r="K61" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L61" s="1054"/>
-      <c r="M61" s="1057"/>
+      <c r="L61" s="1062"/>
+      <c r="M61" s="1065"/>
     </row>
     <row r="62" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E62" s="1064"/>
+      <c r="E62" s="1051"/>
       <c r="F62" s="55"/>
       <c r="G62" s="56"/>
       <c r="H62" s="57" t="s">
@@ -23042,11 +23132,11 @@
       <c r="K62" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L62" s="1054"/>
-      <c r="M62" s="1057"/>
+      <c r="L62" s="1062"/>
+      <c r="M62" s="1065"/>
     </row>
     <row r="63" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E63" s="1064"/>
+      <c r="E63" s="1051"/>
       <c r="F63" s="55"/>
       <c r="G63" s="56"/>
       <c r="H63" s="57" t="s">
@@ -23059,11 +23149,11 @@
       <c r="K63" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="L63" s="1054"/>
-      <c r="M63" s="1057"/>
+      <c r="L63" s="1062"/>
+      <c r="M63" s="1065"/>
     </row>
     <row r="64" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E64" s="1065"/>
+      <c r="E64" s="1053"/>
       <c r="F64" s="58" t="s">
         <v>36</v>
       </c>
@@ -23080,11 +23170,11 @@
       <c r="K64" s="951" t="s">
         <v>32</v>
       </c>
-      <c r="L64" s="1055"/>
-      <c r="M64" s="1058"/>
+      <c r="L64" s="1063"/>
+      <c r="M64" s="1066"/>
     </row>
     <row r="65" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E65" s="1063" t="s">
+      <c r="E65" s="1050" t="s">
         <v>96</v>
       </c>
       <c r="F65" s="61"/>
@@ -23103,7 +23193,7 @@
       <c r="M65" s="955"/>
     </row>
     <row r="66" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E66" s="1064"/>
+      <c r="E66" s="1051"/>
       <c r="F66" s="64"/>
       <c r="G66" s="65"/>
       <c r="H66" s="66" t="s">
@@ -23120,7 +23210,7 @@
       <c r="M66" s="955"/>
     </row>
     <row r="67" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E67" s="1064"/>
+      <c r="E67" s="1051"/>
       <c r="F67" s="64"/>
       <c r="G67" s="65"/>
       <c r="H67" s="66" t="s">
@@ -23137,7 +23227,7 @@
       <c r="M67" s="955"/>
     </row>
     <row r="68" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E68" s="1073"/>
+      <c r="E68" s="1052"/>
       <c r="F68" s="469" t="s">
         <v>25</v>
       </c>
@@ -23160,6 +23250,16 @@
     <row r="69" spans="5:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="M37:M64"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="L21:L26"/>
+    <mergeCell ref="E21:E24"/>
+    <mergeCell ref="E25:E28"/>
+    <mergeCell ref="L5:L20"/>
+    <mergeCell ref="L29:L36"/>
+    <mergeCell ref="L37:L64"/>
     <mergeCell ref="F3:K3"/>
     <mergeCell ref="J50:J52"/>
     <mergeCell ref="E65:E68"/>
@@ -23176,16 +23276,6 @@
     <mergeCell ref="E9:E12"/>
     <mergeCell ref="E13:E16"/>
     <mergeCell ref="E17:E20"/>
-    <mergeCell ref="E21:E24"/>
-    <mergeCell ref="E25:E28"/>
-    <mergeCell ref="L5:L20"/>
-    <mergeCell ref="L29:L36"/>
-    <mergeCell ref="L37:L64"/>
-    <mergeCell ref="M37:M64"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="L27:L28"/>
-    <mergeCell ref="L21:L26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -23212,13 +23302,13 @@
       <c r="C4" s="466" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="1071" t="s">
+      <c r="D4" s="1048" t="s">
         <v>119</v>
       </c>
-      <c r="E4" s="1072"/>
-      <c r="F4" s="1072"/>
-      <c r="G4" s="1072"/>
-      <c r="H4" s="1072"/>
+      <c r="E4" s="1049"/>
+      <c r="F4" s="1049"/>
+      <c r="G4" s="1049"/>
+      <c r="H4" s="1049"/>
       <c r="I4" s="482"/>
     </row>
     <row r="5" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -23245,7 +23335,7 @@
       </c>
     </row>
     <row r="6" spans="3:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="1085" t="s">
+      <c r="C6" s="1076" t="s">
         <v>111</v>
       </c>
       <c r="D6" s="473"/>
@@ -23257,12 +23347,12 @@
       <c r="H6" s="480" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="1076" t="s">
+      <c r="I6" s="1080" t="s">
         <v>795</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="1064"/>
+      <c r="C7" s="1051"/>
       <c r="D7" s="434"/>
       <c r="E7" s="65"/>
       <c r="F7" s="65"/>
@@ -23270,10 +23360,10 @@
       <c r="H7" s="447" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="1077"/>
+      <c r="I7" s="1081"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="1064"/>
+      <c r="C8" s="1051"/>
       <c r="D8" s="434"/>
       <c r="E8" s="65"/>
       <c r="F8" s="65"/>
@@ -23281,10 +23371,10 @@
       <c r="H8" s="447" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="1077"/>
+      <c r="I8" s="1081"/>
     </row>
     <row r="9" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="1065"/>
+      <c r="C9" s="1053"/>
       <c r="D9" s="435" t="s">
         <v>73</v>
       </c>
@@ -23298,10 +23388,10 @@
       <c r="H9" s="468" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="1078"/>
+      <c r="I9" s="1084"/>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="1063" t="s">
+      <c r="C10" s="1050" t="s">
         <v>110</v>
       </c>
       <c r="D10" s="478"/>
@@ -23313,12 +23403,12 @@
       <c r="H10" s="493" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="1079" t="s">
+      <c r="I10" s="1078" t="s">
         <v>798</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="1064"/>
+      <c r="C11" s="1051"/>
       <c r="D11" s="72"/>
       <c r="E11" s="73"/>
       <c r="F11" s="65"/>
@@ -23326,10 +23416,10 @@
       <c r="H11" s="446" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="1079"/>
+      <c r="I11" s="1078"/>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="1064"/>
+      <c r="C12" s="1051"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="65"/>
@@ -23337,10 +23427,10 @@
       <c r="H12" s="446" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="1079"/>
+      <c r="I12" s="1078"/>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="1065"/>
+      <c r="C13" s="1053"/>
       <c r="D13" s="96"/>
       <c r="E13" s="97"/>
       <c r="F13" s="82" t="s">
@@ -23350,10 +23440,10 @@
       <c r="H13" s="491" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="1079"/>
+      <c r="I13" s="1078"/>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="1063" t="s">
+      <c r="C14" s="1050" t="s">
         <v>109</v>
       </c>
       <c r="D14" s="101"/>
@@ -23365,10 +23455,10 @@
       <c r="H14" s="495" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="1079"/>
+      <c r="I14" s="1078"/>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="1064"/>
+      <c r="C15" s="1051"/>
       <c r="D15" s="72"/>
       <c r="E15" s="73"/>
       <c r="F15" s="65"/>
@@ -23376,10 +23466,10 @@
       <c r="H15" s="446" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="1079"/>
+      <c r="I15" s="1078"/>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="1064"/>
+      <c r="C16" s="1051"/>
       <c r="D16" s="96"/>
       <c r="E16" s="97"/>
       <c r="F16" s="65"/>
@@ -23387,10 +23477,10 @@
       <c r="H16" s="446" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="1079"/>
+      <c r="I16" s="1078"/>
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C17" s="1065"/>
+      <c r="C17" s="1053"/>
       <c r="D17" s="104"/>
       <c r="E17" s="105"/>
       <c r="F17" s="113" t="s">
@@ -23400,10 +23490,10 @@
       <c r="H17" s="491" t="s">
         <v>32</v>
       </c>
-      <c r="I17" s="1079"/>
+      <c r="I17" s="1078"/>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C18" s="1063" t="s">
+      <c r="C18" s="1050" t="s">
         <v>108</v>
       </c>
       <c r="D18" s="98"/>
@@ -23415,10 +23505,10 @@
       <c r="H18" s="495" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="1079"/>
+      <c r="I18" s="1078"/>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C19" s="1064"/>
+      <c r="C19" s="1051"/>
       <c r="D19" s="72"/>
       <c r="E19" s="73"/>
       <c r="F19" s="65"/>
@@ -23426,10 +23516,10 @@
       <c r="H19" s="446" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="1079"/>
+      <c r="I19" s="1078"/>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C20" s="1064"/>
+      <c r="C20" s="1051"/>
       <c r="D20" s="96"/>
       <c r="E20" s="97"/>
       <c r="F20" s="65"/>
@@ -23437,10 +23527,10 @@
       <c r="H20" s="446" t="s">
         <v>32</v>
       </c>
-      <c r="I20" s="1079"/>
+      <c r="I20" s="1078"/>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C21" s="1065"/>
+      <c r="C21" s="1053"/>
       <c r="D21" s="104"/>
       <c r="E21" s="105"/>
       <c r="F21" s="82" t="s">
@@ -23450,10 +23540,10 @@
       <c r="H21" s="496" t="s">
         <v>32</v>
       </c>
-      <c r="I21" s="1079"/>
+      <c r="I21" s="1078"/>
     </row>
     <row r="22" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C22" s="1063" t="s">
+      <c r="C22" s="1050" t="s">
         <v>107</v>
       </c>
       <c r="D22" s="98"/>
@@ -23465,10 +23555,10 @@
       <c r="H22" s="494" t="s">
         <v>32</v>
       </c>
-      <c r="I22" s="1079"/>
+      <c r="I22" s="1078"/>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C23" s="1064"/>
+      <c r="C23" s="1051"/>
       <c r="D23" s="72"/>
       <c r="E23" s="73"/>
       <c r="F23" s="65"/>
@@ -23476,10 +23566,10 @@
       <c r="H23" s="446" t="s">
         <v>32</v>
       </c>
-      <c r="I23" s="1079"/>
+      <c r="I23" s="1078"/>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C24" s="1064"/>
+      <c r="C24" s="1051"/>
       <c r="D24" s="72"/>
       <c r="E24" s="73"/>
       <c r="F24" s="81"/>
@@ -23487,10 +23577,10 @@
       <c r="H24" s="446" t="s">
         <v>32</v>
       </c>
-      <c r="I24" s="1079"/>
+      <c r="I24" s="1078"/>
     </row>
     <row r="25" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="1065"/>
+      <c r="C25" s="1053"/>
       <c r="D25" s="96" t="s">
         <v>64</v>
       </c>
@@ -23504,10 +23594,10 @@
       <c r="H25" s="491" t="s">
         <v>32</v>
       </c>
-      <c r="I25" s="1080"/>
+      <c r="I25" s="1079"/>
     </row>
     <row r="26" spans="3:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="1063" t="s">
+      <c r="C26" s="1050" t="s">
         <v>106</v>
       </c>
       <c r="D26" s="474" t="s">
@@ -23530,7 +23620,7 @@
       </c>
     </row>
     <row r="27" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="1064"/>
+      <c r="C27" s="1051"/>
       <c r="D27" s="438"/>
       <c r="E27" s="273"/>
       <c r="F27" s="62"/>
@@ -23540,12 +23630,12 @@
       <c r="H27" s="467" t="s">
         <v>33</v>
       </c>
-      <c r="I27" s="1081" t="s">
+      <c r="I27" s="1085" t="s">
         <v>815</v>
       </c>
     </row>
     <row r="28" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="1064"/>
+      <c r="C28" s="1051"/>
       <c r="D28" s="436"/>
       <c r="E28" s="437"/>
       <c r="F28" s="81"/>
@@ -23553,10 +23643,10 @@
       <c r="H28" s="447" t="s">
         <v>33</v>
       </c>
-      <c r="I28" s="1077"/>
+      <c r="I28" s="1081"/>
     </row>
     <row r="29" spans="3:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="1065"/>
+      <c r="C29" s="1053"/>
       <c r="D29" s="436"/>
       <c r="E29" s="437"/>
       <c r="F29" s="82" t="s">
@@ -23587,7 +23677,7 @@
       </c>
     </row>
     <row r="30" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="1063" t="s">
+      <c r="C30" s="1050" t="s">
         <v>105</v>
       </c>
       <c r="D30" s="439"/>
@@ -23610,12 +23700,12 @@
       <c r="N30" s="452" t="s">
         <v>32</v>
       </c>
-      <c r="O30" s="1076" t="s">
+      <c r="O30" s="1080" t="s">
         <v>813</v>
       </c>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C31" s="1064"/>
+      <c r="C31" s="1051"/>
       <c r="D31" s="64"/>
       <c r="E31" s="65"/>
       <c r="F31" s="65"/>
@@ -23634,10 +23724,10 @@
       <c r="N31" s="446" t="s">
         <v>32</v>
       </c>
-      <c r="O31" s="1077"/>
+      <c r="O31" s="1081"/>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C32" s="1064"/>
+      <c r="C32" s="1051"/>
       <c r="D32" s="64"/>
       <c r="E32" s="65"/>
       <c r="F32" s="65"/>
@@ -23656,10 +23746,10 @@
       <c r="N32" s="446" t="s">
         <v>32</v>
       </c>
-      <c r="O32" s="1077"/>
+      <c r="O32" s="1081"/>
     </row>
     <row r="33" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="1065"/>
+      <c r="C33" s="1053"/>
       <c r="D33" s="442" t="s">
         <v>73</v>
       </c>
@@ -23684,10 +23774,10 @@
       <c r="N33" s="446" t="s">
         <v>32</v>
       </c>
-      <c r="O33" s="1077"/>
+      <c r="O33" s="1081"/>
     </row>
     <row r="34" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C34" s="1063" t="s">
+      <c r="C34" s="1050" t="s">
         <v>104</v>
       </c>
       <c r="D34" s="61"/>
@@ -23710,10 +23800,10 @@
       <c r="N34" s="446" t="s">
         <v>32</v>
       </c>
-      <c r="O34" s="1077"/>
+      <c r="O34" s="1081"/>
     </row>
     <row r="35" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C35" s="1064"/>
+      <c r="C35" s="1051"/>
       <c r="D35" s="64"/>
       <c r="E35" s="65"/>
       <c r="F35" s="65"/>
@@ -23732,10 +23822,10 @@
       <c r="N35" s="446" t="s">
         <v>32</v>
       </c>
-      <c r="O35" s="1077"/>
+      <c r="O35" s="1081"/>
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C36" s="1064"/>
+      <c r="C36" s="1051"/>
       <c r="D36" s="64"/>
       <c r="E36" s="65"/>
       <c r="F36" s="65"/>
@@ -23754,10 +23844,10 @@
       <c r="N36" s="447" t="s">
         <v>33</v>
       </c>
-      <c r="O36" s="1077"/>
+      <c r="O36" s="1081"/>
     </row>
     <row r="37" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="1065"/>
+      <c r="C37" s="1053"/>
       <c r="D37" s="80" t="s">
         <v>73</v>
       </c>
@@ -23789,7 +23879,7 @@
       <c r="O37" s="1082"/>
     </row>
     <row r="38" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="1063" t="s">
+      <c r="C38" s="1050" t="s">
         <v>103</v>
       </c>
       <c r="D38" s="439"/>
@@ -23805,7 +23895,7 @@
       </c>
     </row>
     <row r="39" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C39" s="1064"/>
+      <c r="C39" s="1051"/>
       <c r="D39" s="64"/>
       <c r="E39" s="65"/>
       <c r="F39" s="66" t="s">
@@ -23819,7 +23909,7 @@
       </c>
     </row>
     <row r="40" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C40" s="1064"/>
+      <c r="C40" s="1051"/>
       <c r="D40" s="64"/>
       <c r="E40" s="65"/>
       <c r="F40" s="66" t="s">
@@ -23833,7 +23923,7 @@
       </c>
     </row>
     <row r="41" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C41" s="1065"/>
+      <c r="C41" s="1053"/>
       <c r="D41" s="108"/>
       <c r="E41" s="109"/>
       <c r="F41" s="82" t="s">
@@ -23847,7 +23937,7 @@
       </c>
     </row>
     <row r="42" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C42" s="1063" t="s">
+      <c r="C42" s="1050" t="s">
         <v>102</v>
       </c>
       <c r="D42" s="61"/>
@@ -23863,7 +23953,7 @@
       </c>
     </row>
     <row r="43" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C43" s="1064"/>
+      <c r="C43" s="1051"/>
       <c r="D43" s="64"/>
       <c r="E43" s="65"/>
       <c r="F43" s="66" t="s">
@@ -23877,7 +23967,7 @@
       </c>
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C44" s="1064"/>
+      <c r="C44" s="1051"/>
       <c r="D44" s="64"/>
       <c r="E44" s="65"/>
       <c r="F44" s="82" t="s">
@@ -23891,7 +23981,7 @@
       </c>
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C45" s="1065"/>
+      <c r="C45" s="1053"/>
       <c r="D45" s="80"/>
       <c r="E45" s="81"/>
       <c r="F45" s="113" t="s">
@@ -23905,7 +23995,7 @@
       </c>
     </row>
     <row r="46" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C46" s="1063" t="s">
+      <c r="C46" s="1050" t="s">
         <v>101</v>
       </c>
       <c r="D46" s="106"/>
@@ -23921,7 +24011,7 @@
       </c>
     </row>
     <row r="47" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C47" s="1074"/>
+      <c r="C47" s="1054"/>
       <c r="D47" s="64"/>
       <c r="E47" s="65"/>
       <c r="F47" s="66" t="s">
@@ -23935,7 +24025,7 @@
       </c>
     </row>
     <row r="48" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C48" s="1074"/>
+      <c r="C48" s="1054"/>
       <c r="D48" s="64"/>
       <c r="E48" s="65"/>
       <c r="F48" s="82" t="s">
@@ -23949,7 +24039,7 @@
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C49" s="1075"/>
+      <c r="C49" s="1055"/>
       <c r="D49" s="108"/>
       <c r="E49" s="109"/>
       <c r="F49" s="113" t="s">
@@ -23963,7 +24053,7 @@
       </c>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C50" s="1063" t="s">
+      <c r="C50" s="1050" t="s">
         <v>100</v>
       </c>
       <c r="D50" s="61"/>
@@ -23979,7 +24069,7 @@
       </c>
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C51" s="1064"/>
+      <c r="C51" s="1051"/>
       <c r="D51" s="64"/>
       <c r="E51" s="65"/>
       <c r="F51" s="66" t="s">
@@ -23993,7 +24083,7 @@
       </c>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C52" s="1064"/>
+      <c r="C52" s="1051"/>
       <c r="D52" s="64"/>
       <c r="E52" s="65"/>
       <c r="F52" s="66" t="s">
@@ -24007,7 +24097,7 @@
       </c>
     </row>
     <row r="53" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="1065"/>
+      <c r="C53" s="1053"/>
       <c r="D53" s="442" t="s">
         <v>73</v>
       </c>
@@ -24025,7 +24115,7 @@
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C54" s="1063" t="s">
+      <c r="C54" s="1050" t="s">
         <v>99</v>
       </c>
       <c r="D54" s="61"/>
@@ -24041,7 +24131,7 @@
       </c>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C55" s="1064"/>
+      <c r="C55" s="1051"/>
       <c r="D55" s="64"/>
       <c r="E55" s="65"/>
       <c r="F55" s="66" t="s">
@@ -24055,7 +24145,7 @@
       </c>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C56" s="1064"/>
+      <c r="C56" s="1051"/>
       <c r="D56" s="80"/>
       <c r="E56" s="81"/>
       <c r="F56" s="66" t="s">
@@ -24069,7 +24159,7 @@
       </c>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C57" s="1065"/>
+      <c r="C57" s="1053"/>
       <c r="D57" s="108"/>
       <c r="E57" s="109"/>
       <c r="F57" s="82" t="s">
@@ -24083,7 +24173,7 @@
       </c>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C58" s="1063" t="s">
+      <c r="C58" s="1050" t="s">
         <v>98</v>
       </c>
       <c r="D58" s="61"/>
@@ -24099,7 +24189,7 @@
       </c>
     </row>
     <row r="59" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C59" s="1064"/>
+      <c r="C59" s="1051"/>
       <c r="D59" s="64"/>
       <c r="E59" s="65"/>
       <c r="F59" s="66" t="s">
@@ -24113,7 +24203,7 @@
       </c>
     </row>
     <row r="60" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C60" s="1064"/>
+      <c r="C60" s="1051"/>
       <c r="D60" s="80"/>
       <c r="E60" s="81"/>
       <c r="F60" s="66" t="s">
@@ -24127,7 +24217,7 @@
       </c>
     </row>
     <row r="61" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C61" s="1065"/>
+      <c r="C61" s="1053"/>
       <c r="D61" s="80"/>
       <c r="E61" s="81"/>
       <c r="F61" s="82" t="s">
@@ -24141,7 +24231,7 @@
       </c>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C62" s="1063" t="s">
+      <c r="C62" s="1050" t="s">
         <v>97</v>
       </c>
       <c r="D62" s="106"/>
@@ -24157,7 +24247,7 @@
       </c>
     </row>
     <row r="63" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C63" s="1064"/>
+      <c r="C63" s="1051"/>
       <c r="D63" s="64"/>
       <c r="E63" s="65"/>
       <c r="F63" s="66" t="s">
@@ -24171,7 +24261,7 @@
       </c>
     </row>
     <row r="64" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C64" s="1064"/>
+      <c r="C64" s="1051"/>
       <c r="D64" s="64"/>
       <c r="E64" s="65"/>
       <c r="F64" s="66" t="s">
@@ -24185,7 +24275,7 @@
       </c>
     </row>
     <row r="65" spans="3:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C65" s="1065"/>
+      <c r="C65" s="1053"/>
       <c r="D65" s="110"/>
       <c r="E65" s="109"/>
       <c r="F65" s="113" t="s">
@@ -24217,7 +24307,7 @@
       </c>
     </row>
     <row r="66" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C66" s="1063" t="s">
+      <c r="C66" s="1050" t="s">
         <v>96</v>
       </c>
       <c r="D66" s="61"/>
@@ -24231,7 +24321,7 @@
       <c r="H66" s="467" t="s">
         <v>33</v>
       </c>
-      <c r="I66" s="1084"/>
+      <c r="I66" s="1083"/>
       <c r="J66" s="463"/>
       <c r="K66" s="464"/>
       <c r="L66" s="453" t="s">
@@ -24243,12 +24333,12 @@
       <c r="N66" s="465" t="s">
         <v>33</v>
       </c>
-      <c r="O66" s="1083" t="s">
+      <c r="O66" s="1077" t="s">
         <v>793</v>
       </c>
     </row>
     <row r="67" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C67" s="1064"/>
+      <c r="C67" s="1051"/>
       <c r="D67" s="64"/>
       <c r="E67" s="65"/>
       <c r="F67" s="66" t="s">
@@ -24260,7 +24350,7 @@
       <c r="H67" s="447" t="s">
         <v>33</v>
       </c>
-      <c r="I67" s="1084"/>
+      <c r="I67" s="1083"/>
       <c r="J67" s="455"/>
       <c r="K67" s="65"/>
       <c r="L67" s="66" t="s">
@@ -24272,10 +24362,10 @@
       <c r="N67" s="461" t="s">
         <v>32</v>
       </c>
-      <c r="O67" s="1079"/>
+      <c r="O67" s="1078"/>
     </row>
     <row r="68" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C68" s="1064"/>
+      <c r="C68" s="1051"/>
       <c r="D68" s="64"/>
       <c r="E68" s="65"/>
       <c r="F68" s="66" t="s">
@@ -24287,7 +24377,7 @@
       <c r="H68" s="447" t="s">
         <v>33</v>
       </c>
-      <c r="I68" s="1084"/>
+      <c r="I68" s="1083"/>
       <c r="J68" s="455"/>
       <c r="K68" s="65"/>
       <c r="L68" s="66" t="s">
@@ -24299,10 +24389,10 @@
       <c r="N68" s="461" t="s">
         <v>32</v>
       </c>
-      <c r="O68" s="1079"/>
+      <c r="O68" s="1078"/>
     </row>
     <row r="69" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C69" s="1073"/>
+      <c r="C69" s="1052"/>
       <c r="D69" s="469" t="s">
         <v>73</v>
       </c>
@@ -24318,7 +24408,7 @@
       <c r="H69" s="448" t="s">
         <v>33</v>
       </c>
-      <c r="I69" s="1084"/>
+      <c r="I69" s="1083"/>
       <c r="J69" s="456" t="s">
         <v>25</v>
       </c>
@@ -24334,16 +24424,16 @@
       <c r="N69" s="462" t="s">
         <v>32</v>
       </c>
-      <c r="O69" s="1080"/>
+      <c r="O69" s="1079"/>
     </row>
     <row r="70" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="I6:I9"/>
+    <mergeCell ref="I10:I25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="I27:I29"/>
     <mergeCell ref="O66:O69"/>
     <mergeCell ref="O30:O37"/>
     <mergeCell ref="C38:C41"/>
@@ -24357,11 +24447,11 @@
     <mergeCell ref="C62:C65"/>
     <mergeCell ref="C66:C69"/>
     <mergeCell ref="I66:I69"/>
-    <mergeCell ref="I6:I9"/>
-    <mergeCell ref="I10:I25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C18:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>